<commit_message>
starting adding cases and more comments on structure
</commit_message>
<xml_diff>
--- a/AlitoDataset.xlsx
+++ b/AlitoDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineparnell/alito-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F2811A6-7D56-F349-B417-B00A17E04F25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5C755F-3DAA-284E-8773-90320256C775}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
   </bookViews>
@@ -36,8 +36,11 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={5010FC8D-4B2F-2744-9AA3-E06DCDD6F440}</author>
+    <author>tc={F4821384-192B-DD46-8791-617913EBCE89}</author>
+    <author>tc={4374D2CD-142A-774C-8170-13C907E414CA}</author>
     <author>tc={CB9ADD91-1443-1F48-98DF-AB39A6962234}</author>
     <author>tc={D87AAAD5-35CC-CC42-A5C6-41D0FE831863}</author>
+    <author>tc={AF001A8C-E6AA-3349-9BE9-89B0E896018A}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5010FC8D-4B2F-2744-9AA3-E06DCDD6F440}">
@@ -48,15 +51,33 @@
     Jordan doing even case IDs, Catherine odd</t>
       </text>
     </comment>
-    <comment ref="J1" authorId="1" shapeId="0" xr:uid="{CB9ADD91-1443-1F48-98DF-AB39A6962234}">
+    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{F4821384-192B-DD46-8791-617913EBCE89}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    1 if characterized answer and oyez answer differ, 0 else</t>
+    citation year vs folder year</t>
       </text>
     </comment>
-    <comment ref="M1" authorId="2" shapeId="0" xr:uid="{D87AAAD5-35CC-CC42-A5C6-41D0FE831863}">
+    <comment ref="E1" authorId="2" shapeId="0" xr:uid="{4374D2CD-142A-774C-8170-13C907E414CA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    separate by commas</t>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="3" shapeId="0" xr:uid="{CB9ADD91-1443-1F48-98DF-AB39A6962234}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    1 if characterized answer and oyez answer differ, 0 else
+Reply:
+    basis for difference? more info :)</t>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="4" shapeId="0" xr:uid="{D87AAAD5-35CC-CC42-A5C6-41D0FE831863}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -64,12 +85,20 @@
     For now, split into 3 groups: 0 if unanimous, 1 if contentious, 2 if ambiguous</t>
       </text>
     </comment>
+    <comment ref="N1" authorId="5" shapeId="0" xr:uid="{AF001A8C-E6AA-3349-9BE9-89B0E896018A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    who wrote;justice joined by,justice:new who wrote;justice</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>Case Name</t>
   </si>
@@ -101,12 +130,6 @@
     <t>Vote Count</t>
   </si>
   <si>
-    <t>Majority Justices</t>
-  </si>
-  <si>
-    <t>Dissent Justices</t>
-  </si>
-  <si>
     <t>I-Length</t>
   </si>
   <si>
@@ -219,6 +242,60 @@
   </si>
   <si>
     <t>Case ID</t>
+  </si>
+  <si>
+    <t>Hein v. Freedom From Religion Foundation, Inc.</t>
+  </si>
+  <si>
+    <t>551 US 587 (2007)</t>
+  </si>
+  <si>
+    <t>Establishment Clause, First Amendment,Case or Controversy Clause, Article III: Standing</t>
+  </si>
+  <si>
+    <t>Do plaintiffs have standing as taxpayers to bring Establishment Clause 
+challenges against Executive Branch actions that are funded by general
+appropriations rather than by a specific act of Congress?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>employed largely doctrinal
+and pragmatic reasoning.</t>
+  </si>
+  <si>
+    <t>National Association of Home Builders et al v. Defenders of Wildlife et al.</t>
+  </si>
+  <si>
+    <t>551 US 644 (2007)</t>
+  </si>
+  <si>
+    <t>Section 402(b) of the Clean Water Act,Section 7(a)(2) of the Endangered Species Act of 1973</t>
+  </si>
+  <si>
+    <t>employed primarily doctrinal and textual reasoning</t>
+  </si>
+  <si>
+    <t>5,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does Section 7(a)(2) of the Endangered Species Act of 1973 effectively
+operate as a tenth criterion on which the transfer of EPA permitting 
+power to state authorities under Section 402(b) of the Clean Water Act 
+must be conditioned? </t>
+  </si>
+  <si>
+    <t>Majority</t>
+  </si>
+  <si>
+    <t>Plurality</t>
+  </si>
+  <si>
+    <t>Concurrence</t>
+  </si>
+  <si>
+    <t>Dissent</t>
   </si>
 </sst>
 </file>
@@ -247,12 +324,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -267,9 +350,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,91 +680,105 @@
   <threadedComment ref="A1" dT="2020-06-29T21:44:16.97" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{5010FC8D-4B2F-2744-9AA3-E06DCDD6F440}">
     <text>Jordan doing even case IDs, Catherine odd</text>
   </threadedComment>
+  <threadedComment ref="C1" dT="2020-06-30T20:17:28.47" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{F4821384-192B-DD46-8791-617913EBCE89}">
+    <text>citation year vs folder year</text>
+  </threadedComment>
+  <threadedComment ref="E1" dT="2020-06-30T03:53:05.01" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{4374D2CD-142A-774C-8170-13C907E414CA}">
+    <text>separate by commas</text>
+  </threadedComment>
   <threadedComment ref="J1" dT="2020-06-29T21:33:16.24" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{CB9ADD91-1443-1F48-98DF-AB39A6962234}">
     <text>1 if characterized answer and oyez answer differ, 0 else</text>
   </threadedComment>
+  <threadedComment ref="J1" dT="2020-06-30T20:18:24.00" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{BD49D24B-E482-484A-9EAA-10C021439E89}" parentId="{CB9ADD91-1443-1F48-98DF-AB39A6962234}">
+    <text>basis for difference? more info :)</text>
+  </threadedComment>
   <threadedComment ref="M1" dT="2020-06-29T21:36:26.91" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{D87AAAD5-35CC-CC42-A5C6-41D0FE831863}">
     <text>For now, split into 3 groups: 0 if unanimous, 1 if contentious, 2 if ambiguous</text>
+  </threadedComment>
+  <threadedComment ref="N1" dT="2020-06-30T20:16:50.75" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{AF001A8C-E6AA-3349-9BE9-89B0E896018A}">
+    <text>who wrote;justice joined by,justice:new who wrote;justice</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060A011E-60FD-5047-91C8-6B9B09AABF05}">
-  <dimension ref="A1:AX79"/>
+  <dimension ref="A1:AZ79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="13" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
@@ -692,8 +793,8 @@
       <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
-        <v>47</v>
+      <c r="J1" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -701,146 +802,236 @@
       <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="M1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Y1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AA1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AB1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="X1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AW1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:52" ht="51" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
       <c r="D2">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
+        <v>2007</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>6</v>
+      </c>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2">
+        <v>5.5</v>
+      </c>
+      <c r="AM2">
+        <v>13</v>
+      </c>
+      <c r="AT2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52" ht="68" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
       <c r="D4">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
+        <v>2007</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4">
+        <v>26</v>
+      </c>
+      <c r="L4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>9</v>
+      </c>
+      <c r="Y4">
+        <v>11</v>
+      </c>
+      <c r="AM4">
+        <v>4.5</v>
+      </c>
+      <c r="AT4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -848,7 +1039,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -856,7 +1047,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -864,7 +1055,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -872,7 +1063,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -880,7 +1071,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -888,7 +1079,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -896,7 +1087,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -904,7 +1095,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -912,7 +1103,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -920,7 +1111,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -928,7 +1119,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Began preliminary data entry, entered lines 2-8 evens
</commit_message>
<xml_diff>
--- a/AlitoDataset.xlsx
+++ b/AlitoDataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineparnell/alito-research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jtsanz\alito-research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5C755F-3DAA-284E-8773-90320256C775}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47EDF65-DE99-493C-86AC-A8EB1458EC7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
+    <workbookView xWindow="10360" yWindow="790" windowWidth="14400" windowHeight="7360" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,6 +41,10 @@
     <author>tc={CB9ADD91-1443-1F48-98DF-AB39A6962234}</author>
     <author>tc={D87AAAD5-35CC-CC42-A5C6-41D0FE831863}</author>
     <author>tc={AF001A8C-E6AA-3349-9BE9-89B0E896018A}</author>
+    <author>tc={612DC64F-C5FE-40F8-BAF2-EF4FD089D0F2}</author>
+    <author>tc={0F4748BD-5B03-439A-B8A7-8872FFB421BA}</author>
+    <author>tc={2810AD96-B8B6-4798-A014-AFDE2C354919}</author>
+    <author>tc={A5E80391-6849-4DFE-95FD-14B5F54B00D4}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5010FC8D-4B2F-2744-9AA3-E06DCDD6F440}">
@@ -93,12 +97,44 @@
     who wrote;justice joined by,justice:new who wrote;justice</t>
       </text>
     </comment>
+    <comment ref="R1" authorId="6" shapeId="0" xr:uid="{612DC64F-C5FE-40F8-BAF2-EF4FD089D0F2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Sometimes there is a background section that isn't included in the total count, how do you want to handle?</t>
+      </text>
+    </comment>
+    <comment ref="AT1" authorId="7" shapeId="0" xr:uid="{0F4748BD-5B03-439A-B8A7-8872FFB421BA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Apparently length sometimes has the format of Length (pgs) 2 lines? Want to do 2l for 2 lines or something like that?</t>
+      </text>
+    </comment>
+    <comment ref="G7" authorId="8" shapeId="0" xr:uid="{2810AD96-B8B6-4798-A014-AFDE2C354919}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    No Yes/No answer given: just explanations;</t>
+      </text>
+    </comment>
+    <comment ref="L9" authorId="9" shapeId="0" xr:uid="{A5E80391-6849-4DFE-95FD-14B5F54B00D4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    "7-2 for petitioner?" what does that mean?</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
   <si>
     <t>Case Name</t>
   </si>
@@ -259,10 +295,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>employed largely doctrinal
-and pragmatic reasoning.</t>
   </si>
   <si>
     <t>National Association of Home Builders et al v. Defenders of Wildlife et al.</t>
@@ -296,6 +328,102 @@
   </si>
   <si>
     <t>Dissent</t>
+  </si>
+  <si>
+    <t>Ledbetter v. The Good Year Tire &amp; Rubber Company, Inc.</t>
+  </si>
+  <si>
+    <t>550 US 618 (2007)</t>
+  </si>
+  <si>
+    <t>Title VII of the Civil Rights Act of 1964</t>
+  </si>
+  <si>
+    <t>Can a plaintiff bring a salary discrimination suit under Title VII of the Civil Rights Act of 1964 when the disparate pay is received during the 180-day statutory limitations period, but is the result of discriminatory pay decisions that occurred outside the limitations period?</t>
+  </si>
+  <si>
+    <t>employed largely doctrinal reasoning</t>
+  </si>
+  <si>
+    <t>employed largely doctrinal
+and pragmatic reasoning</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Scalia,Kennedy,Thomas</t>
+  </si>
+  <si>
+    <t>Ginsburg;Stevens,Souter,Breyer</t>
+  </si>
+  <si>
+    <t>Allison Engine Co. v. U.S. ex. rel. Sanders</t>
+  </si>
+  <si>
+    <t>“Present[ment]” requirement in the False Claims Act</t>
+  </si>
+  <si>
+    <t>Must whistleblower claimants prove that a private company directly presented a fraudulent bill to the government in order to prevail in a False Claims Act case?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>mainly textualist analysis</t>
+  </si>
+  <si>
+    <t>MeadWestvaco Corporation v. Illinois Department of Revenue</t>
+  </si>
+  <si>
+    <t>553 US 662 (2008)</t>
+  </si>
+  <si>
+    <t>553 US 16 (2008)</t>
+  </si>
+  <si>
+    <t>Doctrinal question re: how a prior case does or doesn’t control the current tax and
+corporate structure dispute</t>
+  </si>
+  <si>
+    <t>Under the governing Supreme Court precedent, Allied-Signal, Inc. v. Director, Div. of
+Taxation, 504 U.S. 768 (1992), may a parent company use a division as a non-
+taxable investment when the division is involved in a substantially different
+business segment but the parent provides cash infusions, investment advice and
+oversight?</t>
+  </si>
+  <si>
+    <t>primarily doctrinial reasoning</t>
+  </si>
+  <si>
+    <t>9,0</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Stevens,Scalia,Kennedy,Souter,Thomas,Ginsberg,Breyer</t>
+  </si>
+  <si>
+    <t>Thomas;</t>
+  </si>
+  <si>
+    <t>Snyder v. Louisiana</t>
+  </si>
+  <si>
+    <t>552 US 472 (2008)</t>
+  </si>
+  <si>
+    <t>Equal Protection Clause</t>
+  </si>
+  <si>
+    <t>Did the state’s dismissal by peremptory challenge of all of the black potential jurors, combined with the prosecution’s comparisons of the case to the O.J. Simpson trial, amount to a violation of the Equal Protection Clause?</t>
+  </si>
+  <si>
+    <t>primarily pragmatic reasoning, some doctrinal reasoning</t>
+  </si>
+  <si>
+    <t>7,2</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Stevens,Kennedy,Souter,Ginsburg,Breyer</t>
+  </si>
+  <si>
+    <t>Thomas;Scalia</t>
   </si>
 </sst>
 </file>
@@ -318,8 +446,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="9"/>
+      <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -350,13 +478,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,6 +507,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Jordan Sanz" id="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" userId="d35b3cd92db97120" providerId="Windows Live"/>
   <person displayName="Catherine D. Parnell" id="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" userId="S::f003k79@dartmouth.edu::2ae15c9b-b470-4726-a023-26f4a8612d82" providerId="AD"/>
 </personList>
 </file>
@@ -698,6 +830,18 @@
   <threadedComment ref="N1" dT="2020-06-30T20:16:50.75" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{AF001A8C-E6AA-3349-9BE9-89B0E896018A}">
     <text>who wrote;justice joined by,justice:new who wrote;justice</text>
   </threadedComment>
+  <threadedComment ref="R1" dT="2020-07-01T18:26:19.91" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{612DC64F-C5FE-40F8-BAF2-EF4FD089D0F2}">
+    <text>Sometimes there is a background section that isn't included in the total count, how do you want to handle?</text>
+  </threadedComment>
+  <threadedComment ref="AT1" dT="2020-07-01T18:21:57.37" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{0F4748BD-5B03-439A-B8A7-8872FFB421BA}">
+    <text>Apparently length sometimes has the format of Length (pgs) 2 lines? Want to do 2l for 2 lines or something like that?</text>
+  </threadedComment>
+  <threadedComment ref="G7" dT="2020-07-01T18:30:00.55" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{2810AD96-B8B6-4798-A014-AFDE2C354919}">
+    <text>No Yes/No answer given: just explanations;</text>
+  </threadedComment>
+  <threadedComment ref="L9" dT="2020-07-01T18:34:52.90" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{A5E80391-6849-4DFE-95FD-14B5F54B00D4}">
+    <text>"7-2 for petitioner?" what does that mean?</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -705,11 +849,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060A011E-60FD-5047-91C8-6B9B09AABF05}">
   <dimension ref="A1:AZ79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
@@ -765,7 +909,7 @@
     <col min="52" max="52" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -806,18 +950,18 @@
         <v>46</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="R1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="S1" t="s">
@@ -901,7 +1045,7 @@
       <c r="AS1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AU1" s="1" t="s">
@@ -923,7 +1067,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:52" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:52" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -946,13 +1090,13 @@
         <v>52</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="K2">
         <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -976,44 +1120,116 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" ht="65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
       <c r="D3">
         <v>2007</v>
       </c>
-    </row>
-    <row r="4" spans="1:52" ht="68" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>70</v>
+      </c>
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="Y3">
+        <v>15</v>
+      </c>
+      <c r="Z3">
+        <v>151</v>
+      </c>
+      <c r="AA3">
+        <v>52</v>
+      </c>
+      <c r="AC3">
+        <v>37</v>
+      </c>
+      <c r="AD3">
+        <v>7</v>
+      </c>
+      <c r="AM3">
+        <v>4.5</v>
+      </c>
+      <c r="AN3">
+        <v>39</v>
+      </c>
+      <c r="AO3">
+        <v>13</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>9</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52" ht="62" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
         <v>54</v>
-      </c>
-      <c r="C4" t="s">
-        <v>55</v>
       </c>
       <c r="D4">
         <v>2007</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
         <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K4">
         <v>26</v>
       </c>
       <c r="L4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -1031,15 +1247,69 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" ht="37" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
       <c r="D5">
         <v>2007</v>
       </c>
-    </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>1.25</v>
+      </c>
+      <c r="Y5">
+        <v>2.5</v>
+      </c>
+      <c r="AA5">
+        <v>14</v>
+      </c>
+      <c r="AC5">
+        <v>6</v>
+      </c>
+      <c r="AE5">
+        <v>44</v>
+      </c>
+      <c r="AM5">
+        <v>3.25</v>
+      </c>
+      <c r="AP5">
+        <v>14</v>
+      </c>
+      <c r="AQ5">
+        <v>7</v>
+      </c>
+      <c r="AS5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1047,15 +1317,64 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:52" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
       <c r="D7">
         <v>2007</v>
       </c>
-    </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="E7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K7">
+        <v>15</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>83</v>
+      </c>
+      <c r="P7" t="s">
+        <v>84</v>
+      </c>
+      <c r="R7">
+        <v>5.5</v>
+      </c>
+      <c r="Y7">
+        <v>7</v>
+      </c>
+      <c r="Z7">
+        <v>90</v>
+      </c>
+      <c r="AC7">
+        <v>13</v>
+      </c>
+      <c r="AM7">
+        <v>2</v>
+      </c>
+      <c r="AO7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1063,15 +1382,63 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
       <c r="D9">
         <v>2007</v>
       </c>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" t="s">
+        <v>89</v>
+      </c>
+      <c r="K9">
+        <v>13</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>92</v>
+      </c>
+      <c r="R9">
+        <v>3</v>
+      </c>
+      <c r="Y9">
+        <v>10</v>
+      </c>
+      <c r="Z9">
+        <v>44</v>
+      </c>
+      <c r="AB9">
+        <v>125</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1079,7 +1446,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1087,7 +1454,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1095,7 +1462,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1103,7 +1470,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1111,7 +1478,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1119,7 +1486,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1127,7 +1494,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1135,7 +1502,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1143,7 +1510,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1151,7 +1518,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1159,7 +1526,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1167,7 +1534,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1175,7 +1542,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1183,7 +1550,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1191,7 +1558,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1199,7 +1566,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1207,7 +1574,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1215,7 +1582,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1223,7 +1590,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1231,7 +1598,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1239,7 +1606,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1247,7 +1614,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1255,7 +1622,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1263,7 +1630,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1271,7 +1638,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1279,7 +1646,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1287,7 +1654,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1295,7 +1662,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1303,7 +1670,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1311,7 +1678,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1319,7 +1686,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1327,7 +1694,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1335,7 +1702,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1343,7 +1710,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1351,7 +1718,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1359,7 +1726,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1367,7 +1734,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1375,7 +1742,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1383,7 +1750,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1391,7 +1758,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1399,7 +1766,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1407,7 +1774,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1415,7 +1782,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1423,7 +1790,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1431,7 +1798,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1439,7 +1806,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1447,7 +1814,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1455,7 +1822,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1463,7 +1830,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1471,7 +1838,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1479,7 +1846,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1487,7 +1854,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1495,7 +1862,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1503,7 +1870,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1511,7 +1878,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1519,7 +1886,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1527,7 +1894,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1535,7 +1902,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1543,7 +1910,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1551,7 +1918,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1559,7 +1926,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1567,7 +1934,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1575,7 +1942,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1583,7 +1950,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1591,7 +1958,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1599,7 +1966,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1607,7 +1974,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1615,7 +1982,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1623,7 +1990,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1633,6 +2000,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed 2007 year to 2006
</commit_message>
<xml_diff>
--- a/AlitoDataset.xlsx
+++ b/AlitoDataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jtsanz\alito-research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47EDF65-DE99-493C-86AC-A8EB1458EC7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C3C00B-6059-45BC-BB0D-52873F70F2C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10360" yWindow="790" windowWidth="14400" windowHeight="7360" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,14 +37,15 @@
   <authors>
     <author>tc={5010FC8D-4B2F-2744-9AA3-E06DCDD6F440}</author>
     <author>tc={F4821384-192B-DD46-8791-617913EBCE89}</author>
+    <author>tc={61D1E5EF-D958-4E20-BF68-DEC3C3DFE074}</author>
     <author>tc={4374D2CD-142A-774C-8170-13C907E414CA}</author>
     <author>tc={CB9ADD91-1443-1F48-98DF-AB39A6962234}</author>
     <author>tc={D87AAAD5-35CC-CC42-A5C6-41D0FE831863}</author>
     <author>tc={AF001A8C-E6AA-3349-9BE9-89B0E896018A}</author>
     <author>tc={612DC64F-C5FE-40F8-BAF2-EF4FD089D0F2}</author>
+    <author>tc={C4848F86-CB4C-45EE-8700-3A7450D7769A}</author>
     <author>tc={0F4748BD-5B03-439A-B8A7-8872FFB421BA}</author>
     <author>tc={2810AD96-B8B6-4798-A014-AFDE2C354919}</author>
-    <author>tc={A5E80391-6849-4DFE-95FD-14B5F54B00D4}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5010FC8D-4B2F-2744-9AA3-E06DCDD6F440}">
@@ -63,7 +64,15 @@
     citation year vs folder year</t>
       </text>
     </comment>
-    <comment ref="E1" authorId="2" shapeId="0" xr:uid="{4374D2CD-142A-774C-8170-13C907E414CA}">
+    <comment ref="D1" authorId="2" shapeId="0" xr:uid="{61D1E5EF-D958-4E20-BF68-DEC3C3DFE074}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    These are folder year</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="3" shapeId="0" xr:uid="{4374D2CD-142A-774C-8170-13C907E414CA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -71,7 +80,7 @@
     separate by commas</t>
       </text>
     </comment>
-    <comment ref="J1" authorId="3" shapeId="0" xr:uid="{CB9ADD91-1443-1F48-98DF-AB39A6962234}">
+    <comment ref="J1" authorId="4" shapeId="0" xr:uid="{CB9ADD91-1443-1F48-98DF-AB39A6962234}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -81,7 +90,7 @@
     basis for difference? more info :)</t>
       </text>
     </comment>
-    <comment ref="M1" authorId="4" shapeId="0" xr:uid="{D87AAAD5-35CC-CC42-A5C6-41D0FE831863}">
+    <comment ref="M1" authorId="5" shapeId="0" xr:uid="{D87AAAD5-35CC-CC42-A5C6-41D0FE831863}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -89,7 +98,7 @@
     For now, split into 3 groups: 0 if unanimous, 1 if contentious, 2 if ambiguous</t>
       </text>
     </comment>
-    <comment ref="N1" authorId="5" shapeId="0" xr:uid="{AF001A8C-E6AA-3349-9BE9-89B0E896018A}">
+    <comment ref="N1" authorId="6" shapeId="0" xr:uid="{AF001A8C-E6AA-3349-9BE9-89B0E896018A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -97,7 +106,7 @@
     who wrote;justice joined by,justice:new who wrote;justice</t>
       </text>
     </comment>
-    <comment ref="R1" authorId="6" shapeId="0" xr:uid="{612DC64F-C5FE-40F8-BAF2-EF4FD089D0F2}">
+    <comment ref="R1" authorId="7" shapeId="0" xr:uid="{612DC64F-C5FE-40F8-BAF2-EF4FD089D0F2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -105,7 +114,15 @@
     Sometimes there is a background section that isn't included in the total count, how do you want to handle?</t>
       </text>
     </comment>
-    <comment ref="AT1" authorId="7" shapeId="0" xr:uid="{0F4748BD-5B03-439A-B8A7-8872FFB421BA}">
+    <comment ref="AF1" authorId="8" shapeId="0" xr:uid="{C4848F86-CB4C-45EE-8700-3A7450D7769A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Add together with MA1</t>
+      </text>
+    </comment>
+    <comment ref="AT1" authorId="9" shapeId="0" xr:uid="{0F4748BD-5B03-439A-B8A7-8872FFB421BA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -113,20 +130,12 @@
     Apparently length sometimes has the format of Length (pgs) 2 lines? Want to do 2l for 2 lines or something like that?</t>
       </text>
     </comment>
-    <comment ref="G7" authorId="8" shapeId="0" xr:uid="{2810AD96-B8B6-4798-A014-AFDE2C354919}">
+    <comment ref="G7" authorId="10" shapeId="0" xr:uid="{2810AD96-B8B6-4798-A014-AFDE2C354919}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     No Yes/No answer given: just explanations;</t>
-      </text>
-    </comment>
-    <comment ref="L9" authorId="9" shapeId="0" xr:uid="{A5E80391-6849-4DFE-95FD-14B5F54B00D4}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    "7-2 for petitioner?" what does that mean?</t>
       </text>
     </comment>
   </commentList>
@@ -815,6 +824,9 @@
   <threadedComment ref="C1" dT="2020-06-30T20:17:28.47" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{F4821384-192B-DD46-8791-617913EBCE89}">
     <text>citation year vs folder year</text>
   </threadedComment>
+  <threadedComment ref="D1" dT="2020-07-01T19:38:14.17" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{61D1E5EF-D958-4E20-BF68-DEC3C3DFE074}">
+    <text>These are folder year</text>
+  </threadedComment>
   <threadedComment ref="E1" dT="2020-06-30T03:53:05.01" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{4374D2CD-142A-774C-8170-13C907E414CA}">
     <text>separate by commas</text>
   </threadedComment>
@@ -833,14 +845,14 @@
   <threadedComment ref="R1" dT="2020-07-01T18:26:19.91" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{612DC64F-C5FE-40F8-BAF2-EF4FD089D0F2}">
     <text>Sometimes there is a background section that isn't included in the total count, how do you want to handle?</text>
   </threadedComment>
+  <threadedComment ref="AF1" dT="2020-07-01T19:57:27.40" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{C4848F86-CB4C-45EE-8700-3A7450D7769A}">
+    <text>Add together with MA1</text>
+  </threadedComment>
   <threadedComment ref="AT1" dT="2020-07-01T18:21:57.37" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{0F4748BD-5B03-439A-B8A7-8872FFB421BA}">
     <text>Apparently length sometimes has the format of Length (pgs) 2 lines? Want to do 2l for 2 lines or something like that?</text>
   </threadedComment>
   <threadedComment ref="G7" dT="2020-07-01T18:30:00.55" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{2810AD96-B8B6-4798-A014-AFDE2C354919}">
     <text>No Yes/No answer given: just explanations;</text>
-  </threadedComment>
-  <threadedComment ref="L9" dT="2020-07-01T18:34:52.90" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{A5E80391-6849-4DFE-95FD-14B5F54B00D4}">
-    <text>"7-2 for petitioner?" what does that mean?</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -849,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060A011E-60FD-5047-91C8-6B9B09AABF05}">
   <dimension ref="A1:AZ79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -919,7 +931,7 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -1003,7 +1015,7 @@
       <c r="AE1" t="s">
         <v>22</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="3" t="s">
         <v>29</v>
       </c>
       <c r="AG1" t="s">
@@ -1078,7 +1090,7 @@
         <v>49</v>
       </c>
       <c r="D2">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="E2" t="s">
         <v>50</v>
@@ -1131,7 +1143,7 @@
         <v>64</v>
       </c>
       <c r="D3">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="E3" t="s">
         <v>65</v>
@@ -1211,7 +1223,7 @@
         <v>54</v>
       </c>
       <c r="D4">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="E4" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Did cases 2008 and 2009 years
</commit_message>
<xml_diff>
--- a/AlitoDataset.xlsx
+++ b/AlitoDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jtsanz\alito-research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C3C00B-6059-45BC-BB0D-52873F70F2C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{1A84C31C-6443-41F0-9786-986150042EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
   </bookViews>
@@ -46,6 +46,8 @@
     <author>tc={C4848F86-CB4C-45EE-8700-3A7450D7769A}</author>
     <author>tc={0F4748BD-5B03-439A-B8A7-8872FFB421BA}</author>
     <author>tc={2810AD96-B8B6-4798-A014-AFDE2C354919}</author>
+    <author>tc={3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}</author>
+    <author>tc={93985E51-4186-401D-B292-10D9DC17CEB8}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5010FC8D-4B2F-2744-9AA3-E06DCDD6F440}">
@@ -138,12 +140,28 @@
     No Yes/No answer given: just explanations;</t>
       </text>
     </comment>
+    <comment ref="A19" authorId="11" shapeId="0" xr:uid="{3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    missing lengths on a lot of sections, but have line count highlights</t>
+      </text>
+    </comment>
+    <comment ref="M23" authorId="12" shapeId="0" xr:uid="{93985E51-4186-401D-B292-10D9DC17CEB8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    it's 5-3, is this contentious or ambigious? haha</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="143">
   <si>
     <t>Case Name</t>
   </si>
@@ -433,6 +451,156 @@
   </si>
   <si>
     <t>Thomas;Scalia</t>
+  </si>
+  <si>
+    <t>Fitzgerald v. Barnstable School Committee</t>
+  </si>
+  <si>
+    <t>555 U.S. 246 (2009)</t>
+  </si>
+  <si>
+    <t>Title IX of the Education Amendments of 1972,42 U.S.C. §1983</t>
+  </si>
+  <si>
+    <t>Is Title IX’s implied private remedy sufficiently comprehensive to preclude the use of 42 U.S.C. Section 1983 to advance sex discrimination claims against  federally funded institutions?</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Stevens,Scalia, Kennedy,Souter,Thomas,Ginsburg,Breyer</t>
+  </si>
+  <si>
+    <t>0/4</t>
+  </si>
+  <si>
+    <t>Horne v. Flores</t>
+  </si>
+  <si>
+    <t>557 U.S. 433 (2009)</t>
+  </si>
+  <si>
+    <t>Case-or-controversy requirement of Article III,Federal Rule of Civil Procedure 60(b)(5)</t>
+  </si>
+  <si>
+    <t>Did the lower courts err in their analysis under Rule 60(b)(5) regarding Arizona's contention that changes in education law, including increased state funding,  changes in the management of the school district involved, and passage of the No Child Left Behind Act had so altered the foundations of prior court rulings that relief from such judgments was warranted?</t>
+  </si>
+  <si>
+    <t>employs largely purposive-ism, some doctrinal reasoning.</t>
+  </si>
+  <si>
+    <t>mostly pragmatic, some purposive-ism</t>
+  </si>
+  <si>
+    <t>Breyer;Stevens,Souter,Ginsburg</t>
+  </si>
+  <si>
+    <t>Pleasant Grove City v. Summum</t>
+  </si>
+  <si>
+    <t>555 U.S. 460 (2009)</t>
+  </si>
+  <si>
+    <t>Free Speech Clause of the First Amendment</t>
+  </si>
+  <si>
+    <t>Does a city’s refusal to place a religious organization’s monument in a public park violate that organization’s First Amendment free speech rights when the park already contains a monument from a different religious group?</t>
+  </si>
+  <si>
+    <t>vast majority pragmatic reasoning</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Stevens,Scalia,Kennedy,Thomas,Ginsburg,Breyer</t>
+  </si>
+  <si>
+    <t>Stevens;Ginsburg:Scalia;Thomas:Breyer:Souter</t>
+  </si>
+  <si>
+    <t>0/6</t>
+  </si>
+  <si>
+    <t>Jones v. Harris Associates L.P.</t>
+  </si>
+  <si>
+    <t>559 U.S. 335 (2010)</t>
+  </si>
+  <si>
+    <t>Section 36(b) of the Investment Company Act</t>
+  </si>
+  <si>
+    <t>Did the Seventh Circuit err in holding that claims alleging mutual fund management&amp;#39;s fees were too high is not cognizable under Section 36(b) of the Investment Company Act, when that holding is in conflict with those in three other circuits?</t>
+  </si>
+  <si>
+    <t>mostly doctrinal and pragmatic</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Stevens,Scalia,Kennedy,Ginsburg,Breyer,Sotomayor</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>0/3</t>
+  </si>
+  <si>
+    <t>McDonald v. Chicago</t>
+  </si>
+  <si>
+    <t>561 U.S. 742 (2010)</t>
+  </si>
+  <si>
+    <t>Second amendment</t>
+  </si>
+  <si>
+    <t>Does the Second Amendment apply to the states because it is incorporated by the Fourteenth Amendment's Privileges and Immunities or Due Process clauses and thereby made applicable to the states?</t>
+  </si>
+  <si>
+    <t>Really doctrinal but a lot of originalism to make it seem constitutional</t>
+  </si>
+  <si>
+    <t>Alito;Thomas,Scalia,Kennedy,Roberts</t>
+  </si>
+  <si>
+    <t>Sotomayor;Ginsburg,Breyer,Stevens</t>
+  </si>
+  <si>
+    <t>Perdue v. Kenny A.</t>
+  </si>
+  <si>
+    <t>559 U.S. 542 (2010)</t>
+  </si>
+  <si>
+    <t>Federal fee-shifting statute</t>
+  </si>
+  <si>
+    <t>Can the reasonable attorneys' fee award under a federal fee-shifting statute ever be enhanced based solely on the quality of performance and results obtained?</t>
+  </si>
+  <si>
+    <t>mostly pragmatic</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Scalia,Thomas</t>
+  </si>
+  <si>
+    <t>Kennedy;Thomas</t>
+  </si>
+  <si>
+    <t>Breyer;Stevens,Ginsburg,Sotomayor</t>
+  </si>
+  <si>
+    <t>Stolt-Nielsen v. Animalfeeds International Corp.</t>
+  </si>
+  <si>
+    <t>559 U.S. 662 (2010)</t>
+  </si>
+  <si>
+    <t>Federal Arbitration Act</t>
+  </si>
+  <si>
+    <t>Is imposing class arbitration on parties whose arbitration clauses are silent on that issue consistent with the Federal Arbitration Act?</t>
+  </si>
+  <si>
+    <t>5,3</t>
+  </si>
+  <si>
+    <t>Ginsburg;Stevens,Breyer</t>
   </si>
 </sst>
 </file>
@@ -458,7 +626,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -487,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -497,6 +665,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,6 +1023,12 @@
   <threadedComment ref="G7" dT="2020-07-01T18:30:00.55" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{2810AD96-B8B6-4798-A014-AFDE2C354919}">
     <text>No Yes/No answer given: just explanations;</text>
   </threadedComment>
+  <threadedComment ref="A19" dT="2020-07-05T08:06:57.89" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}">
+    <text>missing lengths on a lot of sections, but have line count highlights</text>
+  </threadedComment>
+  <threadedComment ref="M23" dT="2020-07-05T08:11:32.10" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{93985E51-4186-401D-B292-10D9DC17CEB8}">
+    <text>it's 5-3, is this contentious or ambigious? haha</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -861,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060A011E-60FD-5047-91C8-6B9B09AABF05}">
   <dimension ref="A1:AZ79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1462,8 +1637,62 @@
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
       <c r="D11">
         <v>2008</v>
+      </c>
+      <c r="E11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" t="s">
+        <v>103</v>
+      </c>
+      <c r="K11">
+        <v>13</v>
+      </c>
+      <c r="L11" t="s">
+        <v>82</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11" t="s">
+        <v>97</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+      <c r="Y11">
+        <v>8.5</v>
+      </c>
+      <c r="Z11">
+        <v>52</v>
+      </c>
+      <c r="AC11">
+        <v>108</v>
+      </c>
+      <c r="AD11">
+        <v>2</v>
+      </c>
+      <c r="AE11">
+        <v>3</v>
+      </c>
+      <c r="AM11">
+        <v>0</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.35">
@@ -1478,8 +1707,80 @@
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
       <c r="D13">
         <v>2008</v>
+      </c>
+      <c r="E13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" t="s">
+        <v>104</v>
+      </c>
+      <c r="K13">
+        <v>36</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>105</v>
+      </c>
+      <c r="R13">
+        <v>7.5</v>
+      </c>
+      <c r="V13">
+        <v>6</v>
+      </c>
+      <c r="Y13">
+        <v>19</v>
+      </c>
+      <c r="Z13">
+        <v>10</v>
+      </c>
+      <c r="AB13">
+        <v>231</v>
+      </c>
+      <c r="AC13">
+        <v>60</v>
+      </c>
+      <c r="AD13">
+        <v>11</v>
+      </c>
+      <c r="AE13">
+        <v>4</v>
+      </c>
+      <c r="AM13">
+        <v>9</v>
+      </c>
+      <c r="AN13">
+        <v>11</v>
+      </c>
+      <c r="AP13">
+        <v>71</v>
+      </c>
+      <c r="AS13">
+        <v>14</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.35">
@@ -1494,8 +1795,62 @@
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" t="s">
+        <v>107</v>
+      </c>
       <c r="D15">
         <v>2008</v>
+      </c>
+      <c r="E15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" t="s">
+        <v>110</v>
+      </c>
+      <c r="K15">
+        <v>18</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P15" t="s">
+        <v>112</v>
+      </c>
+      <c r="R15">
+        <v>3</v>
+      </c>
+      <c r="Y15">
+        <v>10</v>
+      </c>
+      <c r="Z15">
+        <v>14</v>
+      </c>
+      <c r="AB15">
+        <v>116</v>
+      </c>
+      <c r="AM15">
+        <v>5</v>
+      </c>
+      <c r="AP15">
+        <v>49</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.35">
@@ -1506,15 +1861,75 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" t="s">
+        <v>115</v>
+      </c>
       <c r="D17">
         <v>2009</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17" t="s">
+        <v>116</v>
+      </c>
+      <c r="F17" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" t="s">
+        <v>118</v>
+      </c>
+      <c r="K17">
+        <v>17</v>
+      </c>
+      <c r="L17" t="s">
+        <v>82</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17" t="s">
+        <v>119</v>
+      </c>
+      <c r="P17" t="s">
+        <v>120</v>
+      </c>
+      <c r="R17">
+        <v>6</v>
+      </c>
+      <c r="Y17">
+        <v>11</v>
+      </c>
+      <c r="Z17">
+        <v>65</v>
+      </c>
+      <c r="AB17">
+        <v>56</v>
+      </c>
+      <c r="AC17">
+        <v>26</v>
+      </c>
+      <c r="AD17">
+        <v>27</v>
+      </c>
+      <c r="AE17">
+        <v>5</v>
+      </c>
+      <c r="AM17">
+        <v>0</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1522,15 +1937,84 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19">
+    <row r="19" spans="1:47" ht="62" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
         <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" t="s">
+        <v>123</v>
       </c>
       <c r="D19">
         <v>2009</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G19" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" t="s">
+        <v>126</v>
+      </c>
+      <c r="K19">
+        <v>45</v>
+      </c>
+      <c r="L19" t="s">
+        <v>57</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>128</v>
+      </c>
+      <c r="R19">
+        <v>10</v>
+      </c>
+      <c r="S19">
+        <v>25</v>
+      </c>
+      <c r="Z19">
+        <v>24</v>
+      </c>
+      <c r="AA19">
+        <v>167</v>
+      </c>
+      <c r="AB19">
+        <v>14</v>
+      </c>
+      <c r="AC19">
+        <v>4</v>
+      </c>
+      <c r="AN19">
+        <v>106</v>
+      </c>
+      <c r="AO19">
+        <v>26</v>
+      </c>
+      <c r="AP19">
+        <v>67</v>
+      </c>
+      <c r="AR19">
+        <v>12</v>
+      </c>
+      <c r="AS19">
+        <v>12</v>
+      </c>
+      <c r="AU19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1538,15 +2022,78 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" t="s">
+        <v>130</v>
+      </c>
       <c r="D21">
         <v>2009</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E21" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" t="s">
+        <v>132</v>
+      </c>
+      <c r="G21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" t="s">
+        <v>133</v>
+      </c>
+      <c r="K21">
+        <v>15</v>
+      </c>
+      <c r="L21" t="s">
+        <v>57</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21" t="s">
+        <v>134</v>
+      </c>
+      <c r="P21" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>136</v>
+      </c>
+      <c r="R21">
+        <v>5</v>
+      </c>
+      <c r="Y21">
+        <v>8</v>
+      </c>
+      <c r="Z21">
+        <v>45</v>
+      </c>
+      <c r="AB21">
+        <v>67</v>
+      </c>
+      <c r="AC21">
+        <v>10</v>
+      </c>
+      <c r="AM21">
+        <v>2</v>
+      </c>
+      <c r="AN21">
+        <v>2</v>
+      </c>
+      <c r="AP21">
+        <v>33</v>
+      </c>
+      <c r="AT21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1554,15 +2101,75 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="B23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" t="s">
+        <v>138</v>
+      </c>
       <c r="D23">
         <v>2009</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E23" t="s">
+        <v>139</v>
+      </c>
+      <c r="F23" t="s">
+        <v>140</v>
+      </c>
+      <c r="G23" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" t="s">
+        <v>133</v>
+      </c>
+      <c r="K23">
+        <v>24</v>
+      </c>
+      <c r="L23" t="s">
+        <v>141</v>
+      </c>
+      <c r="M23" s="3">
+        <v>2</v>
+      </c>
+      <c r="N23" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>142</v>
+      </c>
+      <c r="R23">
+        <v>6</v>
+      </c>
+      <c r="Y23">
+        <v>12</v>
+      </c>
+      <c r="Z23">
+        <v>23</v>
+      </c>
+      <c r="AB23">
+        <v>93</v>
+      </c>
+      <c r="AC23">
+        <v>25</v>
+      </c>
+      <c r="AM23">
+        <v>0.5</v>
+      </c>
+      <c r="AN23">
+        <v>4</v>
+      </c>
+      <c r="AP23">
+        <v>3</v>
+      </c>
+      <c r="AT23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1570,7 +2177,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1578,7 +2185,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1586,7 +2193,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1594,7 +2201,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1602,7 +2209,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1610,7 +2217,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1618,7 +2225,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1626,7 +2233,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Fixed blue and green column order
</commit_message>
<xml_diff>
--- a/AlitoDataset.xlsx
+++ b/AlitoDataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jtsanz\alito-research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{1A84C31C-6443-41F0-9786-986150042EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A516A50-DFE6-4BBB-8348-DC204307B57E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
   </bookViews>
@@ -607,7 +607,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -621,12 +621,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1036,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060A011E-60FD-5047-91C8-6B9B09AABF05}">
   <dimension ref="A1:AZ79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="AP4" sqref="AP4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1061,29 +1055,29 @@
     <col min="17" max="17" width="11.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="8.5" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="13.5" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="13.83203125" bestFit="1" customWidth="1"/>
@@ -1155,10 +1149,10 @@
         <v>11</v>
       </c>
       <c r="T1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" t="s">
         <v>12</v>
-      </c>
-      <c r="U1" t="s">
-        <v>13</v>
       </c>
       <c r="V1" t="s">
         <v>14</v>
@@ -1176,10 +1170,10 @@
         <v>17</v>
       </c>
       <c r="AA1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB1" t="s">
         <v>18</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>19</v>
       </c>
       <c r="AC1" t="s">
         <v>20</v>
@@ -1197,10 +1191,10 @@
         <v>23</v>
       </c>
       <c r="AH1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI1" t="s">
         <v>24</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>25</v>
       </c>
       <c r="AJ1" t="s">
         <v>26</v>
@@ -1218,10 +1212,10 @@
         <v>32</v>
       </c>
       <c r="AO1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>35</v>
@@ -1374,9 +1368,6 @@
       <c r="AO3">
         <v>13</v>
       </c>
-      <c r="AP3">
-        <v>0</v>
-      </c>
       <c r="AQ3">
         <v>0</v>
       </c>
@@ -1486,7 +1477,7 @@
       <c r="AM5">
         <v>3.25</v>
       </c>
-      <c r="AP5">
+      <c r="AO5">
         <v>14</v>
       </c>
       <c r="AQ5">
@@ -1618,7 +1609,7 @@
       <c r="Z9">
         <v>44</v>
       </c>
-      <c r="AB9">
+      <c r="AA9">
         <v>125</v>
       </c>
       <c r="AM9">
@@ -1755,7 +1746,7 @@
       <c r="Z13">
         <v>10</v>
       </c>
-      <c r="AB13">
+      <c r="AA13">
         <v>231</v>
       </c>
       <c r="AC13">
@@ -1773,7 +1764,7 @@
       <c r="AN13">
         <v>11</v>
       </c>
-      <c r="AP13">
+      <c r="AO13">
         <v>71</v>
       </c>
       <c r="AS13">
@@ -1840,13 +1831,13 @@
       <c r="Z15">
         <v>14</v>
       </c>
-      <c r="AB15">
+      <c r="AA15">
         <v>116</v>
       </c>
       <c r="AM15">
         <v>5</v>
       </c>
-      <c r="AP15">
+      <c r="AO15">
         <v>49</v>
       </c>
       <c r="AT15" t="s">
@@ -1910,7 +1901,7 @@
       <c r="Z17">
         <v>65</v>
       </c>
-      <c r="AB17">
+      <c r="AA17">
         <v>56</v>
       </c>
       <c r="AC17">
@@ -1987,10 +1978,10 @@
         <v>24</v>
       </c>
       <c r="AA19">
+        <v>14</v>
+      </c>
+      <c r="AB19">
         <v>167</v>
-      </c>
-      <c r="AB19">
-        <v>14</v>
       </c>
       <c r="AC19">
         <v>4</v>
@@ -1999,10 +1990,10 @@
         <v>106</v>
       </c>
       <c r="AO19">
+        <v>67</v>
+      </c>
+      <c r="AP19">
         <v>26</v>
-      </c>
-      <c r="AP19">
-        <v>67</v>
       </c>
       <c r="AR19">
         <v>12</v>
@@ -2074,7 +2065,7 @@
       <c r="Z21">
         <v>45</v>
       </c>
-      <c r="AB21">
+      <c r="AA21">
         <v>67</v>
       </c>
       <c r="AC21">
@@ -2086,7 +2077,7 @@
       <c r="AN21">
         <v>2</v>
       </c>
-      <c r="AP21">
+      <c r="AO21">
         <v>33</v>
       </c>
       <c r="AT21" t="s">
@@ -2150,7 +2141,7 @@
       <c r="Z23">
         <v>23</v>
       </c>
-      <c r="AB23">
+      <c r="AA23">
         <v>93</v>
       </c>
       <c r="AC23">
@@ -2162,7 +2153,7 @@
       <c r="AN23">
         <v>4</v>
       </c>
-      <c r="AP23">
+      <c r="AO23">
         <v>3</v>
       </c>
       <c r="AT23" t="s">

</xml_diff>

<commit_message>
2010 and 11 done
</commit_message>
<xml_diff>
--- a/AlitoDataset.xlsx
+++ b/AlitoDataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jtsanz\alito-research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A516A50-DFE6-4BBB-8348-DC204307B57E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BB6242-05B1-4794-9257-9E7A777D0510}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
+    <workbookView xWindow="11300" yWindow="2120" windowWidth="14400" windowHeight="7360" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,7 @@
     <author>tc={F4821384-192B-DD46-8791-617913EBCE89}</author>
     <author>tc={61D1E5EF-D958-4E20-BF68-DEC3C3DFE074}</author>
     <author>tc={4374D2CD-142A-774C-8170-13C907E414CA}</author>
+    <author>tc={D47810E7-0E09-4CE8-AF5A-5F29BA3FA07D}</author>
     <author>tc={CB9ADD91-1443-1F48-98DF-AB39A6962234}</author>
     <author>tc={D87AAAD5-35CC-CC42-A5C6-41D0FE831863}</author>
     <author>tc={AF001A8C-E6AA-3349-9BE9-89B0E896018A}</author>
@@ -48,6 +49,8 @@
     <author>tc={2810AD96-B8B6-4798-A014-AFDE2C354919}</author>
     <author>tc={3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}</author>
     <author>tc={93985E51-4186-401D-B292-10D9DC17CEB8}</author>
+    <author>tc={916A852D-1D9C-43FD-9526-91B03FAC048E}</author>
+    <author>tc={A4DC1BA9-4A23-4C06-A9DF-A3D4F083B19B}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5010FC8D-4B2F-2744-9AA3-E06DCDD6F440}">
@@ -82,7 +85,15 @@
     separate by commas</t>
       </text>
     </comment>
-    <comment ref="J1" authorId="4" shapeId="0" xr:uid="{CB9ADD91-1443-1F48-98DF-AB39A6962234}">
+    <comment ref="F1" authorId="4" shapeId="0" xr:uid="{D47810E7-0E09-4CE8-AF5A-5F29BA3FA07D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    There can be multiple questions; what do you want to put as divider between them? I put a | sign</t>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="5" shapeId="0" xr:uid="{CB9ADD91-1443-1F48-98DF-AB39A6962234}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -92,7 +103,7 @@
     basis for difference? more info :)</t>
       </text>
     </comment>
-    <comment ref="M1" authorId="5" shapeId="0" xr:uid="{D87AAAD5-35CC-CC42-A5C6-41D0FE831863}">
+    <comment ref="M1" authorId="6" shapeId="0" xr:uid="{D87AAAD5-35CC-CC42-A5C6-41D0FE831863}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -100,7 +111,7 @@
     For now, split into 3 groups: 0 if unanimous, 1 if contentious, 2 if ambiguous</t>
       </text>
     </comment>
-    <comment ref="N1" authorId="6" shapeId="0" xr:uid="{AF001A8C-E6AA-3349-9BE9-89B0E896018A}">
+    <comment ref="N1" authorId="7" shapeId="0" xr:uid="{AF001A8C-E6AA-3349-9BE9-89B0E896018A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -108,7 +119,7 @@
     who wrote;justice joined by,justice:new who wrote;justice</t>
       </text>
     </comment>
-    <comment ref="R1" authorId="7" shapeId="0" xr:uid="{612DC64F-C5FE-40F8-BAF2-EF4FD089D0F2}">
+    <comment ref="R1" authorId="8" shapeId="0" xr:uid="{612DC64F-C5FE-40F8-BAF2-EF4FD089D0F2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -116,7 +127,7 @@
     Sometimes there is a background section that isn't included in the total count, how do you want to handle?</t>
       </text>
     </comment>
-    <comment ref="AF1" authorId="8" shapeId="0" xr:uid="{C4848F86-CB4C-45EE-8700-3A7450D7769A}">
+    <comment ref="AF1" authorId="9" shapeId="0" xr:uid="{C4848F86-CB4C-45EE-8700-3A7450D7769A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -124,7 +135,7 @@
     Add together with MA1</t>
       </text>
     </comment>
-    <comment ref="AT1" authorId="9" shapeId="0" xr:uid="{0F4748BD-5B03-439A-B8A7-8872FFB421BA}">
+    <comment ref="AT1" authorId="10" shapeId="0" xr:uid="{0F4748BD-5B03-439A-B8A7-8872FFB421BA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -132,7 +143,7 @@
     Apparently length sometimes has the format of Length (pgs) 2 lines? Want to do 2l for 2 lines or something like that?</t>
       </text>
     </comment>
-    <comment ref="G7" authorId="10" shapeId="0" xr:uid="{2810AD96-B8B6-4798-A014-AFDE2C354919}">
+    <comment ref="G7" authorId="11" shapeId="0" xr:uid="{2810AD96-B8B6-4798-A014-AFDE2C354919}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -140,7 +151,7 @@
     No Yes/No answer given: just explanations;</t>
       </text>
     </comment>
-    <comment ref="A19" authorId="11" shapeId="0" xr:uid="{3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}">
+    <comment ref="A19" authorId="12" shapeId="0" xr:uid="{3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -148,7 +159,7 @@
     missing lengths on a lot of sections, but have line count highlights</t>
       </text>
     </comment>
-    <comment ref="M23" authorId="12" shapeId="0" xr:uid="{93985E51-4186-401D-B292-10D9DC17CEB8}">
+    <comment ref="M23" authorId="13" shapeId="0" xr:uid="{93985E51-4186-401D-B292-10D9DC17CEB8}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -156,12 +167,28 @@
     it's 5-3, is this contentious or ambigious? haha</t>
       </text>
     </comment>
+    <comment ref="G31" authorId="14" shapeId="0" xr:uid="{916A852D-1D9C-43FD-9526-91B03FAC048E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not sure what to put as the answer here: "Pharmaceutical sales reps are outside salesmen"</t>
+      </text>
+    </comment>
+    <comment ref="A36" authorId="15" shapeId="0" xr:uid="{A4DC1BA9-4A23-4C06-A9DF-A3D4F083B19B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    accidentally got out of order, my b haha</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="190">
   <si>
     <t>Case Name</t>
   </si>
@@ -602,12 +629,155 @@
   <si>
     <t>Ginsburg;Stevens,Breyer</t>
   </si>
+  <si>
+    <t>Global-Tech Appliances v. SEB</t>
+  </si>
+  <si>
+    <t>563 U.S. 754 (2011)</t>
+  </si>
+  <si>
+    <t>35 U. S. C. §271(b)</t>
+  </si>
+  <si>
+    <t>Does induced infringement under the patent clause require knowledge that the induced acts constitute patent infringement?</t>
+  </si>
+  <si>
+    <t>precedent and pragmatism</t>
+  </si>
+  <si>
+    <t>8,1</t>
+  </si>
+  <si>
+    <t>Kennedy</t>
+  </si>
+  <si>
+    <t>Kentucky v. King</t>
+  </si>
+  <si>
+    <t>563 U.S. 452 (2011)</t>
+  </si>
+  <si>
+    <t>The exclusionary rule</t>
+  </si>
+  <si>
+    <t>Does the exclusionary rule, which forbids the use of illegally seized evidence except in emergency situations, apply when the emergency is created by lawful police actions?</t>
+  </si>
+  <si>
+    <t>practical considerations</t>
+  </si>
+  <si>
+    <t>Alito;Scalia,Breyer,Ginsburg,Sotomayor,Kagan,Roberts,Thomas</t>
+  </si>
+  <si>
+    <t>Alito;Scalia,Breyer,Sotomayor,Kagan,Roberts,Kennedy,Thomas</t>
+  </si>
+  <si>
+    <t>Ginsburg</t>
+  </si>
+  <si>
+    <t>Wall v. Kholi</t>
+  </si>
+  <si>
+    <t>562 U.S. 545 (2011)</t>
+  </si>
+  <si>
+    <t>Statute of limitations under AEDPA</t>
+  </si>
+  <si>
+    <t>“Inmates have one year to file a habeas challenge to their sentence in federal court after conviction. The running of that time is delayed while the conviction is under review in state court. Is the time also tolled while a state court considers an inmate's request for a sentence reduction?"</t>
+  </si>
+  <si>
+    <t>pragmatism and precendent</t>
+  </si>
+  <si>
+    <t>Alito;Scalia,Breyer,Sotomayor,Kagan,Roberts,Kennedy,Thomas,Ginsburg</t>
+  </si>
+  <si>
+    <t>Christopher v. Smithkline</t>
+  </si>
+  <si>
+    <t>567 U.S. 143 (2012)</t>
+  </si>
+  <si>
+    <t>Fair Labor Standards Act</t>
+  </si>
+  <si>
+    <t>Pragmatic</t>
+  </si>
+  <si>
+    <t>Kagan;Sotomayor,Ginsburg,Breyer</t>
+  </si>
+  <si>
+    <t>Howes v. Fields</t>
+  </si>
+  <si>
+    <t>565 U.S. 499 (2012)</t>
+  </si>
+  <si>
+    <t>Miranda</t>
+  </si>
+  <si>
+    <t>Must Glaxo and the courts defer to the Secretary of Labor's definition of "outside
+salesman" under the Fair Labor Standards Act?|Does the Secretary of Labor's definition of "outside salesman" apply to
+pharmaceutical sales representatives?</t>
+  </si>
+  <si>
+    <t>Does federal law automatically require Miranda warnings before questioning jail or prison inmates about issues unrelated to the cases for which they were incarcerated?</t>
+  </si>
+  <si>
+    <t>pramatic and precedent</t>
+  </si>
+  <si>
+    <t>6,3</t>
+  </si>
+  <si>
+    <t>Alito;Thomas,Scalia,Kennedy,Roberts,Kagan</t>
+  </si>
+  <si>
+    <t>Sotomayor;Ginsburg,Breyer</t>
+  </si>
+  <si>
+    <t>Rehberg v. Paulk</t>
+  </si>
+  <si>
+    <t>556 U.S. 356 (2012)</t>
+  </si>
+  <si>
+    <t>Grand jury witness immunity in a §1983 action</t>
+  </si>
+  <si>
+    <t>Are government officials who initiate prosecutions by providing false testimony in judicial proceedings absolutely immune from civil suit?</t>
+  </si>
+  <si>
+    <t>precendent</t>
+  </si>
+  <si>
+    <t>Alito;Scalia,Roberts,Kennedy,Thomas,Ginsburg,Breyer,Sotomaor,Kagan</t>
+  </si>
+  <si>
+    <t>Williams v. Illinois</t>
+  </si>
+  <si>
+    <t>567 U.S. 50 (2012)</t>
+  </si>
+  <si>
+    <t>6th Amendment Confrontation Clause</t>
+  </si>
+  <si>
+    <t>"Can an expert witness be called as a stand-in for a lab analyst who actually did a test on criminal evidence, but did not appear at the trial?"</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Kennedy,Thomas,Breyer</t>
+  </si>
+  <si>
+    <t>Scalia;Ginsburg,Sotomayor,Kaga</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -621,6 +791,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -993,6 +1169,9 @@
   <threadedComment ref="E1" dT="2020-06-30T03:53:05.01" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{4374D2CD-142A-774C-8170-13C907E414CA}">
     <text>separate by commas</text>
   </threadedComment>
+  <threadedComment ref="F1" dT="2020-07-17T02:57:23.57" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{D47810E7-0E09-4CE8-AF5A-5F29BA3FA07D}">
+    <text>There can be multiple questions; what do you want to put as divider between them? I put a | sign</text>
+  </threadedComment>
   <threadedComment ref="J1" dT="2020-06-29T21:33:16.24" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{CB9ADD91-1443-1F48-98DF-AB39A6962234}">
     <text>1 if characterized answer and oyez answer differ, 0 else</text>
   </threadedComment>
@@ -1023,6 +1202,12 @@
   <threadedComment ref="M23" dT="2020-07-05T08:11:32.10" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{93985E51-4186-401D-B292-10D9DC17CEB8}">
     <text>it's 5-3, is this contentious or ambigious? haha</text>
   </threadedComment>
+  <threadedComment ref="G31" dT="2020-07-17T02:59:12.36" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{916A852D-1D9C-43FD-9526-91B03FAC048E}">
+    <text>Not sure what to put as the answer here: "Pharmaceutical sales reps are outside salesmen"</text>
+  </threadedComment>
+  <threadedComment ref="A36" dT="2020-07-17T03:38:46.55" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{A4DC1BA9-4A23-4C06-A9DF-A3D4F083B19B}">
+    <text>accidentally got out of order, my b haha</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1030,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060A011E-60FD-5047-91C8-6B9B09AABF05}">
   <dimension ref="A1:AZ79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="AP4" sqref="AP4"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1106,7 +1291,7 @@
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
@@ -2172,8 +2357,65 @@
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" t="s">
+        <v>144</v>
+      </c>
       <c r="D25">
         <v>2010</v>
+      </c>
+      <c r="E25" t="s">
+        <v>145</v>
+      </c>
+      <c r="F25" t="s">
+        <v>146</v>
+      </c>
+      <c r="G25" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" t="s">
+        <v>147</v>
+      </c>
+      <c r="K25">
+        <v>16</v>
+      </c>
+      <c r="L25" t="s">
+        <v>148</v>
+      </c>
+      <c r="M25">
+        <v>2</v>
+      </c>
+      <c r="N25" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>149</v>
+      </c>
+      <c r="R25">
+        <v>3</v>
+      </c>
+      <c r="Y25">
+        <v>11.5</v>
+      </c>
+      <c r="Z25">
+        <v>69</v>
+      </c>
+      <c r="AA25">
+        <v>37</v>
+      </c>
+      <c r="AE25">
+        <v>14</v>
+      </c>
+      <c r="AM25">
+        <v>0.5</v>
+      </c>
+      <c r="AO25">
+        <v>6</v>
+      </c>
+      <c r="AT25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:47" x14ac:dyDescent="0.35">
@@ -2188,8 +2430,68 @@
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27" t="s">
+        <v>150</v>
+      </c>
+      <c r="C27" t="s">
+        <v>151</v>
+      </c>
       <c r="D27">
         <v>2010</v>
+      </c>
+      <c r="E27" t="s">
+        <v>152</v>
+      </c>
+      <c r="F27" t="s">
+        <v>153</v>
+      </c>
+      <c r="G27" t="s">
+        <v>74</v>
+      </c>
+      <c r="H27" t="s">
+        <v>154</v>
+      </c>
+      <c r="K27">
+        <v>19</v>
+      </c>
+      <c r="L27" t="s">
+        <v>148</v>
+      </c>
+      <c r="M27">
+        <v>2</v>
+      </c>
+      <c r="N27" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>157</v>
+      </c>
+      <c r="R27">
+        <v>4</v>
+      </c>
+      <c r="Y27">
+        <v>7</v>
+      </c>
+      <c r="Z27">
+        <v>44</v>
+      </c>
+      <c r="AA27">
+        <v>41</v>
+      </c>
+      <c r="AC27">
+        <v>12</v>
+      </c>
+      <c r="AM27">
+        <v>7.5</v>
+      </c>
+      <c r="AN27">
+        <v>24</v>
+      </c>
+      <c r="AO27">
+        <v>129</v>
+      </c>
+      <c r="AT27">
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:47" x14ac:dyDescent="0.35">
@@ -2204,8 +2506,74 @@
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" t="s">
+        <v>158</v>
+      </c>
+      <c r="C29" t="s">
+        <v>159</v>
+      </c>
       <c r="D29">
         <v>2010</v>
+      </c>
+      <c r="E29" t="s">
+        <v>160</v>
+      </c>
+      <c r="F29" t="s">
+        <v>161</v>
+      </c>
+      <c r="G29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" t="s">
+        <v>162</v>
+      </c>
+      <c r="K29">
+        <v>15</v>
+      </c>
+      <c r="L29" t="s">
+        <v>82</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>163</v>
+      </c>
+      <c r="R29">
+        <v>4.5</v>
+      </c>
+      <c r="Y29">
+        <v>6</v>
+      </c>
+      <c r="Z29">
+        <v>42</v>
+      </c>
+      <c r="AA29">
+        <v>22</v>
+      </c>
+      <c r="AC29">
+        <v>6</v>
+      </c>
+      <c r="AE29">
+        <v>52</v>
+      </c>
+      <c r="AM29">
+        <v>4.5</v>
+      </c>
+      <c r="AN29">
+        <v>20</v>
+      </c>
+      <c r="AO29">
+        <v>39</v>
+      </c>
+      <c r="AQ29">
+        <v>18</v>
+      </c>
+      <c r="AS29">
+        <v>3</v>
+      </c>
+      <c r="AT29">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:47" x14ac:dyDescent="0.35">
@@ -2216,12 +2584,82 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:47" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" t="s">
+        <v>165</v>
+      </c>
       <c r="D31">
         <v>2011</v>
+      </c>
+      <c r="E31" t="s">
+        <v>166</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G31" s="3"/>
+      <c r="H31" t="s">
+        <v>167</v>
+      </c>
+      <c r="K31">
+        <v>25</v>
+      </c>
+      <c r="L31" t="s">
+        <v>57</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>168</v>
+      </c>
+      <c r="R31">
+        <v>8</v>
+      </c>
+      <c r="V31">
+        <v>3</v>
+      </c>
+      <c r="Y31">
+        <v>13</v>
+      </c>
+      <c r="Z31">
+        <v>24</v>
+      </c>
+      <c r="AA31">
+        <v>86</v>
+      </c>
+      <c r="AC31">
+        <v>19</v>
+      </c>
+      <c r="AD31">
+        <v>11</v>
+      </c>
+      <c r="AE31">
+        <v>67</v>
+      </c>
+      <c r="AM31">
+        <v>5</v>
+      </c>
+      <c r="AO31">
+        <v>47</v>
+      </c>
+      <c r="AQ31">
+        <v>3</v>
+      </c>
+      <c r="AS31">
+        <v>51</v>
+      </c>
+      <c r="AT31">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:47" x14ac:dyDescent="0.35">
@@ -2232,15 +2670,63 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
+      <c r="B33" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" t="s">
+        <v>170</v>
+      </c>
       <c r="D33">
         <v>2011</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E33" t="s">
+        <v>171</v>
+      </c>
+      <c r="F33" t="s">
+        <v>173</v>
+      </c>
+      <c r="G33" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" t="s">
+        <v>174</v>
+      </c>
+      <c r="K33">
+        <v>16</v>
+      </c>
+      <c r="L33" t="s">
+        <v>175</v>
+      </c>
+      <c r="M33">
+        <v>2</v>
+      </c>
+      <c r="N33" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>177</v>
+      </c>
+      <c r="R33">
+        <v>4</v>
+      </c>
+      <c r="Z33">
+        <v>63</v>
+      </c>
+      <c r="AA33">
+        <v>181</v>
+      </c>
+      <c r="AN33">
+        <v>56</v>
+      </c>
+      <c r="AZ33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2248,31 +2734,152 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
+      <c r="B35" t="s">
+        <v>178</v>
+      </c>
+      <c r="C35" t="s">
+        <v>179</v>
+      </c>
       <c r="D35">
         <v>2011</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36">
+      <c r="E35" t="s">
+        <v>180</v>
+      </c>
+      <c r="F35" t="s">
+        <v>181</v>
+      </c>
+      <c r="G35" t="s">
+        <v>74</v>
+      </c>
+      <c r="H35" t="s">
+        <v>182</v>
+      </c>
+      <c r="K35">
+        <v>18</v>
+      </c>
+      <c r="L35" t="s">
+        <v>82</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35" t="s">
+        <v>183</v>
+      </c>
+      <c r="R35">
+        <v>2.5</v>
+      </c>
+      <c r="Y35">
+        <v>9.5</v>
+      </c>
+      <c r="Z35">
+        <v>111</v>
+      </c>
+      <c r="AA35">
+        <v>58</v>
+      </c>
+      <c r="AC35">
+        <v>8</v>
+      </c>
+      <c r="AM35">
+        <v>4.5</v>
+      </c>
+      <c r="AO35">
+        <v>81</v>
+      </c>
+      <c r="AP35">
+        <v>20</v>
+      </c>
+      <c r="AT35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
+      <c r="B36" t="s">
+        <v>184</v>
+      </c>
+      <c r="C36" t="s">
+        <v>185</v>
+      </c>
       <c r="D36">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2012</v>
+      </c>
+      <c r="E36" t="s">
+        <v>186</v>
+      </c>
+      <c r="F36" t="s">
+        <v>187</v>
+      </c>
+      <c r="G36" t="s">
+        <v>74</v>
+      </c>
+      <c r="H36" t="s">
+        <v>182</v>
+      </c>
+      <c r="K36">
+        <v>33</v>
+      </c>
+      <c r="L36" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>189</v>
+      </c>
+      <c r="R36">
+        <v>11</v>
+      </c>
+      <c r="S36">
+        <v>74</v>
+      </c>
+      <c r="Y36">
+        <v>11.5</v>
+      </c>
+      <c r="Z36">
+        <v>156</v>
+      </c>
+      <c r="AA36">
+        <v>108</v>
+      </c>
+      <c r="AB36">
+        <v>19</v>
+      </c>
+      <c r="AM36">
+        <v>10</v>
+      </c>
+      <c r="AN36">
+        <v>12</v>
+      </c>
+      <c r="AO36">
+        <v>200</v>
+      </c>
+      <c r="AS36">
+        <v>20</v>
+      </c>
+      <c r="AT36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="D37">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="L37" s="7"/>
+    </row>
+    <row r="38" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2280,7 +2887,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2288,7 +2895,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2296,7 +2903,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2304,7 +2911,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2312,7 +2919,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2320,7 +2927,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2328,7 +2935,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2336,7 +2943,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2344,7 +2951,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2352,7 +2959,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
odds through 15 done
</commit_message>
<xml_diff>
--- a/AlitoDataset.xlsx
+++ b/AlitoDataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jtsanz\alito-research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineparnell/alito-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BB6242-05B1-4794-9257-9E7A777D0510}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBDFAD1-890E-D04C-8A62-59BDADF54E08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11300" yWindow="2120" windowWidth="14400" windowHeight="7360" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
+    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,11 @@
     <author>tc={D87AAAD5-35CC-CC42-A5C6-41D0FE831863}</author>
     <author>tc={AF001A8C-E6AA-3349-9BE9-89B0E896018A}</author>
     <author>tc={612DC64F-C5FE-40F8-BAF2-EF4FD089D0F2}</author>
-    <author>tc={C4848F86-CB4C-45EE-8700-3A7450D7769A}</author>
     <author>tc={0F4748BD-5B03-439A-B8A7-8872FFB421BA}</author>
     <author>tc={2810AD96-B8B6-4798-A014-AFDE2C354919}</author>
+    <author>tc={3A0F3EBF-F4B9-214C-9AA5-DBFCC7D44035}</author>
+    <author>tc={915C01E3-6C9F-0E49-9FDE-186D12E45115}</author>
+    <author>tc={85C62DE5-A215-7844-ADDB-F6A767BB5222}</author>
     <author>tc={3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}</author>
     <author>tc={93985E51-4186-401D-B292-10D9DC17CEB8}</author>
     <author>tc={916A852D-1D9C-43FD-9526-91B03FAC048E}</author>
@@ -127,15 +129,7 @@
     Sometimes there is a background section that isn't included in the total count, how do you want to handle?</t>
       </text>
     </comment>
-    <comment ref="AF1" authorId="9" shapeId="0" xr:uid="{C4848F86-CB4C-45EE-8700-3A7450D7769A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Add together with MA1</t>
-      </text>
-    </comment>
-    <comment ref="AT1" authorId="10" shapeId="0" xr:uid="{0F4748BD-5B03-439A-B8A7-8872FFB421BA}">
+    <comment ref="AM1" authorId="9" shapeId="0" xr:uid="{0F4748BD-5B03-439A-B8A7-8872FFB421BA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -143,7 +137,7 @@
     Apparently length sometimes has the format of Length (pgs) 2 lines? Want to do 2l for 2 lines or something like that?</t>
       </text>
     </comment>
-    <comment ref="G7" authorId="11" shapeId="0" xr:uid="{2810AD96-B8B6-4798-A014-AFDE2C354919}">
+    <comment ref="G7" authorId="10" shapeId="0" xr:uid="{2810AD96-B8B6-4798-A014-AFDE2C354919}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -151,7 +145,31 @@
     No Yes/No answer given: just explanations;</t>
       </text>
     </comment>
-    <comment ref="A19" authorId="12" shapeId="0" xr:uid="{3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}">
+    <comment ref="F10" authorId="11" shapeId="0" xr:uid="{3A0F3EBF-F4B9-214C-9AA5-DBFCC7D44035}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    There are three different ones?</t>
+      </text>
+    </comment>
+    <comment ref="AM10" authorId="12" shapeId="0" xr:uid="{915C01E3-6C9F-0E49-9FDE-186D12E45115}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    6 lines</t>
+      </text>
+    </comment>
+    <comment ref="AM14" authorId="13" shapeId="0" xr:uid="{85C62DE5-A215-7844-ADDB-F6A767BB5222}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    5 lines</t>
+      </text>
+    </comment>
+    <comment ref="A19" authorId="14" shapeId="0" xr:uid="{3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -159,7 +177,7 @@
     missing lengths on a lot of sections, but have line count highlights</t>
       </text>
     </comment>
-    <comment ref="M23" authorId="13" shapeId="0" xr:uid="{93985E51-4186-401D-B292-10D9DC17CEB8}">
+    <comment ref="M23" authorId="15" shapeId="0" xr:uid="{93985E51-4186-401D-B292-10D9DC17CEB8}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -167,7 +185,7 @@
     it's 5-3, is this contentious or ambigious? haha</t>
       </text>
     </comment>
-    <comment ref="G31" authorId="14" shapeId="0" xr:uid="{916A852D-1D9C-43FD-9526-91B03FAC048E}">
+    <comment ref="G31" authorId="16" shapeId="0" xr:uid="{916A852D-1D9C-43FD-9526-91B03FAC048E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -175,7 +193,7 @@
     Not sure what to put as the answer here: "Pharmaceutical sales reps are outside salesmen"</t>
       </text>
     </comment>
-    <comment ref="A36" authorId="15" shapeId="0" xr:uid="{A4DC1BA9-4A23-4C06-A9DF-A3D4F083B19B}">
+    <comment ref="A36" authorId="17" shapeId="0" xr:uid="{A4DC1BA9-4A23-4C06-A9DF-A3D4F083B19B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -188,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="222">
   <si>
     <t>Case Name</t>
   </si>
@@ -259,27 +277,6 @@
     <t>MA1-Count-Yellow</t>
   </si>
   <si>
-    <t>MA2-Count-Pink</t>
-  </si>
-  <si>
-    <t>MA2-Count-Blue</t>
-  </si>
-  <si>
-    <t>MA2-Count Green</t>
-  </si>
-  <si>
-    <t>MA2-Count-Orange</t>
-  </si>
-  <si>
-    <t>MA2-Count-Purple</t>
-  </si>
-  <si>
-    <t>MA2-Count-Yellow</t>
-  </si>
-  <si>
-    <t>MA2-Length</t>
-  </si>
-  <si>
     <t>MA1-Length</t>
   </si>
   <si>
@@ -335,9 +332,6 @@
   </si>
   <si>
     <t>Hein v. Freedom From Religion Foundation, Inc.</t>
-  </si>
-  <si>
-    <t>551 US 587 (2007)</t>
   </si>
   <si>
     <t>Establishment Clause, First Amendment,Case or Controversy Clause, Article III: Standing</t>
@@ -352,9 +346,6 @@
   </si>
   <si>
     <t>National Association of Home Builders et al v. Defenders of Wildlife et al.</t>
-  </si>
-  <si>
-    <t>551 US 644 (2007)</t>
   </si>
   <si>
     <t>Section 402(b) of the Clean Water Act,Section 7(a)(2) of the Endangered Species Act of 1973</t>
@@ -387,9 +378,6 @@
     <t>Ledbetter v. The Good Year Tire &amp; Rubber Company, Inc.</t>
   </si>
   <si>
-    <t>550 US 618 (2007)</t>
-  </si>
-  <si>
     <t>Title VII of the Civil Rights Act of 1964</t>
   </si>
   <si>
@@ -425,12 +413,6 @@
   </si>
   <si>
     <t>MeadWestvaco Corporation v. Illinois Department of Revenue</t>
-  </si>
-  <si>
-    <t>553 US 662 (2008)</t>
-  </si>
-  <si>
-    <t>553 US 16 (2008)</t>
   </si>
   <si>
     <t>Doctrinal question re: how a prior case does or doesn’t control the current tax and
@@ -492,9 +474,6 @@
     <t>Is Title IX’s implied private remedy sufficiently comprehensive to preclude the use of 42 U.S.C. Section 1983 to advance sex discrimination claims against  federally funded institutions?</t>
   </si>
   <si>
-    <t>Alito;Roberts,Stevens,Scalia, Kennedy,Souter,Thomas,Ginsburg,Breyer</t>
-  </si>
-  <si>
     <t>0/4</t>
   </si>
   <si>
@@ -553,9 +532,6 @@
   </si>
   <si>
     <t>Did the Seventh Circuit err in holding that claims alleging mutual fund management&amp;#39;s fees were too high is not cognizable under Section 36(b) of the Investment Company Act, when that holding is in conflict with those in three other circuits?</t>
-  </si>
-  <si>
-    <t>mostly doctrinal and pragmatic</t>
   </si>
   <si>
     <t>Alito;Roberts,Stevens,Scalia,Kennedy,Ginsburg,Breyer,Sotomayor</t>
@@ -771,6 +747,144 @@
   </si>
   <si>
     <t>Scalia;Ginsburg,Sotomayor,Kaga</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Kennedy</t>
+  </si>
+  <si>
+    <t>Kennedy:Scalia;Thomas</t>
+  </si>
+  <si>
+    <t>Souter;Stevens,Ginsburg</t>
+  </si>
+  <si>
+    <t>Roberts,Scalia,Kennedy,Thomas,Alito</t>
+  </si>
+  <si>
+    <t>Stevens,Souter,Ginsburg,Breyer</t>
+  </si>
+  <si>
+    <t>Davis v. FEC</t>
+  </si>
+  <si>
+    <t>554 U.S. 724 (2008)</t>
+  </si>
+  <si>
+    <t>553 U.S. 662 (2008)</t>
+  </si>
+  <si>
+    <t>551 U.S. 644 (2007)</t>
+  </si>
+  <si>
+    <t>550 U.S. 618 (2007)</t>
+  </si>
+  <si>
+    <t>551 U.S. 587 (2007)</t>
+  </si>
+  <si>
+    <t>Campaign finance laws and the 1st Amendment (&amp; Equal Protection principle of 5th)</t>
+  </si>
+  <si>
+    <t>Does the Millionaire's Amendment to the 2002 campaign finance law, which raises the contribution limit for those running against a self-financed candidate, violate free speech clause of the First Amendment and the equal protection principle of the Fifth Amendment?</t>
+  </si>
+  <si>
+    <t>Mainly doctrinal analysis re: Buckley precedent, pragmatic discussion showing impact</t>
+  </si>
+  <si>
+    <t>Alito,Thomas,Scalia,Roberts,Kennedy</t>
+  </si>
+  <si>
+    <t>Richlin Security Service Co. v. Chertoff</t>
+  </si>
+  <si>
+    <t>553 U.S. 571 (2008)</t>
+  </si>
+  <si>
+    <t>553 U.S. 16 (2008)</t>
+  </si>
+  <si>
+    <t>Equal Access to Justice Act – reimbursement rates for “fees and other expenses”</t>
+  </si>
+  <si>
+    <t>Is a plaintiff who has successfully sued the federal government entitled to reimbursement of paralegal feels at market rates or as an expense compensable at cost ot the firm under the Equal Access to Justice Act, which allows for recovery of "fees and other expenses" incurred in the proceedings?</t>
+  </si>
+  <si>
+    <t>two parts, one textual, one doctrinal</t>
+  </si>
+  <si>
+    <t>U.S. v. Rodriquez</t>
+  </si>
+  <si>
+    <t>553 U.S. 377 (2008)</t>
+  </si>
+  <si>
+    <t>Armed Career Criminal Act (ACCA) 18 U.S.C. §924(e)(2)(A)(ii)</t>
+  </si>
+  <si>
+    <t>green and yellow reasons</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Stevens,Scalia,Kennedy,Souter,Thomas,Ginsburg,Breyer</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Scalia,Kennedy,Thomas,Breyer</t>
+  </si>
+  <si>
+    <t>Hawaii v. Office of Hawaiian Affairs</t>
+  </si>
+  <si>
+    <t>556 U.S. 163 (2009)</t>
+  </si>
+  <si>
+    <t>Apology resolution</t>
+  </si>
+  <si>
+    <t>Does the symbolic Apology Resolution restrict the State of Hawaii's sovereign authority to transfer publicly held land for private development, at least until claims over such land are resolved?</t>
+  </si>
+  <si>
+    <t>employs a lot of textualism</t>
+  </si>
+  <si>
+    <t>Alito,Roberts,Stevens,Scalia,Kennedy,Souter,Thomas,Ginsburg,Breyer</t>
+  </si>
+  <si>
+    <t>Kansas v. Colorado</t>
+  </si>
+  <si>
+    <t>556 U.S. 98 (2009)</t>
+  </si>
+  <si>
+    <t>28 USC §1821(b)</t>
+  </si>
+  <si>
+    <t>Should expert witness attendance fees available in cases brought before the supreme court be the same as those available in the federal district courts?</t>
+  </si>
+  <si>
+    <t>pragmatic</t>
+  </si>
+  <si>
+    <t>Roberts;Souter</t>
+  </si>
+  <si>
+    <t>Hamilton v. Lanning</t>
+  </si>
+  <si>
+    <t>560 U.S. 505 (2010)</t>
+  </si>
+  <si>
+    <t>Chapter 13 Repayment Plan</t>
+  </si>
+  <si>
+    <t>In calculating a debtor's "projected disposable income", may the bankruptcy court consider evidence suggesting that the debtor's income or expenses during that period are likely to be different from the debtor's income or expenses during the pre-filing period?</t>
+  </si>
+  <si>
+    <t>bankruptcy courts should use a forward looking approach. Mostly orange and yellow</t>
+  </si>
+  <si>
+    <t>Alito,Thomas,Kagan,Sotomayor,Ginsburg,Breyer,Kennedy,Roberts</t>
+  </si>
+  <si>
+    <t>Scalia</t>
   </si>
 </sst>
 </file>
@@ -793,10 +907,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -825,7 +939,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -836,6 +950,7 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1187,14 +1302,20 @@
   <threadedComment ref="R1" dT="2020-07-01T18:26:19.91" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{612DC64F-C5FE-40F8-BAF2-EF4FD089D0F2}">
     <text>Sometimes there is a background section that isn't included in the total count, how do you want to handle?</text>
   </threadedComment>
-  <threadedComment ref="AF1" dT="2020-07-01T19:57:27.40" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{C4848F86-CB4C-45EE-8700-3A7450D7769A}">
-    <text>Add together with MA1</text>
-  </threadedComment>
-  <threadedComment ref="AT1" dT="2020-07-01T18:21:57.37" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{0F4748BD-5B03-439A-B8A7-8872FFB421BA}">
+  <threadedComment ref="AM1" dT="2020-07-01T18:21:57.37" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{0F4748BD-5B03-439A-B8A7-8872FFB421BA}">
     <text>Apparently length sometimes has the format of Length (pgs) 2 lines? Want to do 2l for 2 lines or something like that?</text>
   </threadedComment>
   <threadedComment ref="G7" dT="2020-07-01T18:30:00.55" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{2810AD96-B8B6-4798-A014-AFDE2C354919}">
     <text>No Yes/No answer given: just explanations;</text>
+  </threadedComment>
+  <threadedComment ref="F10" dT="2020-07-17T13:39:40.63" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{3A0F3EBF-F4B9-214C-9AA5-DBFCC7D44035}">
+    <text>There are three different ones?</text>
+  </threadedComment>
+  <threadedComment ref="AM10" dT="2020-07-17T13:45:40.48" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{915C01E3-6C9F-0E49-9FDE-186D12E45115}">
+    <text>6 lines</text>
+  </threadedComment>
+  <threadedComment ref="AM14" dT="2020-07-17T14:06:17.88" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{85C62DE5-A215-7844-ADDB-F6A767BB5222}">
+    <text>5 lines</text>
   </threadedComment>
   <threadedComment ref="A19" dT="2020-07-05T08:06:57.89" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}">
     <text>missing lengths on a lot of sections, but have line count highlights</text>
@@ -1213,13 +1334,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060A011E-60FD-5047-91C8-6B9B09AABF05}">
-  <dimension ref="A1:AZ79"/>
+  <dimension ref="A1:AS79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="S5" workbookViewId="0">
+      <selection activeCell="AT16" sqref="AT16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
@@ -1252,32 +1373,25 @@
     <col min="29" max="29" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1304,7 +1418,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -1313,19 +1427,19 @@
         <v>9</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>10</v>
@@ -1349,7 +1463,7 @@
         <v>16</v>
       </c>
       <c r="Y1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="Z1" t="s">
         <v>17</v>
@@ -1369,38 +1483,38 @@
       <c r="AE1" t="s">
         <v>22</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AM1" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="AO1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>35</v>
@@ -1411,120 +1525,174 @@
       <c r="AS1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AT1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:52" ht="46.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:45" ht="51" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>186</v>
       </c>
       <c r="D2">
         <v>2006</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="K2">
         <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
+      <c r="N2" t="s">
+        <v>176</v>
+      </c>
+      <c r="P2" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>178</v>
+      </c>
       <c r="R2">
         <v>6</v>
       </c>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
+      <c r="S2" s="8">
+        <v>0</v>
+      </c>
+      <c r="T2" s="8">
+        <v>0</v>
+      </c>
+      <c r="U2" s="8">
+        <v>0</v>
+      </c>
+      <c r="V2" s="8">
+        <v>0</v>
+      </c>
+      <c r="W2" s="8">
+        <v>0</v>
+      </c>
+      <c r="X2" s="8">
+        <v>0</v>
+      </c>
       <c r="Y2">
-        <v>5.5</v>
+        <v>5</v>
+      </c>
+      <c r="Z2">
+        <v>59</v>
+      </c>
+      <c r="AA2">
+        <v>6</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>3</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>13</v>
+      </c>
+      <c r="AG2">
+        <v>101.5</v>
+      </c>
+      <c r="AH2">
+        <v>65</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>32</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
       </c>
       <c r="AM2">
-        <v>13</v>
-      </c>
-      <c r="AT2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:52" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="AN2">
+        <v>9</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" ht="65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>185</v>
       </c>
       <c r="D3">
         <v>2006</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="K3">
         <v>24</v>
       </c>
       <c r="L3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="Q3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="R3">
         <v>3</v>
@@ -1544,105 +1712,186 @@
       <c r="AD3">
         <v>7</v>
       </c>
-      <c r="AM3">
+      <c r="AF3">
         <v>4.5</v>
       </c>
-      <c r="AN3">
+      <c r="AG3">
         <v>39</v>
       </c>
-      <c r="AO3">
+      <c r="AH3">
         <v>13</v>
       </c>
-      <c r="AQ3">
-        <v>0</v>
-      </c>
-      <c r="AR3">
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
         <v>9</v>
       </c>
-      <c r="AS3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:52" ht="62" x14ac:dyDescent="0.35">
+      <c r="AL3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" ht="68" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>184</v>
       </c>
       <c r="D4">
         <v>2006</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="K4">
         <v>26</v>
       </c>
       <c r="L4" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="M4">
         <v>1</v>
       </c>
+      <c r="N4" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>180</v>
+      </c>
       <c r="R4">
         <v>9</v>
       </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
       <c r="Y4">
         <v>11</v>
       </c>
+      <c r="Z4">
+        <v>106</v>
+      </c>
+      <c r="AA4">
+        <v>51</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>31</v>
+      </c>
+      <c r="AE4">
+        <v>91</v>
+      </c>
+      <c r="AF4">
+        <v>4.5</v>
+      </c>
+      <c r="AG4">
+        <v>24</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>11</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>46</v>
+      </c>
       <c r="AM4">
-        <v>4.5</v>
-      </c>
-      <c r="AT4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:52" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AN4">
+        <v>2</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>183</v>
       </c>
       <c r="D5">
         <v>2007</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H5" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="K5">
         <v>10</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="M5">
         <v>0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>208</v>
       </c>
       <c r="R5">
         <v>1.25</v>
@@ -1659,64 +1908,181 @@
       <c r="AE5">
         <v>44</v>
       </c>
-      <c r="AM5">
+      <c r="AF5">
         <v>3.25</v>
       </c>
-      <c r="AO5">
+      <c r="AH5">
         <v>14</v>
       </c>
-      <c r="AQ5">
+      <c r="AJ5">
         <v>7</v>
       </c>
-      <c r="AS5">
+      <c r="AL5">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:45" ht="68" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C6" t="s">
+        <v>182</v>
+      </c>
       <c r="D6">
         <v>2007</v>
       </c>
-    </row>
-    <row r="7" spans="1:52" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>187</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" t="s">
+        <v>189</v>
+      </c>
+      <c r="K6">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>180</v>
+      </c>
+      <c r="R6">
+        <v>5</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>10</v>
+      </c>
+      <c r="Z6">
+        <v>110.5</v>
+      </c>
+      <c r="AA6">
+        <v>98.5</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>3</v>
+      </c>
+      <c r="AG6">
+        <v>28</v>
+      </c>
+      <c r="AH6">
+        <v>29</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>7.5</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>3.5</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" ht="153" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>193</v>
       </c>
       <c r="D7">
         <v>2007</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="K7">
         <v>15</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="P7" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="R7">
         <v>5.5</v>
@@ -1730,60 +2096,171 @@
       <c r="AC7">
         <v>13</v>
       </c>
-      <c r="AM7">
+      <c r="AF7">
         <v>2</v>
       </c>
-      <c r="AO7">
+      <c r="AH7">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:45" ht="85" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" t="s">
+        <v>192</v>
+      </c>
       <c r="D8">
         <v>2007</v>
       </c>
-    </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>194</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" t="s">
+        <v>196</v>
+      </c>
+      <c r="K8">
+        <v>18</v>
+      </c>
+      <c r="L8" t="s">
+        <v>70</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0.25</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>3</v>
+      </c>
+      <c r="Z8">
+        <v>43</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>6.25</v>
+      </c>
+      <c r="AF8">
+        <v>12</v>
+      </c>
+      <c r="AG8">
+        <v>68</v>
+      </c>
+      <c r="AH8">
+        <v>30</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>91</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>61.5</v>
+      </c>
+      <c r="AM8">
+        <v>7</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D9">
         <v>2007</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="G9" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="K9">
         <v>13</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="M9">
         <v>2</v>
       </c>
       <c r="N9" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="Q9" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="R9">
         <v>3</v>
@@ -1797,54 +2274,167 @@
       <c r="AA9">
         <v>125</v>
       </c>
-      <c r="AM9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="AF9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C10" t="s">
+        <v>198</v>
+      </c>
       <c r="D10">
         <v>2007</v>
       </c>
-    </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>199</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" t="s">
+        <v>200</v>
+      </c>
+      <c r="K10">
+        <v>14</v>
+      </c>
+      <c r="L10" t="s">
+        <v>161</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>178</v>
+      </c>
+      <c r="R10">
+        <v>3</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>2</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>31</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>8</v>
+      </c>
+      <c r="AF10">
+        <v>9</v>
+      </c>
+      <c r="AG10">
+        <v>33.5</v>
+      </c>
+      <c r="AH10">
+        <v>42</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>44.5</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>14.5</v>
+      </c>
+      <c r="AM10" s="3"/>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>0</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D11">
         <v>2008</v>
       </c>
       <c r="E11" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H11" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="K11">
         <v>13</v>
       </c>
       <c r="L11" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
       <c r="R11">
         <v>4</v>
@@ -1864,60 +2454,174 @@
       <c r="AE11">
         <v>3</v>
       </c>
-      <c r="AM11">
-        <v>0</v>
-      </c>
-      <c r="AT11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" t="s">
+        <v>204</v>
+      </c>
       <c r="D12">
         <v>2008</v>
       </c>
-    </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>205</v>
+      </c>
+      <c r="F12" t="s">
+        <v>206</v>
+      </c>
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" t="s">
+        <v>207</v>
+      </c>
+      <c r="K12">
+        <v>11</v>
+      </c>
+      <c r="L12" t="s">
+        <v>70</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R12">
+        <v>5.5</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>3.5</v>
+      </c>
+      <c r="Z12">
+        <v>5</v>
+      </c>
+      <c r="AA12">
+        <v>14</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>27</v>
+      </c>
+      <c r="AF12">
+        <v>2</v>
+      </c>
+      <c r="AG12">
+        <v>8</v>
+      </c>
+      <c r="AH12">
+        <v>11</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+      <c r="AJ12">
+        <v>0</v>
+      </c>
+      <c r="AK12">
+        <v>0</v>
+      </c>
+      <c r="AL12">
+        <v>25</v>
+      </c>
+      <c r="AM12">
+        <v>0.5</v>
+      </c>
+      <c r="AN12">
+        <v>0</v>
+      </c>
+      <c r="AO12">
+        <v>8</v>
+      </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+      <c r="AQ12">
+        <v>8</v>
+      </c>
+      <c r="AR12">
+        <v>0</v>
+      </c>
+      <c r="AS12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D13">
         <v>2008</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="F13" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="G13" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H13" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="K13">
         <v>36</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="Q13" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="R13">
         <v>7.5</v>
@@ -1943,69 +2647,181 @@
       <c r="AE13">
         <v>4</v>
       </c>
-      <c r="AM13">
+      <c r="AF13">
         <v>9</v>
       </c>
-      <c r="AN13">
+      <c r="AG13">
         <v>11</v>
       </c>
-      <c r="AO13">
+      <c r="AH13">
         <v>71</v>
       </c>
-      <c r="AS13">
+      <c r="AL13">
         <v>14</v>
       </c>
-      <c r="AT13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="AM13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>209</v>
+      </c>
+      <c r="C14" t="s">
+        <v>210</v>
+      </c>
       <c r="D14">
         <v>2008</v>
       </c>
-    </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="E14" t="s">
+        <v>211</v>
+      </c>
+      <c r="F14" t="s">
+        <v>212</v>
+      </c>
+      <c r="G14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" t="s">
+        <v>213</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="L14" t="s">
+        <v>70</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="P14" t="s">
+        <v>214</v>
+      </c>
+      <c r="R14">
+        <v>4</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>13</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>0</v>
+      </c>
+      <c r="AH14">
+        <v>0</v>
+      </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14">
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="3"/>
+      <c r="AN14">
+        <v>0</v>
+      </c>
+      <c r="AO14">
+        <v>0</v>
+      </c>
+      <c r="AP14">
+        <v>0</v>
+      </c>
+      <c r="AQ14">
+        <v>0</v>
+      </c>
+      <c r="AR14">
+        <v>0</v>
+      </c>
+      <c r="AS14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="D15">
         <v>2008</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="F15" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="G15" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H15" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="K15">
         <v>18</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="P15" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="R15">
         <v>3</v>
@@ -2019,63 +2835,177 @@
       <c r="AA15">
         <v>116</v>
       </c>
-      <c r="AM15">
+      <c r="AF15">
         <v>5</v>
       </c>
-      <c r="AO15">
+      <c r="AH15">
         <v>49</v>
       </c>
-      <c r="AT15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="AM15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16" t="s">
+        <v>215</v>
+      </c>
+      <c r="C16" t="s">
+        <v>216</v>
+      </c>
       <c r="D16">
         <v>2009</v>
       </c>
-    </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="E16" t="s">
+        <v>217</v>
+      </c>
+      <c r="F16" t="s">
+        <v>218</v>
+      </c>
+      <c r="G16" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" t="s">
+        <v>219</v>
+      </c>
+      <c r="K16">
+        <v>18</v>
+      </c>
+      <c r="L16" t="s">
+        <v>134</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>221</v>
+      </c>
+      <c r="R16">
+        <v>6</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>5.5</v>
+      </c>
+      <c r="Z16">
+        <v>6</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>27</v>
+      </c>
+      <c r="AD16">
+        <v>4</v>
+      </c>
+      <c r="AE16">
+        <v>37</v>
+      </c>
+      <c r="AF16">
+        <v>5.5</v>
+      </c>
+      <c r="AG16">
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <v>53</v>
+      </c>
+      <c r="AI16">
+        <v>0</v>
+      </c>
+      <c r="AJ16">
+        <v>12</v>
+      </c>
+      <c r="AK16">
+        <v>8</v>
+      </c>
+      <c r="AL16">
+        <v>13</v>
+      </c>
+      <c r="AM16">
+        <v>1</v>
+      </c>
+      <c r="AN16">
+        <v>0</v>
+      </c>
+      <c r="AO16">
+        <v>2</v>
+      </c>
+      <c r="AP16">
+        <v>0</v>
+      </c>
+      <c r="AQ16">
+        <v>0</v>
+      </c>
+      <c r="AR16">
+        <v>0</v>
+      </c>
+      <c r="AS16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D17">
         <v>2009</v>
       </c>
       <c r="E17" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="G17" t="s">
-        <v>74</v>
-      </c>
-      <c r="H17" t="s">
-        <v>118</v>
+        <v>64</v>
       </c>
       <c r="K17">
         <v>17</v>
       </c>
       <c r="L17" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="P17" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="R17">
         <v>6</v>
@@ -2098,14 +3028,14 @@
       <c r="AE17">
         <v>5</v>
       </c>
-      <c r="AM17">
-        <v>0</v>
-      </c>
-      <c r="AT17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2113,45 +3043,45 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="19" spans="1:47" ht="62" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:40" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="C19" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="D19">
         <v>2009</v>
       </c>
       <c r="E19" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="G19" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H19" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="K19">
         <v>45</v>
       </c>
       <c r="L19" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="M19">
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="Q19" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="R19">
         <v>10</v>
@@ -2171,26 +3101,26 @@
       <c r="AC19">
         <v>4</v>
       </c>
+      <c r="AG19">
+        <v>106</v>
+      </c>
+      <c r="AH19">
+        <v>67</v>
+      </c>
+      <c r="AI19">
+        <v>26</v>
+      </c>
+      <c r="AK19">
+        <v>12</v>
+      </c>
+      <c r="AL19">
+        <v>12</v>
+      </c>
       <c r="AN19">
-        <v>106</v>
-      </c>
-      <c r="AO19">
-        <v>67</v>
-      </c>
-      <c r="AP19">
-        <v>26</v>
-      </c>
-      <c r="AR19">
-        <v>12</v>
-      </c>
-      <c r="AS19">
-        <v>12</v>
-      </c>
-      <c r="AU19">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2198,48 +3128,48 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D21">
         <v>2009</v>
       </c>
       <c r="E21" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="F21" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="G21" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H21" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="K21">
         <v>15</v>
       </c>
       <c r="L21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="M21">
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="P21" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="Q21" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="R21">
         <v>5</v>
@@ -2256,20 +3186,20 @@
       <c r="AC21">
         <v>10</v>
       </c>
-      <c r="AM21">
+      <c r="AF21">
         <v>2</v>
       </c>
-      <c r="AN21">
+      <c r="AG21">
         <v>2</v>
       </c>
-      <c r="AO21">
+      <c r="AH21">
         <v>33</v>
       </c>
-      <c r="AT21" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AM21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2277,45 +3207,45 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C23" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="D23">
         <v>2009</v>
       </c>
       <c r="E23" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="F23" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="G23" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H23" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="K23">
         <v>24</v>
       </c>
       <c r="L23" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="M23" s="3">
         <v>2</v>
       </c>
       <c r="N23" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="Q23" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="R23">
         <v>6</v>
@@ -2332,20 +3262,20 @@
       <c r="AC23">
         <v>25</v>
       </c>
-      <c r="AM23">
+      <c r="AF23">
         <v>0.5</v>
       </c>
-      <c r="AN23">
+      <c r="AG23">
         <v>4</v>
       </c>
-      <c r="AO23">
+      <c r="AH23">
         <v>3</v>
       </c>
-      <c r="AT23" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AM23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2353,45 +3283,45 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C25" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D25">
         <v>2010</v>
       </c>
       <c r="E25" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="F25" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="G25" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H25" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="K25">
         <v>16</v>
       </c>
       <c r="L25" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="M25">
         <v>2</v>
       </c>
       <c r="N25" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="Q25" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="R25">
         <v>3</v>
@@ -2408,17 +3338,17 @@
       <c r="AE25">
         <v>14</v>
       </c>
+      <c r="AF25">
+        <v>0.5</v>
+      </c>
+      <c r="AH25">
+        <v>6</v>
+      </c>
       <c r="AM25">
-        <v>0.5</v>
-      </c>
-      <c r="AO25">
-        <v>6</v>
-      </c>
-      <c r="AT25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2426,45 +3356,45 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="C27" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="D27">
         <v>2010</v>
       </c>
       <c r="E27" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="F27" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="G27" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H27" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="K27">
         <v>19</v>
       </c>
       <c r="L27" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="M27">
         <v>2</v>
       </c>
       <c r="N27" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="Q27" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="R27">
         <v>4</v>
@@ -2481,20 +3411,20 @@
       <c r="AC27">
         <v>12</v>
       </c>
+      <c r="AF27">
+        <v>7.5</v>
+      </c>
+      <c r="AG27">
+        <v>24</v>
+      </c>
+      <c r="AH27">
+        <v>129</v>
+      </c>
       <c r="AM27">
-        <v>7.5</v>
-      </c>
-      <c r="AN27">
-        <v>24</v>
-      </c>
-      <c r="AO27">
-        <v>129</v>
-      </c>
-      <c r="AT27">
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2502,42 +3432,42 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C29" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D29">
         <v>2010</v>
       </c>
       <c r="E29" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="F29" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="G29" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H29" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="K29">
         <v>15</v>
       </c>
       <c r="L29" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="M29">
         <v>0</v>
       </c>
       <c r="N29" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="R29">
         <v>4.5</v>
@@ -2557,26 +3487,26 @@
       <c r="AE29">
         <v>52</v>
       </c>
+      <c r="AF29">
+        <v>4.5</v>
+      </c>
+      <c r="AG29">
+        <v>20</v>
+      </c>
+      <c r="AH29">
+        <v>39</v>
+      </c>
+      <c r="AJ29">
+        <v>18</v>
+      </c>
+      <c r="AL29">
+        <v>3</v>
+      </c>
       <c r="AM29">
-        <v>4.5</v>
-      </c>
-      <c r="AN29">
-        <v>20</v>
-      </c>
-      <c r="AO29">
-        <v>39</v>
-      </c>
-      <c r="AQ29">
-        <v>18</v>
-      </c>
-      <c r="AS29">
-        <v>3</v>
-      </c>
-      <c r="AT29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2584,43 +3514,43 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="31" spans="1:47" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:40" ht="85" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C31" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="D31">
         <v>2011</v>
       </c>
       <c r="E31" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="K31">
         <v>25</v>
       </c>
       <c r="L31" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="M31">
         <v>1</v>
       </c>
       <c r="N31" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="Q31" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="R31">
         <v>8</v>
@@ -2646,23 +3576,23 @@
       <c r="AE31">
         <v>67</v>
       </c>
+      <c r="AF31">
+        <v>5</v>
+      </c>
+      <c r="AH31">
+        <v>47</v>
+      </c>
+      <c r="AJ31">
+        <v>3</v>
+      </c>
+      <c r="AL31">
+        <v>51</v>
+      </c>
       <c r="AM31">
-        <v>5</v>
-      </c>
-      <c r="AO31">
-        <v>47</v>
-      </c>
-      <c r="AQ31">
-        <v>3</v>
-      </c>
-      <c r="AS31">
-        <v>51</v>
-      </c>
-      <c r="AT31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2670,45 +3600,45 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C33" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="D33">
         <v>2011</v>
       </c>
       <c r="E33" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="F33" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="G33" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H33" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="K33">
         <v>16</v>
       </c>
       <c r="L33" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="M33">
         <v>2</v>
       </c>
       <c r="N33" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="Q33" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="R33">
         <v>4</v>
@@ -2719,14 +3649,14 @@
       <c r="AA33">
         <v>181</v>
       </c>
-      <c r="AN33">
+      <c r="AG33">
         <v>56</v>
       </c>
-      <c r="AZ33">
+      <c r="AS33">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2734,42 +3664,42 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="35" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="C35" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="D35">
         <v>2011</v>
       </c>
       <c r="E35" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="F35" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="G35" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H35" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="K35">
         <v>18</v>
       </c>
       <c r="L35" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="M35">
         <v>0</v>
       </c>
       <c r="N35" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="R35">
         <v>2.5</v>
@@ -2786,58 +3716,58 @@
       <c r="AC35">
         <v>8</v>
       </c>
+      <c r="AF35">
+        <v>4.5</v>
+      </c>
+      <c r="AH35">
+        <v>81</v>
+      </c>
+      <c r="AI35">
+        <v>20</v>
+      </c>
       <c r="AM35">
-        <v>4.5</v>
-      </c>
-      <c r="AO35">
-        <v>81</v>
-      </c>
-      <c r="AP35">
-        <v>20</v>
-      </c>
-      <c r="AT35">
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="C36" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="D36">
         <v>2012</v>
       </c>
       <c r="E36" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="F36" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="G36" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H36" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="K36">
         <v>33</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="M36">
         <v>1</v>
       </c>
       <c r="N36" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="Q36" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="R36">
         <v>11</v>
@@ -2857,29 +3787,29 @@
       <c r="AB36">
         <v>19</v>
       </c>
+      <c r="AF36">
+        <v>10</v>
+      </c>
+      <c r="AG36">
+        <v>12</v>
+      </c>
+      <c r="AH36">
+        <v>200</v>
+      </c>
+      <c r="AL36">
+        <v>20</v>
+      </c>
       <c r="AM36">
-        <v>10</v>
-      </c>
-      <c r="AN36">
-        <v>12</v>
-      </c>
-      <c r="AO36">
-        <v>200</v>
-      </c>
-      <c r="AS36">
-        <v>20</v>
-      </c>
-      <c r="AT36">
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="L37" s="7"/>
     </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2887,7 +3817,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2895,7 +3825,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2903,7 +3833,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2911,7 +3841,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2919,7 +3849,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2927,7 +3857,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2935,7 +3865,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="45" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2943,7 +3873,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2951,7 +3881,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="47" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2959,7 +3889,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2967,7 +3897,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2975,7 +3905,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2983,7 +3913,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2991,7 +3921,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2999,7 +3929,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3007,7 +3937,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3015,7 +3945,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3023,7 +3953,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3031,7 +3961,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3039,7 +3969,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3047,7 +3977,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3055,7 +3985,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3063,7 +3993,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3071,7 +4001,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3079,7 +4009,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3087,7 +4017,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3095,7 +4025,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3103,7 +4033,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3111,7 +4041,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3119,7 +4049,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3127,7 +4057,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3135,7 +4065,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3143,7 +4073,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3151,7 +4081,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3159,7 +4089,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3167,7 +4097,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3175,7 +4105,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3183,7 +4113,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3191,7 +4121,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3199,7 +4129,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3207,7 +4137,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
Evens through 2013 and added missing 0's
</commit_message>
<xml_diff>
--- a/AlitoDataset.xlsx
+++ b/AlitoDataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineparnell/alito-research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jtsanz\alito-research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBDFAD1-890E-D04C-8A62-59BDADF54E08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7955A2DF-27DB-4C29-BAFE-D4E69FE40113}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,6 +52,7 @@
     <author>tc={3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}</author>
     <author>tc={93985E51-4186-401D-B292-10D9DC17CEB8}</author>
     <author>tc={916A852D-1D9C-43FD-9526-91B03FAC048E}</author>
+    <author>tc={191E2626-B001-4B9D-95BB-3DFE681133E5}</author>
     <author>tc={A4DC1BA9-4A23-4C06-A9DF-A3D4F083B19B}</author>
   </authors>
   <commentList>
@@ -193,7 +194,15 @@
     Not sure what to put as the answer here: "Pharmaceutical sales reps are outside salesmen"</t>
       </text>
     </comment>
-    <comment ref="A36" authorId="17" shapeId="0" xr:uid="{A4DC1BA9-4A23-4C06-A9DF-A3D4F083B19B}">
+    <comment ref="Y33" authorId="17" shapeId="0" xr:uid="{191E2626-B001-4B9D-95BB-3DFE681133E5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Howes v Fields, no MA length given</t>
+      </text>
+    </comment>
+    <comment ref="A36" authorId="18" shapeId="0" xr:uid="{A4DC1BA9-4A23-4C06-A9DF-A3D4F083B19B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -206,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="261">
   <si>
     <t>Case Name</t>
   </si>
@@ -663,9 +672,6 @@
     <t>“Inmates have one year to file a habeas challenge to their sentence in federal court after conviction. The running of that time is delayed while the conviction is under review in state court. Is the time also tolled while a state court considers an inmate's request for a sentence reduction?"</t>
   </si>
   <si>
-    <t>pragmatism and precendent</t>
-  </si>
-  <si>
     <t>Alito;Scalia,Breyer,Sotomayor,Kagan,Roberts,Kennedy,Thomas,Ginsburg</t>
   </si>
   <si>
@@ -725,9 +731,6 @@
     <t>Are government officials who initiate prosecutions by providing false testimony in judicial proceedings absolutely immune from civil suit?</t>
   </si>
   <si>
-    <t>precendent</t>
-  </si>
-  <si>
     <t>Alito;Scalia,Roberts,Kennedy,Thomas,Ginsburg,Breyer,Sotomaor,Kagan</t>
   </si>
   <si>
@@ -885,6 +888,129 @@
   </si>
   <si>
     <t>Scalia</t>
+  </si>
+  <si>
+    <t>Adoptive Couple v. Baby Girl</t>
+  </si>
+  <si>
+    <t>570 U.S. 637 (2013)</t>
+  </si>
+  <si>
+    <t>ICWA, §1912(f) and §1912(d)</t>
+  </si>
+  <si>
+    <t>Can a non-custodial parent invoke ICWA to block an adoption voluntarily and lawfully initiated by a non-Indian parent under state law?|Does ICWA define "parent" to include an unwed biological father who has not complied with state law rules to attain legal status as a parent?</t>
+  </si>
+  <si>
+    <t>incorrect interpretation of the language of the statute</t>
+  </si>
+  <si>
+    <t>Alito;Thomas,Breyer,Kennedy,Roberts</t>
+  </si>
+  <si>
+    <t>Kagan;Sotomayor,Ginsburg,Scalia</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Stevens,Scalia,Kennedy,Souter,Thomas,Ginsberg,Breyer,Thomas</t>
+  </si>
+  <si>
+    <t>Johnson v. Wlliams</t>
+  </si>
+  <si>
+    <t>568 U.S. 289 (2013)</t>
+  </si>
+  <si>
+    <t>Sixth Amendment jury trial claim, 28 U.S.C. § 2254</t>
+  </si>
+  <si>
+    <t>Is a habeas petitioner’s claim “adjudicated on the merits” if the state court denied relief in an explained decision but did not expressly acknowledge the federal-law basis for the claim?</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Kennedy,Thomas,Ginsburg,Breyer,Sotomayor,Kagan</t>
+  </si>
+  <si>
+    <t>0/5</t>
+  </si>
+  <si>
+    <t>Salinas v. Texas</t>
+  </si>
+  <si>
+    <t>570 U.S. 178 (2013)</t>
+  </si>
+  <si>
+    <t>Self-Incrimination Clause, Fifth Amendment</t>
+  </si>
+  <si>
+    <t>Does the Fifth Amendment’s Self-Incrimination Clause protect a defendant’s refusal to answer questions asked by law enforcement before he has been arrested or read his Miranda rights?</t>
+  </si>
+  <si>
+    <t>doctrinal and pragmatic</t>
+  </si>
+  <si>
+    <t>Breyer;Ginsburg,Sotomayor,Kagan</t>
+  </si>
+  <si>
+    <t>Atlantic Marine Construction Co., Inc v. US Dist. Ct for the Western Dist of TX</t>
+  </si>
+  <si>
+    <t>571 U.S. 49 (2013)</t>
+  </si>
+  <si>
+    <t>28 U.S.C. § 1404(a)</t>
+  </si>
+  <si>
+    <t>Did the Supreme Court&amp;#39;s decision in Stewart Organization, Inc. v. Ricoh Corp. limit review of forum selection clauses to a discretionary, balancing-of-conveniences analysis under 28 U.S.C. § 1404(a) | If so, who has the burden of proof when a party seeks to enforce or avoid a forum selection clause?</t>
+  </si>
+  <si>
+    <t>precedent</t>
+  </si>
+  <si>
+    <t>pragmatism and precedent</t>
+  </si>
+  <si>
+    <t>Burwell v. Hobby Lobby Stores</t>
+  </si>
+  <si>
+    <t>573 U.S. 682 (2014)</t>
+  </si>
+  <si>
+    <t>Religious Freedom Restoration Act of 1993</t>
+  </si>
+  <si>
+    <t>Does the Religious Freedom Restoration Act of 1993 allow a for-profit company to deny its employees health coverage of contraception to which the employees would otherwise be entitled based on the religious objections of the company's owners?</t>
+  </si>
+  <si>
+    <t>purposive-ism and pragmatism</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Kennedy,Scalia,Thomas</t>
+  </si>
+  <si>
+    <t>Ginsburg;Breyer,Sotomayor,Kagan</t>
+  </si>
+  <si>
+    <t>Limelight v. Akamai</t>
+  </si>
+  <si>
+    <t>574 U.S. 915 (2014)</t>
+  </si>
+  <si>
+    <t>35 U.S.C. § 271(a) and § 271(b), federal laws prohibiting patent infringement</t>
+  </si>
+  <si>
+    <t>“Did the Federal Circuit court err in holding that a defendant may be liable for inducing patent infringement under § 271(b) even if no party committed direct infringement under §271(a)?”</t>
+  </si>
+  <si>
+    <t>Plumhoff v. Rickard</t>
+  </si>
+  <si>
+    <t>572 U.S. 765 (2014)</t>
+  </si>
+  <si>
+    <t>Qualified immunity for police officers</t>
+  </si>
+  <si>
+    <t>Did the Sixth Circuit err when it looked at whether subsequent case law supported the police's actions rather than determining if the police's actions were prohibited in 2004?|Did the Sixth Circuit properly dismiss the police's qualified immunity defense by finding that the police acted unreasonably?”</t>
   </si>
 </sst>
 </file>
@@ -907,10 +1033,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="9"/>
+      <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1326,6 +1452,9 @@
   <threadedComment ref="G31" dT="2020-07-17T02:59:12.36" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{916A852D-1D9C-43FD-9526-91B03FAC048E}">
     <text>Not sure what to put as the answer here: "Pharmaceutical sales reps are outside salesmen"</text>
   </threadedComment>
+  <threadedComment ref="Y33" dT="2020-07-18T08:13:23.37" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{191E2626-B001-4B9D-95BB-3DFE681133E5}">
+    <text>Howes v Fields, no MA length given</text>
+  </threadedComment>
   <threadedComment ref="A36" dT="2020-07-17T03:38:46.55" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{A4DC1BA9-4A23-4C06-A9DF-A3D4F083B19B}">
     <text>accidentally got out of order, my b haha</text>
   </threadedComment>
@@ -1336,11 +1465,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060A011E-60FD-5047-91C8-6B9B09AABF05}">
   <dimension ref="A1:AS79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S5" workbookViewId="0">
-      <selection activeCell="AT16" sqref="AT16"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
@@ -1389,7 +1518,7 @@
     <col min="45" max="45" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1526,7 +1655,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1534,7 +1663,7 @@
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D2">
         <v>2006</v>
@@ -1561,13 +1690,13 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
+        <v>174</v>
+      </c>
+      <c r="P2" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q2" t="s">
         <v>176</v>
-      </c>
-      <c r="P2" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>178</v>
       </c>
       <c r="R2">
         <v>6</v>
@@ -1654,7 +1783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:45" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" ht="65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1662,7 +1791,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D3">
         <v>2006</v>
@@ -1697,6 +1826,24 @@
       <c r="R3">
         <v>3</v>
       </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
       <c r="Y3">
         <v>15</v>
       </c>
@@ -1706,12 +1853,18 @@
       <c r="AA3">
         <v>52</v>
       </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
       <c r="AC3">
         <v>37</v>
       </c>
       <c r="AD3">
         <v>7</v>
       </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
       <c r="AF3">
         <v>4.5</v>
       </c>
@@ -1721,6 +1874,9 @@
       <c r="AH3">
         <v>13</v>
       </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
       <c r="AJ3">
         <v>0</v>
       </c>
@@ -1730,8 +1886,29 @@
       <c r="AL3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:45" ht="68" x14ac:dyDescent="0.2">
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" ht="62" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1739,7 +1916,7 @@
         <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D4">
         <v>2006</v>
@@ -1766,10 +1943,10 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="Q4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="R4">
         <v>9</v>
@@ -1856,7 +2033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:45" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" ht="37" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1864,7 +2041,7 @@
         <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D5">
         <v>2007</v>
@@ -1891,60 +2068,117 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="R5">
         <v>1.25</v>
       </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
       <c r="Y5">
         <v>2.5</v>
       </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
       <c r="AA5">
         <v>14</v>
       </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
       <c r="AC5">
         <v>6</v>
       </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
       <c r="AE5">
         <v>44</v>
       </c>
       <c r="AF5">
         <v>3.25</v>
       </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
       <c r="AH5">
         <v>14</v>
       </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
       <c r="AJ5">
         <v>7</v>
       </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
       <c r="AL5">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:45" ht="68" x14ac:dyDescent="0.2">
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" ht="62" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D6">
         <v>2007</v>
       </c>
       <c r="E6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G6" t="s">
         <v>64</v>
       </c>
       <c r="H6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K6">
         <v>18</v>
@@ -1956,10 +2190,10 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="Q6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="R6">
         <v>5</v>
@@ -2046,7 +2280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:45" ht="153" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:45" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2054,7 +2288,7 @@
         <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D7">
         <v>2007</v>
@@ -2087,46 +2321,112 @@
       <c r="R7">
         <v>5.5</v>
       </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
       <c r="Y7">
         <v>7</v>
       </c>
       <c r="Z7">
         <v>90</v>
       </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
       <c r="AC7">
         <v>13</v>
       </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
       <c r="AF7">
         <v>2</v>
       </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
       <c r="AH7">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:45" ht="85" x14ac:dyDescent="0.2">
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D8">
         <v>2007</v>
       </c>
       <c r="E8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G8" t="s">
         <v>64</v>
       </c>
       <c r="H8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K8">
         <v>18</v>
@@ -2137,6 +2437,9 @@
       <c r="M8">
         <v>0</v>
       </c>
+      <c r="N8" t="s">
+        <v>227</v>
+      </c>
       <c r="R8">
         <v>0.25</v>
       </c>
@@ -2222,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2265,6 +2568,24 @@
       <c r="R9">
         <v>3</v>
       </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
       <c r="Y9">
         <v>10</v>
       </c>
@@ -2274,47 +2595,95 @@
       <c r="AA9">
         <v>125</v>
       </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
       <c r="AF9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D10">
         <v>2007</v>
       </c>
       <c r="E10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" t="s">
         <v>64</v>
       </c>
       <c r="H10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K10">
         <v>14</v>
       </c>
       <c r="L10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M10">
         <v>2</v>
       </c>
       <c r="N10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="Q10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="R10">
         <v>3</v>
@@ -2399,7 +2768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2434,17 +2803,41 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="R11">
         <v>4</v>
       </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
       <c r="Y11">
         <v>8.5</v>
       </c>
       <c r="Z11">
         <v>52</v>
       </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
       <c r="AC11">
         <v>108</v>
       </c>
@@ -2457,34 +2850,70 @@
       <c r="AF11">
         <v>0</v>
       </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
       <c r="AM11" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>0</v>
+      </c>
+      <c r="AP11">
+        <v>0</v>
+      </c>
+      <c r="AQ11">
+        <v>0</v>
+      </c>
+      <c r="AR11">
+        <v>0</v>
+      </c>
+      <c r="AS11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D12">
         <v>2008</v>
       </c>
       <c r="E12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G12" t="s">
         <v>44</v>
       </c>
       <c r="H12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K12">
         <v>11</v>
@@ -2496,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="R12">
         <v>5.5</v>
@@ -2583,7 +3012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2626,9 +3055,24 @@
       <c r="R13">
         <v>7.5</v>
       </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
       <c r="V13">
         <v>6</v>
       </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
       <c r="Y13">
         <v>19</v>
       </c>
@@ -2638,6 +3082,9 @@
       <c r="AA13">
         <v>231</v>
       </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
       <c r="AC13">
         <v>60</v>
       </c>
@@ -2656,37 +3103,64 @@
       <c r="AH13">
         <v>71</v>
       </c>
+      <c r="AI13">
+        <v>0</v>
+      </c>
+      <c r="AJ13">
+        <v>0</v>
+      </c>
+      <c r="AK13">
+        <v>0</v>
+      </c>
       <c r="AL13">
         <v>14</v>
       </c>
       <c r="AM13" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AN13">
+        <v>0</v>
+      </c>
+      <c r="AO13">
+        <v>0</v>
+      </c>
+      <c r="AP13">
+        <v>0</v>
+      </c>
+      <c r="AQ13">
+        <v>0</v>
+      </c>
+      <c r="AR13">
+        <v>0</v>
+      </c>
+      <c r="AS13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D14">
         <v>2008</v>
       </c>
       <c r="E14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G14" t="s">
         <v>64</v>
       </c>
       <c r="H14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K14">
         <v>5</v>
@@ -2695,10 +3169,10 @@
         <v>70</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="P14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="R14">
         <v>4</v>
@@ -2783,7 +3257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2826,6 +3300,24 @@
       <c r="R15">
         <v>3</v>
       </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
       <c r="Y15">
         <v>10</v>
       </c>
@@ -2835,40 +3327,85 @@
       <c r="AA15">
         <v>116</v>
       </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
       <c r="AF15">
         <v>5</v>
       </c>
+      <c r="AG15">
+        <v>0</v>
+      </c>
       <c r="AH15">
         <v>49</v>
       </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+      <c r="AJ15">
+        <v>0</v>
+      </c>
+      <c r="AK15">
+        <v>0</v>
+      </c>
+      <c r="AL15">
+        <v>0</v>
+      </c>
       <c r="AM15" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AN15">
+        <v>0</v>
+      </c>
+      <c r="AO15">
+        <v>0</v>
+      </c>
+      <c r="AP15">
+        <v>0</v>
+      </c>
+      <c r="AQ15">
+        <v>0</v>
+      </c>
+      <c r="AR15">
+        <v>0</v>
+      </c>
+      <c r="AS15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D16">
         <v>2009</v>
       </c>
       <c r="E16" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G16" t="s">
         <v>64</v>
       </c>
       <c r="H16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K16">
         <v>18</v>
@@ -2880,10 +3417,10 @@
         <v>2</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="Q16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R16">
         <v>6</v>
@@ -2970,7 +3507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3010,6 +3547,24 @@
       <c r="R17">
         <v>6</v>
       </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
       <c r="Y17">
         <v>11</v>
       </c>
@@ -3019,6 +3574,9 @@
       <c r="AA17">
         <v>56</v>
       </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
       <c r="AC17">
         <v>26</v>
       </c>
@@ -3031,11 +3589,47 @@
       <c r="AF17">
         <v>0</v>
       </c>
+      <c r="AG17">
+        <v>0</v>
+      </c>
+      <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
+        <v>0</v>
+      </c>
+      <c r="AJ17">
+        <v>0</v>
+      </c>
+      <c r="AK17">
+        <v>0</v>
+      </c>
+      <c r="AL17">
+        <v>0</v>
+      </c>
       <c r="AM17" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AN17">
+        <v>0</v>
+      </c>
+      <c r="AO17">
+        <v>0</v>
+      </c>
+      <c r="AP17">
+        <v>0</v>
+      </c>
+      <c r="AQ17">
+        <v>0</v>
+      </c>
+      <c r="AR17">
+        <v>0</v>
+      </c>
+      <c r="AS17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3043,7 +3637,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="19" spans="1:40" ht="68" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:45" ht="62" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3089,6 +3683,24 @@
       <c r="S19">
         <v>25</v>
       </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
       <c r="Z19">
         <v>24</v>
       </c>
@@ -3101,6 +3713,15 @@
       <c r="AC19">
         <v>4</v>
       </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
       <c r="AG19">
         <v>106</v>
       </c>
@@ -3110,17 +3731,38 @@
       <c r="AI19">
         <v>26</v>
       </c>
+      <c r="AJ19">
+        <v>0</v>
+      </c>
       <c r="AK19">
         <v>12</v>
       </c>
       <c r="AL19">
         <v>12</v>
       </c>
+      <c r="AM19">
+        <v>0</v>
+      </c>
       <c r="AN19">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO19">
+        <v>0</v>
+      </c>
+      <c r="AP19">
+        <v>0</v>
+      </c>
+      <c r="AQ19">
+        <v>0</v>
+      </c>
+      <c r="AR19">
+        <v>0</v>
+      </c>
+      <c r="AS19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3128,7 +3770,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3174,6 +3816,24 @@
       <c r="R21">
         <v>5</v>
       </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
       <c r="Y21">
         <v>8</v>
       </c>
@@ -3183,9 +3843,18 @@
       <c r="AA21">
         <v>67</v>
       </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
       <c r="AC21">
         <v>10</v>
       </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
       <c r="AF21">
         <v>2</v>
       </c>
@@ -3195,11 +3864,41 @@
       <c r="AH21">
         <v>33</v>
       </c>
+      <c r="AI21">
+        <v>0</v>
+      </c>
+      <c r="AJ21">
+        <v>0</v>
+      </c>
+      <c r="AK21">
+        <v>0</v>
+      </c>
+      <c r="AL21">
+        <v>0</v>
+      </c>
       <c r="AM21" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AN21">
+        <v>0</v>
+      </c>
+      <c r="AO21">
+        <v>0</v>
+      </c>
+      <c r="AP21">
+        <v>0</v>
+      </c>
+      <c r="AQ21">
+        <v>0</v>
+      </c>
+      <c r="AR21">
+        <v>0</v>
+      </c>
+      <c r="AS21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3207,7 +3906,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3250,6 +3949,24 @@
       <c r="R23">
         <v>6</v>
       </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
       <c r="Y23">
         <v>12</v>
       </c>
@@ -3259,9 +3976,18 @@
       <c r="AA23">
         <v>93</v>
       </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
       <c r="AC23">
         <v>25</v>
       </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
       <c r="AF23">
         <v>0.5</v>
       </c>
@@ -3271,11 +3997,41 @@
       <c r="AH23">
         <v>3</v>
       </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
+        <v>0</v>
+      </c>
+      <c r="AK23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
       <c r="AM23" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AN23">
+        <v>0</v>
+      </c>
+      <c r="AO23">
+        <v>0</v>
+      </c>
+      <c r="AP23">
+        <v>0</v>
+      </c>
+      <c r="AQ23">
+        <v>0</v>
+      </c>
+      <c r="AR23">
+        <v>0</v>
+      </c>
+      <c r="AS23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3283,7 +4039,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3326,6 +4082,24 @@
       <c r="R25">
         <v>3</v>
       </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
       <c r="Y25">
         <v>11.5</v>
       </c>
@@ -3335,20 +4109,62 @@
       <c r="AA25">
         <v>37</v>
       </c>
+      <c r="AB25">
+        <v>0</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
       <c r="AE25">
         <v>14</v>
       </c>
       <c r="AF25">
         <v>0.5</v>
       </c>
+      <c r="AG25">
+        <v>0</v>
+      </c>
       <c r="AH25">
         <v>6</v>
       </c>
+      <c r="AI25">
+        <v>0</v>
+      </c>
+      <c r="AJ25">
+        <v>0</v>
+      </c>
+      <c r="AK25">
+        <v>0</v>
+      </c>
+      <c r="AL25">
+        <v>0</v>
+      </c>
       <c r="AM25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AN25">
+        <v>0</v>
+      </c>
+      <c r="AO25">
+        <v>0</v>
+      </c>
+      <c r="AP25">
+        <v>0</v>
+      </c>
+      <c r="AQ25">
+        <v>0</v>
+      </c>
+      <c r="AR25">
+        <v>0</v>
+      </c>
+      <c r="AS25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3356,7 +4172,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3399,6 +4215,24 @@
       <c r="R27">
         <v>4</v>
       </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
       <c r="Y27">
         <v>7</v>
       </c>
@@ -3408,9 +4242,18 @@
       <c r="AA27">
         <v>41</v>
       </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
       <c r="AC27">
         <v>12</v>
       </c>
+      <c r="AD27">
+        <v>0</v>
+      </c>
+      <c r="AE27">
+        <v>0</v>
+      </c>
       <c r="AF27">
         <v>7.5</v>
       </c>
@@ -3420,11 +4263,41 @@
       <c r="AH27">
         <v>129</v>
       </c>
+      <c r="AI27">
+        <v>0</v>
+      </c>
+      <c r="AJ27">
+        <v>0</v>
+      </c>
+      <c r="AK27">
+        <v>0</v>
+      </c>
+      <c r="AL27">
+        <v>0</v>
+      </c>
       <c r="AM27">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AN27">
+        <v>0</v>
+      </c>
+      <c r="AO27">
+        <v>0</v>
+      </c>
+      <c r="AP27">
+        <v>0</v>
+      </c>
+      <c r="AQ27">
+        <v>0</v>
+      </c>
+      <c r="AR27">
+        <v>0</v>
+      </c>
+      <c r="AS27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3432,7 +4305,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3455,7 +4328,7 @@
         <v>64</v>
       </c>
       <c r="H29" t="s">
-        <v>148</v>
+        <v>245</v>
       </c>
       <c r="K29">
         <v>15</v>
@@ -3467,11 +4340,29 @@
         <v>0</v>
       </c>
       <c r="N29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="R29">
         <v>4.5</v>
       </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
       <c r="Y29">
         <v>6</v>
       </c>
@@ -3481,9 +4372,15 @@
       <c r="AA29">
         <v>22</v>
       </c>
+      <c r="AB29">
+        <v>0</v>
+      </c>
       <c r="AC29">
         <v>6</v>
       </c>
+      <c r="AD29">
+        <v>0</v>
+      </c>
       <c r="AE29">
         <v>52</v>
       </c>
@@ -3496,17 +4393,41 @@
       <c r="AH29">
         <v>39</v>
       </c>
+      <c r="AI29">
+        <v>0</v>
+      </c>
       <c r="AJ29">
         <v>18</v>
       </c>
+      <c r="AK29">
+        <v>0</v>
+      </c>
       <c r="AL29">
         <v>3</v>
       </c>
       <c r="AM29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AN29">
+        <v>0</v>
+      </c>
+      <c r="AO29">
+        <v>0</v>
+      </c>
+      <c r="AP29">
+        <v>0</v>
+      </c>
+      <c r="AQ29">
+        <v>0</v>
+      </c>
+      <c r="AR29">
+        <v>0</v>
+      </c>
+      <c r="AS29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3514,28 +4435,28 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="31" spans="1:40" ht="85" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:45" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>149</v>
+      </c>
+      <c r="C31" t="s">
         <v>150</v>
-      </c>
-      <c r="C31" t="s">
-        <v>151</v>
       </c>
       <c r="D31">
         <v>2011</v>
       </c>
       <c r="E31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K31">
         <v>25</v>
@@ -3550,14 +4471,29 @@
         <v>113</v>
       </c>
       <c r="Q31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R31">
         <v>8</v>
       </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
       <c r="V31">
         <v>3</v>
       </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
       <c r="Y31">
         <v>13</v>
       </c>
@@ -3567,6 +4503,9 @@
       <c r="AA31">
         <v>86</v>
       </c>
+      <c r="AB31">
+        <v>0</v>
+      </c>
       <c r="AC31">
         <v>19</v>
       </c>
@@ -3579,20 +4518,47 @@
       <c r="AF31">
         <v>5</v>
       </c>
+      <c r="AG31">
+        <v>0</v>
+      </c>
       <c r="AH31">
         <v>47</v>
       </c>
+      <c r="AI31">
+        <v>0</v>
+      </c>
       <c r="AJ31">
         <v>3</v>
       </c>
+      <c r="AK31">
+        <v>0</v>
+      </c>
       <c r="AL31">
         <v>51</v>
       </c>
       <c r="AM31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AN31">
+        <v>0</v>
+      </c>
+      <c r="AO31">
+        <v>0</v>
+      </c>
+      <c r="AP31">
+        <v>0</v>
+      </c>
+      <c r="AQ31">
+        <v>0</v>
+      </c>
+      <c r="AR31">
+        <v>0</v>
+      </c>
+      <c r="AS31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3600,63 +4566,130 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" t="s">
         <v>155</v>
-      </c>
-      <c r="C33" t="s">
-        <v>156</v>
       </c>
       <c r="D33">
         <v>2011</v>
       </c>
       <c r="E33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G33" t="s">
         <v>44</v>
       </c>
       <c r="H33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K33">
         <v>16</v>
       </c>
       <c r="L33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M33">
         <v>2</v>
       </c>
       <c r="N33" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q33" t="s">
         <v>162</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>163</v>
       </c>
       <c r="R33">
         <v>4</v>
       </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="3"/>
       <c r="Z33">
         <v>63</v>
       </c>
       <c r="AA33">
         <v>181</v>
       </c>
+      <c r="AB33">
+        <v>0</v>
+      </c>
+      <c r="AC33">
+        <v>0</v>
+      </c>
+      <c r="AD33">
+        <v>0</v>
+      </c>
+      <c r="AE33">
+        <v>0</v>
+      </c>
+      <c r="AF33">
+        <v>0</v>
+      </c>
       <c r="AG33">
         <v>56</v>
       </c>
+      <c r="AH33">
+        <v>0</v>
+      </c>
+      <c r="AI33">
+        <v>0</v>
+      </c>
+      <c r="AJ33">
+        <v>0</v>
+      </c>
+      <c r="AK33">
+        <v>0</v>
+      </c>
+      <c r="AL33">
+        <v>0</v>
+      </c>
+      <c r="AM33">
+        <v>0</v>
+      </c>
+      <c r="AN33">
+        <v>0</v>
+      </c>
+      <c r="AO33">
+        <v>0</v>
+      </c>
+      <c r="AP33">
+        <v>0</v>
+      </c>
+      <c r="AQ33">
+        <v>0</v>
+      </c>
+      <c r="AR33">
+        <v>0</v>
+      </c>
       <c r="AS33">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3664,30 +4697,30 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" t="s">
         <v>164</v>
-      </c>
-      <c r="C35" t="s">
-        <v>165</v>
       </c>
       <c r="D35">
         <v>2011</v>
       </c>
       <c r="E35" t="s">
+        <v>165</v>
+      </c>
+      <c r="F35" t="s">
         <v>166</v>
-      </c>
-      <c r="F35" t="s">
-        <v>167</v>
       </c>
       <c r="G35" t="s">
         <v>64</v>
       </c>
       <c r="H35" t="s">
-        <v>168</v>
+        <v>244</v>
       </c>
       <c r="K35">
         <v>18</v>
@@ -3699,11 +4732,29 @@
         <v>0</v>
       </c>
       <c r="N35" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="R35">
         <v>2.5</v>
       </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <v>0</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
       <c r="Y35">
         <v>9.5</v>
       </c>
@@ -3713,46 +4764,85 @@
       <c r="AA35">
         <v>58</v>
       </c>
+      <c r="AB35">
+        <v>0</v>
+      </c>
       <c r="AC35">
         <v>8</v>
       </c>
+      <c r="AD35">
+        <v>0</v>
+      </c>
+      <c r="AE35">
+        <v>0</v>
+      </c>
       <c r="AF35">
         <v>4.5</v>
       </c>
+      <c r="AG35">
+        <v>0</v>
+      </c>
       <c r="AH35">
         <v>81</v>
       </c>
       <c r="AI35">
         <v>20</v>
       </c>
+      <c r="AJ35">
+        <v>0</v>
+      </c>
+      <c r="AK35">
+        <v>0</v>
+      </c>
+      <c r="AL35">
+        <v>0</v>
+      </c>
       <c r="AM35">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AN35">
+        <v>0</v>
+      </c>
+      <c r="AO35">
+        <v>0</v>
+      </c>
+      <c r="AP35">
+        <v>0</v>
+      </c>
+      <c r="AQ35">
+        <v>0</v>
+      </c>
+      <c r="AR35">
+        <v>0</v>
+      </c>
+      <c r="AS35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>168</v>
+      </c>
+      <c r="C36" t="s">
+        <v>169</v>
+      </c>
+      <c r="D36">
+        <v>2011</v>
+      </c>
+      <c r="E36" t="s">
         <v>170</v>
       </c>
-      <c r="C36" t="s">
+      <c r="F36" t="s">
         <v>171</v>
-      </c>
-      <c r="D36">
-        <v>2012</v>
-      </c>
-      <c r="E36" t="s">
-        <v>172</v>
-      </c>
-      <c r="F36" t="s">
-        <v>173</v>
       </c>
       <c r="G36" t="s">
         <v>64</v>
       </c>
       <c r="H36" t="s">
-        <v>168</v>
+        <v>244</v>
       </c>
       <c r="K36">
         <v>33</v>
@@ -3764,10 +4854,10 @@
         <v>1</v>
       </c>
       <c r="N36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="Q36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="R36">
         <v>11</v>
@@ -3775,6 +4865,21 @@
       <c r="S36">
         <v>74</v>
       </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <v>0</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
       <c r="Y36">
         <v>11.5</v>
       </c>
@@ -3787,6 +4892,15 @@
       <c r="AB36">
         <v>19</v>
       </c>
+      <c r="AC36">
+        <v>0</v>
+      </c>
+      <c r="AD36">
+        <v>0</v>
+      </c>
+      <c r="AE36">
+        <v>0</v>
+      </c>
       <c r="AF36">
         <v>10</v>
       </c>
@@ -3796,20 +4910,166 @@
       <c r="AH36">
         <v>200</v>
       </c>
+      <c r="AI36">
+        <v>0</v>
+      </c>
+      <c r="AJ36">
+        <v>0</v>
+      </c>
+      <c r="AK36">
+        <v>0</v>
+      </c>
       <c r="AL36">
         <v>20</v>
       </c>
       <c r="AM36">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AN36">
+        <v>0</v>
+      </c>
+      <c r="AO36">
+        <v>0</v>
+      </c>
+      <c r="AP36">
+        <v>0</v>
+      </c>
+      <c r="AQ36">
+        <v>0</v>
+      </c>
+      <c r="AR36">
+        <v>0</v>
+      </c>
+      <c r="AS36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="L37" s="7"/>
-    </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>220</v>
+      </c>
+      <c r="C37" t="s">
+        <v>221</v>
+      </c>
+      <c r="D37">
+        <v>2012</v>
+      </c>
+      <c r="E37" t="s">
+        <v>222</v>
+      </c>
+      <c r="F37" t="s">
+        <v>223</v>
+      </c>
+      <c r="G37" t="s">
+        <v>44</v>
+      </c>
+      <c r="H37" t="s">
+        <v>224</v>
+      </c>
+      <c r="K37">
+        <v>17</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>226</v>
+      </c>
+      <c r="R37">
+        <v>2</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>0</v>
+      </c>
+      <c r="X37">
+        <v>0</v>
+      </c>
+      <c r="Y37">
+        <v>9</v>
+      </c>
+      <c r="Z37">
+        <v>0</v>
+      </c>
+      <c r="AA37">
+        <v>18</v>
+      </c>
+      <c r="AB37">
+        <v>0</v>
+      </c>
+      <c r="AC37">
+        <v>4</v>
+      </c>
+      <c r="AD37">
+        <v>43</v>
+      </c>
+      <c r="AE37">
+        <v>63</v>
+      </c>
+      <c r="AF37">
+        <v>6</v>
+      </c>
+      <c r="AG37">
+        <v>0</v>
+      </c>
+      <c r="AH37">
+        <v>14</v>
+      </c>
+      <c r="AI37">
+        <v>0</v>
+      </c>
+      <c r="AJ37">
+        <v>40</v>
+      </c>
+      <c r="AK37">
+        <v>0</v>
+      </c>
+      <c r="AL37">
+        <v>28</v>
+      </c>
+      <c r="AM37">
+        <v>0</v>
+      </c>
+      <c r="AN37">
+        <v>0</v>
+      </c>
+      <c r="AO37">
+        <v>0</v>
+      </c>
+      <c r="AP37">
+        <v>0</v>
+      </c>
+      <c r="AQ37">
+        <v>0</v>
+      </c>
+      <c r="AR37">
+        <v>0</v>
+      </c>
+      <c r="AS37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3817,15 +5077,132 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
+      <c r="B39" t="s">
+        <v>228</v>
+      </c>
+      <c r="C39" t="s">
+        <v>229</v>
+      </c>
       <c r="D39">
         <v>2012</v>
       </c>
-    </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
+        <v>230</v>
+      </c>
+      <c r="F39" t="s">
+        <v>231</v>
+      </c>
+      <c r="G39" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" t="s">
+        <v>211</v>
+      </c>
+      <c r="K39">
+        <v>16</v>
+      </c>
+      <c r="L39" t="s">
+        <v>70</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39" t="s">
+        <v>232</v>
+      </c>
+      <c r="P39" t="s">
+        <v>219</v>
+      </c>
+      <c r="R39">
+        <v>6.5</v>
+      </c>
+      <c r="S39">
+        <v>0</v>
+      </c>
+      <c r="T39">
+        <v>0</v>
+      </c>
+      <c r="U39">
+        <v>0</v>
+      </c>
+      <c r="V39">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>0</v>
+      </c>
+      <c r="X39">
+        <v>0</v>
+      </c>
+      <c r="Y39">
+        <v>3</v>
+      </c>
+      <c r="Z39">
+        <v>14</v>
+      </c>
+      <c r="AA39">
+        <v>43</v>
+      </c>
+      <c r="AB39">
+        <v>0</v>
+      </c>
+      <c r="AC39">
+        <v>0</v>
+      </c>
+      <c r="AD39">
+        <v>0</v>
+      </c>
+      <c r="AE39">
+        <v>0</v>
+      </c>
+      <c r="AF39">
+        <v>6</v>
+      </c>
+      <c r="AG39">
+        <v>0</v>
+      </c>
+      <c r="AH39">
+        <v>68</v>
+      </c>
+      <c r="AI39">
+        <v>0</v>
+      </c>
+      <c r="AJ39">
+        <v>7</v>
+      </c>
+      <c r="AK39">
+        <v>0</v>
+      </c>
+      <c r="AL39">
+        <v>27</v>
+      </c>
+      <c r="AM39" t="s">
+        <v>233</v>
+      </c>
+      <c r="AN39">
+        <v>0</v>
+      </c>
+      <c r="AO39">
+        <v>0</v>
+      </c>
+      <c r="AP39">
+        <v>0</v>
+      </c>
+      <c r="AQ39">
+        <v>0</v>
+      </c>
+      <c r="AR39">
+        <v>0</v>
+      </c>
+      <c r="AS39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3833,15 +5210,135 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
+      <c r="B41" t="s">
+        <v>234</v>
+      </c>
+      <c r="C41" t="s">
+        <v>235</v>
+      </c>
       <c r="D41">
         <v>2012</v>
       </c>
-    </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>236</v>
+      </c>
+      <c r="F41" t="s">
+        <v>237</v>
+      </c>
+      <c r="G41" t="s">
+        <v>44</v>
+      </c>
+      <c r="H41" t="s">
+        <v>238</v>
+      </c>
+      <c r="K41">
+        <v>12</v>
+      </c>
+      <c r="L41" t="s">
+        <v>48</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41" t="s">
+        <v>174</v>
+      </c>
+      <c r="P41" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>239</v>
+      </c>
+      <c r="R41">
+        <v>3</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="T41">
+        <v>3</v>
+      </c>
+      <c r="U41">
+        <v>0</v>
+      </c>
+      <c r="V41">
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <v>0</v>
+      </c>
+      <c r="X41">
+        <v>0</v>
+      </c>
+      <c r="Y41">
+        <v>2.5</v>
+      </c>
+      <c r="Z41">
+        <v>40</v>
+      </c>
+      <c r="AA41">
+        <v>23</v>
+      </c>
+      <c r="AB41">
+        <v>0</v>
+      </c>
+      <c r="AC41">
+        <v>7</v>
+      </c>
+      <c r="AD41">
+        <v>0</v>
+      </c>
+      <c r="AE41">
+        <v>0</v>
+      </c>
+      <c r="AF41">
+        <v>5.5</v>
+      </c>
+      <c r="AG41">
+        <v>33</v>
+      </c>
+      <c r="AH41">
+        <v>66</v>
+      </c>
+      <c r="AI41">
+        <v>0</v>
+      </c>
+      <c r="AJ41">
+        <v>0</v>
+      </c>
+      <c r="AK41">
+        <v>0</v>
+      </c>
+      <c r="AL41">
+        <v>4</v>
+      </c>
+      <c r="AM41" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN41">
+        <v>0</v>
+      </c>
+      <c r="AO41">
+        <v>0</v>
+      </c>
+      <c r="AP41">
+        <v>0</v>
+      </c>
+      <c r="AQ41">
+        <v>0</v>
+      </c>
+      <c r="AR41">
+        <v>0</v>
+      </c>
+      <c r="AS41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3849,15 +5346,129 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
+      <c r="B43" t="s">
+        <v>240</v>
+      </c>
+      <c r="C43" t="s">
+        <v>241</v>
+      </c>
       <c r="D43">
         <v>2013</v>
       </c>
-    </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="E43" t="s">
+        <v>242</v>
+      </c>
+      <c r="F43" t="s">
+        <v>243</v>
+      </c>
+      <c r="G43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H43" t="s">
+        <v>133</v>
+      </c>
+      <c r="K43">
+        <v>18</v>
+      </c>
+      <c r="L43" t="s">
+        <v>70</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43" t="s">
+        <v>148</v>
+      </c>
+      <c r="R43">
+        <v>3</v>
+      </c>
+      <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="T43">
+        <v>0</v>
+      </c>
+      <c r="U43">
+        <v>0</v>
+      </c>
+      <c r="V43">
+        <v>0</v>
+      </c>
+      <c r="W43">
+        <v>0</v>
+      </c>
+      <c r="X43">
+        <v>0</v>
+      </c>
+      <c r="Y43">
+        <v>11</v>
+      </c>
+      <c r="Z43">
+        <v>73</v>
+      </c>
+      <c r="AA43">
+        <v>91</v>
+      </c>
+      <c r="AB43">
+        <v>0</v>
+      </c>
+      <c r="AC43">
+        <v>0</v>
+      </c>
+      <c r="AD43">
+        <v>29</v>
+      </c>
+      <c r="AE43">
+        <v>70</v>
+      </c>
+      <c r="AF43">
+        <v>4</v>
+      </c>
+      <c r="AG43">
+        <v>24</v>
+      </c>
+      <c r="AH43">
+        <v>55</v>
+      </c>
+      <c r="AI43">
+        <v>0</v>
+      </c>
+      <c r="AJ43">
+        <v>17</v>
+      </c>
+      <c r="AK43">
+        <v>3</v>
+      </c>
+      <c r="AL43">
+        <v>7</v>
+      </c>
+      <c r="AM43">
+        <v>0</v>
+      </c>
+      <c r="AN43">
+        <v>0</v>
+      </c>
+      <c r="AO43">
+        <v>0</v>
+      </c>
+      <c r="AP43">
+        <v>0</v>
+      </c>
+      <c r="AQ43">
+        <v>0</v>
+      </c>
+      <c r="AR43">
+        <v>0</v>
+      </c>
+      <c r="AS43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3865,15 +5476,132 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
+      <c r="B45" t="s">
+        <v>246</v>
+      </c>
+      <c r="C45" t="s">
+        <v>247</v>
+      </c>
       <c r="D45">
         <v>2013</v>
       </c>
-    </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="E45" t="s">
+        <v>248</v>
+      </c>
+      <c r="F45" t="s">
+        <v>249</v>
+      </c>
+      <c r="G45" t="s">
+        <v>64</v>
+      </c>
+      <c r="H45" t="s">
+        <v>250</v>
+      </c>
+      <c r="K45">
+        <v>49</v>
+      </c>
+      <c r="L45" t="s">
+        <v>48</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>252</v>
+      </c>
+      <c r="R45">
+        <v>15.5</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="T45">
+        <v>2</v>
+      </c>
+      <c r="U45">
+        <v>0</v>
+      </c>
+      <c r="V45">
+        <v>0</v>
+      </c>
+      <c r="W45">
+        <v>0</v>
+      </c>
+      <c r="X45">
+        <v>0</v>
+      </c>
+      <c r="Y45">
+        <v>5.5</v>
+      </c>
+      <c r="Z45">
+        <v>0</v>
+      </c>
+      <c r="AA45">
+        <v>44</v>
+      </c>
+      <c r="AB45">
+        <v>0</v>
+      </c>
+      <c r="AC45">
+        <v>0</v>
+      </c>
+      <c r="AD45">
+        <v>0</v>
+      </c>
+      <c r="AE45">
+        <v>43</v>
+      </c>
+      <c r="AF45">
+        <v>29</v>
+      </c>
+      <c r="AG45">
+        <v>116</v>
+      </c>
+      <c r="AH45">
+        <v>242</v>
+      </c>
+      <c r="AI45">
+        <v>0</v>
+      </c>
+      <c r="AJ45">
+        <v>75</v>
+      </c>
+      <c r="AK45">
+        <v>11</v>
+      </c>
+      <c r="AL45">
+        <v>46</v>
+      </c>
+      <c r="AM45">
+        <v>0</v>
+      </c>
+      <c r="AN45">
+        <v>0</v>
+      </c>
+      <c r="AO45">
+        <v>0</v>
+      </c>
+      <c r="AP45">
+        <v>0</v>
+      </c>
+      <c r="AQ45">
+        <v>0</v>
+      </c>
+      <c r="AR45">
+        <v>0</v>
+      </c>
+      <c r="AS45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3881,15 +5609,129 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
+      <c r="B47" t="s">
+        <v>253</v>
+      </c>
+      <c r="C47" t="s">
+        <v>254</v>
+      </c>
       <c r="D47">
         <v>2013</v>
       </c>
-    </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>255</v>
+      </c>
+      <c r="F47" t="s">
+        <v>256</v>
+      </c>
+      <c r="G47" t="s">
+        <v>64</v>
+      </c>
+      <c r="H47" t="s">
+        <v>133</v>
+      </c>
+      <c r="K47">
+        <v>11</v>
+      </c>
+      <c r="L47" t="s">
+        <v>70</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47" t="s">
+        <v>148</v>
+      </c>
+      <c r="R47">
+        <v>4</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47">
+        <v>0</v>
+      </c>
+      <c r="U47">
+        <v>0</v>
+      </c>
+      <c r="V47">
+        <v>0</v>
+      </c>
+      <c r="W47">
+        <v>0</v>
+      </c>
+      <c r="X47">
+        <v>0</v>
+      </c>
+      <c r="Y47">
+        <v>4</v>
+      </c>
+      <c r="Z47">
+        <v>39</v>
+      </c>
+      <c r="AA47">
+        <v>0</v>
+      </c>
+      <c r="AB47">
+        <v>0</v>
+      </c>
+      <c r="AC47">
+        <v>8</v>
+      </c>
+      <c r="AD47">
+        <v>18</v>
+      </c>
+      <c r="AE47">
+        <v>0</v>
+      </c>
+      <c r="AF47">
+        <v>3</v>
+      </c>
+      <c r="AG47">
+        <v>23</v>
+      </c>
+      <c r="AH47">
+        <v>31</v>
+      </c>
+      <c r="AI47">
+        <v>0</v>
+      </c>
+      <c r="AJ47">
+        <v>0</v>
+      </c>
+      <c r="AK47">
+        <v>3</v>
+      </c>
+      <c r="AL47">
+        <v>3</v>
+      </c>
+      <c r="AM47">
+        <v>0</v>
+      </c>
+      <c r="AN47">
+        <v>0</v>
+      </c>
+      <c r="AO47">
+        <v>0</v>
+      </c>
+      <c r="AP47">
+        <v>0</v>
+      </c>
+      <c r="AQ47">
+        <v>0</v>
+      </c>
+      <c r="AR47">
+        <v>0</v>
+      </c>
+      <c r="AS47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3897,15 +5739,129 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
+      <c r="B49" t="s">
+        <v>257</v>
+      </c>
+      <c r="C49" t="s">
+        <v>258</v>
+      </c>
       <c r="D49">
         <v>2013</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>259</v>
+      </c>
+      <c r="F49" t="s">
+        <v>260</v>
+      </c>
+      <c r="G49" t="s">
+        <v>64</v>
+      </c>
+      <c r="H49" t="s">
+        <v>244</v>
+      </c>
+      <c r="K49">
+        <v>15</v>
+      </c>
+      <c r="L49" t="s">
+        <v>70</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49" t="s">
+        <v>148</v>
+      </c>
+      <c r="R49">
+        <v>4</v>
+      </c>
+      <c r="S49">
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <v>0</v>
+      </c>
+      <c r="U49">
+        <v>0</v>
+      </c>
+      <c r="V49">
+        <v>0</v>
+      </c>
+      <c r="W49">
+        <v>0</v>
+      </c>
+      <c r="X49">
+        <v>0</v>
+      </c>
+      <c r="Y49">
+        <v>7.5</v>
+      </c>
+      <c r="Z49">
+        <v>162</v>
+      </c>
+      <c r="AA49">
+        <v>57</v>
+      </c>
+      <c r="AB49">
+        <v>0</v>
+      </c>
+      <c r="AC49">
+        <v>0</v>
+      </c>
+      <c r="AD49">
+        <v>0</v>
+      </c>
+      <c r="AE49">
+        <v>0</v>
+      </c>
+      <c r="AF49">
+        <v>3</v>
+      </c>
+      <c r="AG49">
+        <v>49</v>
+      </c>
+      <c r="AH49">
+        <v>32</v>
+      </c>
+      <c r="AI49">
+        <v>0</v>
+      </c>
+      <c r="AJ49">
+        <v>0</v>
+      </c>
+      <c r="AK49">
+        <v>0</v>
+      </c>
+      <c r="AL49">
+        <v>0</v>
+      </c>
+      <c r="AM49">
+        <v>0.5</v>
+      </c>
+      <c r="AN49">
+        <v>0</v>
+      </c>
+      <c r="AO49">
+        <v>0</v>
+      </c>
+      <c r="AP49">
+        <v>0</v>
+      </c>
+      <c r="AQ49">
+        <v>0</v>
+      </c>
+      <c r="AR49">
+        <v>0</v>
+      </c>
+      <c r="AS49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3913,7 +5869,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3921,7 +5877,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3929,7 +5885,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3937,7 +5893,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3945,7 +5901,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3953,7 +5909,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3961,7 +5917,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3969,7 +5925,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3977,7 +5933,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3985,7 +5941,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3993,7 +5949,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4001,7 +5957,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4009,7 +5965,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4017,7 +5973,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4025,7 +5981,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4033,7 +5989,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4041,7 +5997,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4049,7 +6005,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4057,7 +6013,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4065,7 +6021,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4073,7 +6029,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4081,7 +6037,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4089,7 +6045,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4097,7 +6053,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4105,7 +6061,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4113,7 +6069,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4121,7 +6077,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4129,7 +6085,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4137,7 +6093,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
up to 50 done
</commit_message>
<xml_diff>
--- a/AlitoDataset.xlsx
+++ b/AlitoDataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jtsanz\alito-research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineparnell/alito-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB24666-8010-4409-91E1-4954AF2DA6E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685E5E44-453C-6240-BAF7-B7D97D2F786F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -206,7 +206,7 @@
     it's 5-3, is this contentious or ambigious? haha</t>
       </text>
     </comment>
-    <comment ref="G31" authorId="17" shapeId="0" xr:uid="{916A852D-1D9C-43FD-9526-91B03FAC048E}">
+    <comment ref="G30" authorId="17" shapeId="0" xr:uid="{916A852D-1D9C-43FD-9526-91B03FAC048E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -214,7 +214,7 @@
     Not sure what to put as the answer here: "Pharmaceutical sales reps are outside salesmen"</t>
       </text>
     </comment>
-    <comment ref="Y33" authorId="18" shapeId="0" xr:uid="{191E2626-B001-4B9D-95BB-3DFE681133E5}">
+    <comment ref="Y32" authorId="18" shapeId="0" xr:uid="{191E2626-B001-4B9D-95BB-3DFE681133E5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -325,7 +325,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="444">
   <si>
     <t>Case Name</t>
   </si>
@@ -1536,12 +1536,147 @@
   <si>
     <t>pragmatism and textualism</t>
   </si>
+  <si>
+    <t>Does union contract violate first and fourteenth amendments</t>
+  </si>
+  <si>
+    <t>May a state consistent with the first and fourteenth amendments, condition employment on the payment of a special union assessment intended solely for political and ideological expenditures without first providing a notice that includes information about that assessment and provides an opportunity to object to its exaction and condition public employment on the payment of union agency fees for the purposes of financing political expenditures for ballot measures?</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>Alito,Thomas,Scalia,Kennedy,Roberts,Sotomayor,Ginsburg</t>
+  </si>
+  <si>
+    <t>Kagan,Breyer</t>
+  </si>
+  <si>
+    <t>Taniguchi v. Kan Pacific</t>
+  </si>
+  <si>
+    <t>566 U.S. 560 (2012)</t>
+  </si>
+  <si>
+    <t>U.S.C. Section § 1920(6)</t>
+  </si>
+  <si>
+    <t>Are costs incurred in translating documents "compensation of interpreters" under U.S.C. Section § 1920(6)?</t>
+  </si>
+  <si>
+    <t>literal meaning of statute</t>
+  </si>
+  <si>
+    <t>Alito,Scalia,Roberts,Kennedy,Thomas,Kagan</t>
+  </si>
+  <si>
+    <t>Ginsburg,Breyer,Sotomayor</t>
+  </si>
+  <si>
+    <t>Clapper v. Amnest International</t>
+  </si>
+  <si>
+    <t>568 US 398 (2013)</t>
+  </si>
+  <si>
+    <t>Article III of the constitution</t>
+  </si>
+  <si>
+    <t>Do respondents have article III standing to seek prospective relief under FISA?</t>
+  </si>
+  <si>
+    <t>Mutual Pharmaceutical Co. v. Bartlett</t>
+  </si>
+  <si>
+    <t>570 US 472 (2013)</t>
+  </si>
+  <si>
+    <t>The federal food, drug, and cosmetic act</t>
+  </si>
+  <si>
+    <t>Does federal law preempt a state design defect claim against a generic drug manufacturer?</t>
+  </si>
+  <si>
+    <t>practical considerations and precedent</t>
+  </si>
+  <si>
+    <t>Ginsburg,Breyer,Sotomayor,Kagan</t>
+  </si>
+  <si>
+    <t>Alito,Scalia,Roberts,Kennedy,Thomas</t>
+  </si>
+  <si>
+    <t>Vance v. Ball State</t>
+  </si>
+  <si>
+    <t>570 US 421 (2013)</t>
+  </si>
+  <si>
+    <t>workplace harassment under title VII</t>
+  </si>
+  <si>
+    <t>can a coworker who is vested with the authority to oversee the daily work of another worker be considered a supervisor for the purpose of determining employer liability for workplace harassment?</t>
+  </si>
+  <si>
+    <t>Roberts,Scalia,Kennedy,Alito</t>
+  </si>
+  <si>
+    <t>Kagan,Sotomayor,Ginsburg,Breyer</t>
+  </si>
+  <si>
+    <t>Burt v. Titlow</t>
+  </si>
+  <si>
+    <t>571 U.S. 12 (2013)</t>
+  </si>
+  <si>
+    <t>antiterrorism and effective death penalty act</t>
+  </si>
+  <si>
+    <t>did the sixth circuit give appropriate deference to the michigan trial court under the AEDPA? Can a defendant establish prejudice in an ineffective assisstance claim by presenting subjective testimony that he would have accepted the plea offer absent the attorney's deficient advice? does the court's decision in Lafler v. Cooper require a state trial court to resentence a defendant when he claims that ineffective assistance of ocnsel led him to reject a plea offer?</t>
+  </si>
+  <si>
+    <t>Alito,Scalia,Breyer,Ginsburg,Sotomayor,Kagan,Roberts,Kennedy,Thomas</t>
+  </si>
+  <si>
+    <t>Harris v. Quinn</t>
+  </si>
+  <si>
+    <t>573 US 616 (2014)</t>
+  </si>
+  <si>
+    <t>first amendment, fair share provision for union fees (part of overturning Abood sequence)</t>
+  </si>
+  <si>
+    <t>does the fair share provision in the collective bargaining agreement between the state of Illinois and the union representative violate the first amendment rights to freedom of speech and freedom of association of personal assistants who are not members of the union?</t>
+  </si>
+  <si>
+    <t>Yes | Unanswered</t>
+  </si>
+  <si>
+    <t>Alito,Roberts,Kennedy,Scalia,Thomas</t>
+  </si>
+  <si>
+    <t>Northwest v. Ginsberg</t>
+  </si>
+  <si>
+    <t>572 U.S. 273 (2014)</t>
+  </si>
+  <si>
+    <t>airline deregulation act of 1978</t>
+  </si>
+  <si>
+    <t>are claims arising from a frequent flyer program contract preempted by the airline deregulation act as dealing with the price, route, or service of an air carrier?</t>
+  </si>
+  <si>
+    <t>pragmatism</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1555,12 +1690,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1976,10 +2105,10 @@
   <threadedComment ref="M23" dT="2020-07-05T08:11:32.10" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{93985E51-4186-401D-B292-10D9DC17CEB8}">
     <text>it's 5-3, is this contentious or ambigious? haha</text>
   </threadedComment>
-  <threadedComment ref="G31" dT="2020-07-17T02:59:12.36" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{916A852D-1D9C-43FD-9526-91B03FAC048E}">
+  <threadedComment ref="G30" dT="2020-07-17T02:59:12.36" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{916A852D-1D9C-43FD-9526-91B03FAC048E}">
     <text>Not sure what to put as the answer here: "Pharmaceutical sales reps are outside salesmen"</text>
   </threadedComment>
-  <threadedComment ref="Y33" dT="2020-07-18T08:13:23.37" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{191E2626-B001-4B9D-95BB-3DFE681133E5}">
+  <threadedComment ref="Y32" dT="2020-07-18T08:13:23.37" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{191E2626-B001-4B9D-95BB-3DFE681133E5}">
     <text>Howes v Fields, no MA length given</text>
   </threadedComment>
   <threadedComment ref="A36" dT="2020-07-17T03:38:46.55" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{A4DC1BA9-4A23-4C06-A9DF-A3D4F083B19B}">
@@ -2028,11 +2157,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060A011E-60FD-5047-91C8-6B9B09AABF05}">
   <dimension ref="A1:AS78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
@@ -2081,7 +2210,7 @@
     <col min="45" max="45" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -2218,7 +2347,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:45" ht="51" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2346,7 +2475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:45" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:45" ht="65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2471,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:45" ht="62" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:45" ht="68" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2596,7 +2725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:45" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:45" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2718,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:45" ht="62" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:45" ht="68" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2843,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:45" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:45" ht="153" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2966,7 +3095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:45" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:45" ht="85" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3088,7 +3217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3210,7 +3339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3333,7 +3462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3455,7 +3584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3577,7 +3706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3702,7 +3831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3824,7 +3953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3949,7 +4078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4074,7 +4203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4196,7 +4325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4315,7 +4444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:45" ht="62" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:45" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -4438,7 +4567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4563,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4691,7 +4820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4816,7 +4945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4941,7 +5070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5066,7 +5195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5191,7 +5320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5307,7 +5436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5432,7 +5561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5557,7 +5686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5679,54 +5808,171 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:45" ht="85" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30" t="s">
+        <v>150</v>
+      </c>
       <c r="D30">
         <v>2011</v>
       </c>
+      <c r="E30" t="s">
+        <v>151</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G30" s="3"/>
+      <c r="H30" t="s">
+        <v>152</v>
+      </c>
+      <c r="K30">
+        <v>25</v>
+      </c>
+      <c r="L30" t="s">
+        <v>48</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>153</v>
+      </c>
+      <c r="R30">
+        <v>8</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>3</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>13</v>
+      </c>
+      <c r="Z30">
+        <v>24</v>
+      </c>
+      <c r="AA30">
+        <v>86</v>
+      </c>
+      <c r="AB30">
+        <v>0</v>
+      </c>
+      <c r="AC30">
+        <v>19</v>
+      </c>
+      <c r="AD30">
+        <v>11</v>
+      </c>
+      <c r="AE30">
+        <v>67</v>
+      </c>
+      <c r="AF30">
+        <v>5</v>
+      </c>
+      <c r="AG30">
+        <v>0</v>
+      </c>
+      <c r="AH30">
+        <v>47</v>
+      </c>
+      <c r="AI30">
+        <v>0</v>
+      </c>
+      <c r="AJ30">
+        <v>3</v>
+      </c>
+      <c r="AK30">
+        <v>0</v>
+      </c>
+      <c r="AL30">
+        <v>51</v>
+      </c>
+      <c r="AM30">
+        <v>0</v>
+      </c>
+      <c r="AN30">
+        <v>0</v>
+      </c>
+      <c r="AO30">
+        <v>0</v>
+      </c>
+      <c r="AP30">
+        <v>0</v>
+      </c>
+      <c r="AQ30">
+        <v>0</v>
+      </c>
+      <c r="AR30">
+        <v>0</v>
+      </c>
+      <c r="AS30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:45" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>149</v>
+        <v>301</v>
       </c>
       <c r="C31" t="s">
-        <v>150</v>
+        <v>302</v>
       </c>
       <c r="D31">
         <v>2011</v>
       </c>
       <c r="E31" t="s">
-        <v>151</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G31" s="3"/>
+        <v>303</v>
+      </c>
+      <c r="F31" t="s">
+        <v>304</v>
+      </c>
+      <c r="G31" t="s">
+        <v>305</v>
+      </c>
       <c r="H31" t="s">
-        <v>152</v>
+        <v>306</v>
       </c>
       <c r="K31">
         <v>25</v>
       </c>
       <c r="L31" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="M31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N31" t="s">
-        <v>113</v>
+        <v>307</v>
       </c>
       <c r="Q31" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="R31">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="S31">
         <v>0</v>
@@ -5738,34 +5984,34 @@
         <v>0</v>
       </c>
       <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <v>14</v>
+      </c>
+      <c r="Z31">
+        <v>22</v>
+      </c>
+      <c r="AA31">
         <v>3</v>
       </c>
-      <c r="W31">
-        <v>0</v>
-      </c>
-      <c r="X31">
-        <v>0</v>
-      </c>
-      <c r="Y31">
-        <v>13</v>
-      </c>
-      <c r="Z31">
-        <v>24</v>
-      </c>
-      <c r="AA31">
-        <v>86</v>
-      </c>
       <c r="AB31">
         <v>0</v>
       </c>
       <c r="AC31">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="AD31">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="AE31">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AF31">
         <v>5</v>
@@ -5774,22 +6020,22 @@
         <v>0</v>
       </c>
       <c r="AH31">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="AI31">
         <v>0</v>
       </c>
       <c r="AJ31">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="AK31">
         <v>0</v>
       </c>
       <c r="AL31">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="AM31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN31">
         <v>0</v>
@@ -5807,51 +6053,51 @@
         <v>0</v>
       </c>
       <c r="AS31">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>301</v>
+        <v>154</v>
       </c>
       <c r="C32" t="s">
-        <v>302</v>
+        <v>155</v>
       </c>
       <c r="D32">
         <v>2011</v>
       </c>
       <c r="E32" t="s">
-        <v>303</v>
+        <v>156</v>
       </c>
       <c r="F32" t="s">
-        <v>304</v>
+        <v>158</v>
       </c>
       <c r="G32" t="s">
-        <v>305</v>
+        <v>44</v>
       </c>
       <c r="H32" t="s">
-        <v>306</v>
+        <v>159</v>
       </c>
       <c r="K32">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="L32" t="s">
-        <v>127</v>
+        <v>160</v>
       </c>
       <c r="M32">
         <v>2</v>
       </c>
       <c r="N32" t="s">
-        <v>307</v>
+        <v>161</v>
       </c>
       <c r="Q32" t="s">
         <v>162</v>
       </c>
       <c r="R32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S32">
         <v>0</v>
@@ -5871,50 +6117,48 @@
       <c r="X32">
         <v>0</v>
       </c>
-      <c r="Y32">
-        <v>14</v>
-      </c>
+      <c r="Y32" s="3"/>
       <c r="Z32">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="AA32">
-        <v>3</v>
+        <v>181</v>
       </c>
       <c r="AB32">
         <v>0</v>
       </c>
       <c r="AC32">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AD32">
         <v>0</v>
       </c>
       <c r="AE32">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="AF32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AG32">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="AH32">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AI32">
         <v>0</v>
       </c>
       <c r="AJ32">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="AK32">
         <v>0</v>
       </c>
       <c r="AL32">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="AM32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN32">
         <v>0</v>
@@ -5935,48 +6179,48 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>154</v>
+        <v>308</v>
       </c>
       <c r="C33" t="s">
-        <v>155</v>
+        <v>309</v>
       </c>
       <c r="D33">
         <v>2011</v>
       </c>
       <c r="E33" t="s">
-        <v>156</v>
+        <v>399</v>
       </c>
       <c r="F33" t="s">
-        <v>158</v>
+        <v>400</v>
       </c>
       <c r="G33" t="s">
         <v>44</v>
       </c>
       <c r="H33" t="s">
-        <v>159</v>
+        <v>401</v>
       </c>
       <c r="K33">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="L33" t="s">
-        <v>160</v>
+        <v>78</v>
       </c>
       <c r="M33">
         <v>2</v>
       </c>
       <c r="N33" t="s">
-        <v>161</v>
+        <v>402</v>
       </c>
       <c r="Q33" t="s">
-        <v>162</v>
+        <v>403</v>
       </c>
       <c r="R33">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S33">
         <v>0</v>
@@ -5996,18 +6240,17 @@
       <c r="X33">
         <v>0</v>
       </c>
-      <c r="Y33" s="3"/>
       <c r="Z33">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="AA33">
-        <v>181</v>
+        <v>124</v>
       </c>
       <c r="AB33">
         <v>0</v>
       </c>
       <c r="AC33">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="AD33">
         <v>0</v>
@@ -6015,20 +6258,17 @@
       <c r="AE33">
         <v>0</v>
       </c>
-      <c r="AF33">
-        <v>0</v>
-      </c>
       <c r="AG33">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="AH33">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="AI33">
         <v>0</v>
       </c>
       <c r="AJ33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK33">
         <v>0</v>
@@ -6037,7 +6277,7 @@
         <v>0</v>
       </c>
       <c r="AM33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN33">
         <v>0</v>
@@ -6049,68 +6289,179 @@
         <v>0</v>
       </c>
       <c r="AQ33">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AR33">
         <v>0</v>
       </c>
       <c r="AS33">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>308</v>
+        <v>163</v>
       </c>
       <c r="C34" t="s">
-        <v>309</v>
+        <v>164</v>
       </c>
       <c r="D34">
         <v>2011</v>
       </c>
+      <c r="E34" t="s">
+        <v>165</v>
+      </c>
+      <c r="F34" t="s">
+        <v>166</v>
+      </c>
+      <c r="G34" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" t="s">
+        <v>243</v>
+      </c>
+      <c r="K34">
+        <v>18</v>
+      </c>
+      <c r="L34" t="s">
+        <v>70</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34" t="s">
+        <v>167</v>
+      </c>
+      <c r="R34">
+        <v>2.5</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <v>9.5</v>
+      </c>
+      <c r="Z34">
+        <v>111</v>
+      </c>
+      <c r="AA34">
+        <v>58</v>
+      </c>
+      <c r="AB34">
+        <v>0</v>
+      </c>
+      <c r="AC34">
+        <v>8</v>
+      </c>
+      <c r="AD34">
+        <v>0</v>
+      </c>
+      <c r="AE34">
+        <v>0</v>
+      </c>
+      <c r="AF34">
+        <v>4.5</v>
+      </c>
+      <c r="AG34">
+        <v>0</v>
+      </c>
+      <c r="AH34">
+        <v>81</v>
+      </c>
+      <c r="AI34">
+        <v>20</v>
+      </c>
+      <c r="AJ34">
+        <v>0</v>
+      </c>
+      <c r="AK34">
+        <v>0</v>
+      </c>
+      <c r="AL34">
+        <v>0</v>
+      </c>
+      <c r="AM34">
+        <v>0.5</v>
+      </c>
+      <c r="AN34">
+        <v>0</v>
+      </c>
+      <c r="AO34">
+        <v>0</v>
+      </c>
+      <c r="AP34">
+        <v>0</v>
+      </c>
+      <c r="AQ34">
+        <v>0</v>
+      </c>
+      <c r="AR34">
+        <v>0</v>
+      </c>
+      <c r="AS34">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>163</v>
+        <v>404</v>
       </c>
       <c r="C35" t="s">
-        <v>164</v>
+        <v>405</v>
       </c>
       <c r="D35">
         <v>2011</v>
       </c>
       <c r="E35" t="s">
-        <v>165</v>
+        <v>406</v>
       </c>
       <c r="F35" t="s">
-        <v>166</v>
+        <v>407</v>
       </c>
       <c r="G35" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="H35" t="s">
-        <v>243</v>
+        <v>408</v>
       </c>
       <c r="K35">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L35" t="s">
-        <v>70</v>
+        <v>160</v>
       </c>
       <c r="M35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N35" t="s">
-        <v>167</v>
+        <v>409</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>410</v>
       </c>
       <c r="R35">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="S35">
         <v>0</v>
@@ -6131,46 +6482,46 @@
         <v>0</v>
       </c>
       <c r="Y35">
-        <v>9.5</v>
+        <v>6.5</v>
       </c>
       <c r="Z35">
-        <v>111</v>
+        <v>5</v>
       </c>
       <c r="AA35">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="AB35">
         <v>0</v>
       </c>
       <c r="AC35">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AD35">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="AE35">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="AF35">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="AG35">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AH35">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="AI35">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AJ35">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AK35">
         <v>0</v>
       </c>
       <c r="AL35">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="AM35">
         <v>0.5</v>
@@ -6191,10 +6542,10 @@
         <v>0</v>
       </c>
       <c r="AS35">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -6319,7 +6670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6444,15 +6795,132 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
+      <c r="B38" t="s">
+        <v>411</v>
+      </c>
+      <c r="C38" t="s">
+        <v>412</v>
+      </c>
       <c r="D38">
         <v>2012</v>
       </c>
+      <c r="E38" t="s">
+        <v>413</v>
+      </c>
+      <c r="F38" t="s">
+        <v>414</v>
+      </c>
+      <c r="G38" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" t="s">
+        <v>321</v>
+      </c>
+      <c r="K38">
+        <v>24</v>
+      </c>
+      <c r="L38" t="s">
+        <v>48</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>238</v>
+      </c>
+      <c r="R38">
+        <v>8</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>0</v>
+      </c>
+      <c r="X38">
+        <v>0</v>
+      </c>
+      <c r="Y38">
+        <v>7</v>
+      </c>
+      <c r="Z38">
+        <v>46</v>
+      </c>
+      <c r="AA38">
+        <v>100</v>
+      </c>
+      <c r="AB38">
+        <v>0</v>
+      </c>
+      <c r="AC38">
+        <v>16</v>
+      </c>
+      <c r="AD38">
+        <v>0</v>
+      </c>
+      <c r="AE38">
+        <v>0</v>
+      </c>
+      <c r="AF38">
+        <v>8</v>
+      </c>
+      <c r="AG38">
+        <v>92</v>
+      </c>
+      <c r="AH38">
+        <v>73</v>
+      </c>
+      <c r="AI38">
+        <v>0</v>
+      </c>
+      <c r="AJ38">
+        <v>0</v>
+      </c>
+      <c r="AK38">
+        <v>0</v>
+      </c>
+      <c r="AL38">
+        <v>0</v>
+      </c>
+      <c r="AM38">
+        <v>7</v>
+      </c>
+      <c r="AN38">
+        <v>0</v>
+      </c>
+      <c r="AO38">
+        <v>0</v>
+      </c>
+      <c r="AP38">
+        <v>0</v>
+      </c>
+      <c r="AQ38">
+        <v>0</v>
+      </c>
+      <c r="AR38">
+        <v>0</v>
+      </c>
+      <c r="AS38">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -6577,15 +7045,132 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="B40" t="s">
+        <v>415</v>
+      </c>
+      <c r="C40" t="s">
+        <v>416</v>
+      </c>
       <c r="D40">
         <v>2012</v>
       </c>
+      <c r="E40" t="s">
+        <v>417</v>
+      </c>
+      <c r="F40" t="s">
+        <v>418</v>
+      </c>
+      <c r="G40" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" t="s">
+        <v>419</v>
+      </c>
+      <c r="K40">
+        <v>20</v>
+      </c>
+      <c r="L40" t="s">
+        <v>48</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>420</v>
+      </c>
+      <c r="R40">
+        <v>5</v>
+      </c>
+      <c r="S40">
+        <v>8</v>
+      </c>
+      <c r="T40">
+        <v>4</v>
+      </c>
+      <c r="U40">
+        <v>0</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <v>0</v>
+      </c>
+      <c r="X40">
+        <v>0</v>
+      </c>
+      <c r="Y40">
+        <v>5</v>
+      </c>
+      <c r="Z40">
+        <v>42</v>
+      </c>
+      <c r="AA40">
+        <v>68</v>
+      </c>
+      <c r="AB40">
+        <v>0</v>
+      </c>
+      <c r="AC40">
+        <v>3</v>
+      </c>
+      <c r="AD40">
+        <v>0</v>
+      </c>
+      <c r="AE40">
+        <v>0</v>
+      </c>
+      <c r="AF40">
+        <v>9.5</v>
+      </c>
+      <c r="AG40">
+        <v>113</v>
+      </c>
+      <c r="AH40">
+        <v>121</v>
+      </c>
+      <c r="AI40">
+        <v>0</v>
+      </c>
+      <c r="AJ40">
+        <v>4</v>
+      </c>
+      <c r="AK40">
+        <v>0</v>
+      </c>
+      <c r="AL40">
+        <v>5</v>
+      </c>
+      <c r="AM40">
+        <v>0.5</v>
+      </c>
+      <c r="AN40">
+        <v>3</v>
+      </c>
+      <c r="AO40">
+        <v>13</v>
+      </c>
+      <c r="AP40">
+        <v>0</v>
+      </c>
+      <c r="AQ40">
+        <v>0</v>
+      </c>
+      <c r="AR40">
+        <v>0</v>
+      </c>
+      <c r="AS40">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -6713,15 +7298,135 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
+      <c r="B42" t="s">
+        <v>422</v>
+      </c>
+      <c r="C42" t="s">
+        <v>423</v>
+      </c>
       <c r="D42">
         <v>2012</v>
       </c>
+      <c r="E42" t="s">
+        <v>424</v>
+      </c>
+      <c r="F42" t="s">
+        <v>425</v>
+      </c>
+      <c r="G42" t="s">
+        <v>44</v>
+      </c>
+      <c r="H42" t="s">
+        <v>211</v>
+      </c>
+      <c r="K42">
+        <v>30</v>
+      </c>
+      <c r="L42" t="s">
+        <v>48</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42" t="s">
+        <v>426</v>
+      </c>
+      <c r="P42" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>427</v>
+      </c>
+      <c r="R42">
+        <v>4.5</v>
+      </c>
+      <c r="S42">
+        <v>0</v>
+      </c>
+      <c r="T42">
+        <v>0</v>
+      </c>
+      <c r="U42">
+        <v>0</v>
+      </c>
+      <c r="V42">
+        <v>0</v>
+      </c>
+      <c r="W42">
+        <v>0</v>
+      </c>
+      <c r="X42">
+        <v>0</v>
+      </c>
+      <c r="Y42">
+        <v>14.5</v>
+      </c>
+      <c r="Z42">
+        <v>120</v>
+      </c>
+      <c r="AA42">
+        <v>70</v>
+      </c>
+      <c r="AB42">
+        <v>0</v>
+      </c>
+      <c r="AC42">
+        <v>0</v>
+      </c>
+      <c r="AD42">
+        <v>0</v>
+      </c>
+      <c r="AE42">
+        <v>25</v>
+      </c>
+      <c r="AF42">
+        <v>10.5</v>
+      </c>
+      <c r="AG42">
+        <v>17</v>
+      </c>
+      <c r="AH42">
+        <v>89</v>
+      </c>
+      <c r="AI42">
+        <v>0</v>
+      </c>
+      <c r="AJ42">
+        <v>0</v>
+      </c>
+      <c r="AK42">
+        <v>0</v>
+      </c>
+      <c r="AL42">
+        <v>0</v>
+      </c>
+      <c r="AM42">
+        <v>0.5</v>
+      </c>
+      <c r="AN42">
+        <v>0</v>
+      </c>
+      <c r="AO42">
+        <v>0</v>
+      </c>
+      <c r="AP42">
+        <v>0</v>
+      </c>
+      <c r="AQ42">
+        <v>0</v>
+      </c>
+      <c r="AR42">
+        <v>0</v>
+      </c>
+      <c r="AS42">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -6843,15 +7548,129 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
+      <c r="B44" t="s">
+        <v>428</v>
+      </c>
+      <c r="C44" t="s">
+        <v>429</v>
+      </c>
       <c r="D44">
         <v>2013</v>
       </c>
+      <c r="E44" t="s">
+        <v>430</v>
+      </c>
+      <c r="F44" t="s">
+        <v>431</v>
+      </c>
+      <c r="G44" t="s">
+        <v>305</v>
+      </c>
+      <c r="H44" t="s">
+        <v>419</v>
+      </c>
+      <c r="K44">
+        <v>11</v>
+      </c>
+      <c r="L44" t="s">
+        <v>70</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44" t="s">
+        <v>432</v>
+      </c>
+      <c r="R44">
+        <v>4</v>
+      </c>
+      <c r="S44">
+        <v>0</v>
+      </c>
+      <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44">
+        <v>0</v>
+      </c>
+      <c r="V44">
+        <v>0</v>
+      </c>
+      <c r="W44">
+        <v>0</v>
+      </c>
+      <c r="X44">
+        <v>0</v>
+      </c>
+      <c r="Y44">
+        <v>4</v>
+      </c>
+      <c r="Z44">
+        <v>25</v>
+      </c>
+      <c r="AA44">
+        <v>23</v>
+      </c>
+      <c r="AB44">
+        <v>0</v>
+      </c>
+      <c r="AC44">
+        <v>8</v>
+      </c>
+      <c r="AD44">
+        <v>0</v>
+      </c>
+      <c r="AE44">
+        <v>34</v>
+      </c>
+      <c r="AF44">
+        <v>3</v>
+      </c>
+      <c r="AG44">
+        <v>11</v>
+      </c>
+      <c r="AH44">
+        <v>26</v>
+      </c>
+      <c r="AI44">
+        <v>0</v>
+      </c>
+      <c r="AJ44">
+        <v>0</v>
+      </c>
+      <c r="AK44">
+        <v>0</v>
+      </c>
+      <c r="AL44">
+        <v>0</v>
+      </c>
+      <c r="AM44">
+        <v>0</v>
+      </c>
+      <c r="AN44">
+        <v>0</v>
+      </c>
+      <c r="AO44">
+        <v>0</v>
+      </c>
+      <c r="AP44">
+        <v>0</v>
+      </c>
+      <c r="AQ44">
+        <v>0</v>
+      </c>
+      <c r="AR44">
+        <v>0</v>
+      </c>
+      <c r="AS44">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -6976,15 +7795,132 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
+      <c r="B46" t="s">
+        <v>433</v>
+      </c>
+      <c r="C46" t="s">
+        <v>434</v>
+      </c>
       <c r="D46">
         <v>2013</v>
       </c>
+      <c r="E46" t="s">
+        <v>435</v>
+      </c>
+      <c r="F46" t="s">
+        <v>436</v>
+      </c>
+      <c r="G46" t="s">
+        <v>437</v>
+      </c>
+      <c r="H46" t="s">
+        <v>244</v>
+      </c>
+      <c r="K46">
+        <v>39</v>
+      </c>
+      <c r="L46" t="s">
+        <v>48</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46" t="s">
+        <v>438</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>420</v>
+      </c>
+      <c r="R46">
+        <v>8</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+      <c r="T46">
+        <v>0</v>
+      </c>
+      <c r="U46">
+        <v>0</v>
+      </c>
+      <c r="V46">
+        <v>0</v>
+      </c>
+      <c r="W46">
+        <v>0</v>
+      </c>
+      <c r="X46">
+        <v>0</v>
+      </c>
+      <c r="Y46">
+        <v>21</v>
+      </c>
+      <c r="Z46">
+        <v>238</v>
+      </c>
+      <c r="AA46">
+        <v>179</v>
+      </c>
+      <c r="AB46">
+        <v>0</v>
+      </c>
+      <c r="AC46">
+        <v>0</v>
+      </c>
+      <c r="AD46">
+        <v>6</v>
+      </c>
+      <c r="AE46">
+        <v>5</v>
+      </c>
+      <c r="AF46">
+        <v>9</v>
+      </c>
+      <c r="AG46">
+        <v>70</v>
+      </c>
+      <c r="AH46">
+        <v>131</v>
+      </c>
+      <c r="AI46">
+        <v>0</v>
+      </c>
+      <c r="AJ46">
+        <v>0</v>
+      </c>
+      <c r="AK46">
+        <v>0</v>
+      </c>
+      <c r="AL46">
+        <v>0</v>
+      </c>
+      <c r="AM46">
+        <v>0.5</v>
+      </c>
+      <c r="AN46">
+        <v>0</v>
+      </c>
+      <c r="AO46">
+        <v>6</v>
+      </c>
+      <c r="AP46">
+        <v>0</v>
+      </c>
+      <c r="AQ46">
+        <v>6</v>
+      </c>
+      <c r="AR46">
+        <v>0</v>
+      </c>
+      <c r="AS46">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -7106,15 +8042,129 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
+      <c r="B48" t="s">
+        <v>439</v>
+      </c>
+      <c r="C48" t="s">
+        <v>440</v>
+      </c>
       <c r="D48">
         <v>2013</v>
       </c>
+      <c r="E48" t="s">
+        <v>441</v>
+      </c>
+      <c r="F48" t="s">
+        <v>442</v>
+      </c>
+      <c r="G48" t="s">
+        <v>64</v>
+      </c>
+      <c r="H48" t="s">
+        <v>443</v>
+      </c>
+      <c r="K48">
+        <v>14</v>
+      </c>
+      <c r="L48" t="s">
+        <v>70</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48" t="s">
+        <v>148</v>
+      </c>
+      <c r="R48">
+        <v>5.5</v>
+      </c>
+      <c r="S48">
+        <v>0</v>
+      </c>
+      <c r="T48">
+        <v>0</v>
+      </c>
+      <c r="U48">
+        <v>0</v>
+      </c>
+      <c r="V48">
+        <v>0</v>
+      </c>
+      <c r="W48">
+        <v>0</v>
+      </c>
+      <c r="X48">
+        <v>0</v>
+      </c>
+      <c r="Y48">
+        <v>5</v>
+      </c>
+      <c r="Z48">
+        <v>17</v>
+      </c>
+      <c r="AA48">
+        <v>34</v>
+      </c>
+      <c r="AB48">
+        <v>0</v>
+      </c>
+      <c r="AC48">
+        <v>23</v>
+      </c>
+      <c r="AD48">
+        <v>0</v>
+      </c>
+      <c r="AE48">
+        <v>28</v>
+      </c>
+      <c r="AF48">
+        <v>3</v>
+      </c>
+      <c r="AG48">
+        <v>18</v>
+      </c>
+      <c r="AH48">
+        <v>44</v>
+      </c>
+      <c r="AI48">
+        <v>0</v>
+      </c>
+      <c r="AJ48">
+        <v>0</v>
+      </c>
+      <c r="AK48">
+        <v>21</v>
+      </c>
+      <c r="AL48">
+        <v>0</v>
+      </c>
+      <c r="AM48">
+        <v>0.5</v>
+      </c>
+      <c r="AN48">
+        <v>0</v>
+      </c>
+      <c r="AO48">
+        <v>3</v>
+      </c>
+      <c r="AP48">
+        <v>0</v>
+      </c>
+      <c r="AQ48">
+        <v>0</v>
+      </c>
+      <c r="AR48">
+        <v>0</v>
+      </c>
+      <c r="AS48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -7236,7 +8286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -7244,7 +8294,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -7366,7 +8416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -7374,7 +8424,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -7499,7 +8549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -7507,7 +8557,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -7632,7 +8682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -7640,7 +8690,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -7765,7 +8815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -7773,7 +8823,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -7895,7 +8945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -7903,7 +8953,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -8026,7 +9076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -8034,7 +9084,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -8157,7 +9207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -8165,7 +9215,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -8290,7 +9340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -8298,7 +9348,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="67" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -8426,7 +9476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -8434,7 +9484,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -8556,7 +9606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -8564,7 +9614,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="71" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -8682,7 +9732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -8690,7 +9740,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -8816,7 +9866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -8824,7 +9874,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="75" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -8949,7 +9999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -8957,7 +10007,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="77" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -9079,7 +10129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
up to 2016 done
</commit_message>
<xml_diff>
--- a/AlitoDataset.xlsx
+++ b/AlitoDataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineparnell/alito-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685E5E44-453C-6240-BAF7-B7D97D2F786F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A87ADD-0C0C-B441-B72D-3B8B693F2223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,6 +58,7 @@
     <author>tc={B21FA207-DD6C-4EC4-AA1E-647AEEC95CBA}</author>
     <author>tc={EDBFDAAD-D50D-473D-8856-A184FE763FEC}</author>
     <author>tc={F5907484-1F67-418A-8263-E2E9C18888C5}</author>
+    <author>tc={172A06DA-0462-7942-A104-EFAF337D8F7F}</author>
     <author>tc={29BD8916-C473-4AD3-99BD-980DB0A6B111}</author>
     <author>tc={E76B42E8-7392-42FF-9D0D-4771AF924F11}</author>
     <author>tc={72089604-F3E5-43FD-BB29-19F63B5D3451}</author>
@@ -254,7 +255,15 @@
     Scalia's seat empty, so contentious?</t>
       </text>
     </comment>
-    <comment ref="G63" authorId="23" shapeId="0" xr:uid="{29BD8916-C473-4AD3-99BD-980DB0A6B111}">
+    <comment ref="B62" authorId="23" shapeId="0" xr:uid="{172A06DA-0462-7942-A104-EFAF337D8F7F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    There is so much going on idk what to do</t>
+      </text>
+    </comment>
+    <comment ref="G63" authorId="24" shapeId="0" xr:uid="{29BD8916-C473-4AD3-99BD-980DB0A6B111}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -262,7 +271,7 @@
     remanded for further consideration</t>
       </text>
     </comment>
-    <comment ref="C67" authorId="24" shapeId="0" xr:uid="{E76B42E8-7392-42FF-9D0D-4771AF924F11}">
+    <comment ref="C67" authorId="25" shapeId="0" xr:uid="{E76B42E8-7392-42FF-9D0D-4771AF924F11}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -270,7 +279,7 @@
     Date is off for a case in 2016 term; case was reargued in 2017</t>
       </text>
     </comment>
-    <comment ref="P67" authorId="25" shapeId="0" xr:uid="{72089604-F3E5-43FD-BB29-19F63B5D3451}">
+    <comment ref="P67" authorId="26" shapeId="0" xr:uid="{72089604-F3E5-43FD-BB29-19F63B5D3451}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -280,7 +289,7 @@
     ???</t>
       </text>
     </comment>
-    <comment ref="C69" authorId="26" shapeId="0" xr:uid="{332B7A30-BB9D-49DC-BFB2-C0D3DF1392D4}">
+    <comment ref="C69" authorId="27" shapeId="0" xr:uid="{332B7A30-BB9D-49DC-BFB2-C0D3DF1392D4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -288,7 +297,7 @@
     Should this be 2016? Is this correct?</t>
       </text>
     </comment>
-    <comment ref="G71" authorId="27" shapeId="0" xr:uid="{007B5D8A-F2ED-4913-B91D-14040B184733}">
+    <comment ref="G71" authorId="28" shapeId="0" xr:uid="{007B5D8A-F2ED-4913-B91D-14040B184733}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -296,7 +305,7 @@
     No answer listed?</t>
       </text>
     </comment>
-    <comment ref="H71" authorId="28" shapeId="0" xr:uid="{72CF621A-23CD-487A-A5C4-F1F5F52BEE03}">
+    <comment ref="H71" authorId="29" shapeId="0" xr:uid="{72CF621A-23CD-487A-A5C4-F1F5F52BEE03}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -304,7 +313,7 @@
     no reasoning listed</t>
       </text>
     </comment>
-    <comment ref="G73" authorId="29" shapeId="0" xr:uid="{945D29AB-E037-4687-BFF4-24AB13377B9D}">
+    <comment ref="G73" authorId="30" shapeId="0" xr:uid="{945D29AB-E037-4687-BFF4-24AB13377B9D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -312,7 +321,7 @@
     "Yes to first, no to questions about merits"</t>
       </text>
     </comment>
-    <comment ref="AF73" authorId="30" shapeId="0" xr:uid="{A8BB29DE-2D6C-43B6-AB81-6C0E7925BF84}">
+    <comment ref="AF73" authorId="31" shapeId="0" xr:uid="{A8BB29DE-2D6C-43B6-AB81-6C0E7925BF84}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -325,7 +334,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="487">
   <si>
     <t>Case Name</t>
   </si>
@@ -1671,12 +1680,141 @@
   <si>
     <t>pragmatism</t>
   </si>
+  <si>
+    <t>575 US __ (2015)</t>
+  </si>
+  <si>
+    <t>issue preclusion</t>
+  </si>
+  <si>
+    <t>Does a finding of a likelihood of confusion by the trademark trial and appeal board preclude a re-litigation in federal court?</t>
+  </si>
+  <si>
+    <t>Alito,Roberts,Kennedy,Ginsburg,Breyer,Sotomayor,Kagan</t>
+  </si>
+  <si>
+    <t>Scalia,Thomas</t>
+  </si>
+  <si>
+    <t>B&amp;B Hardware v. Hargis</t>
+  </si>
+  <si>
+    <t>Davis v. Ayala</t>
+  </si>
+  <si>
+    <t>576 U.S. ____ (2015)</t>
+  </si>
+  <si>
+    <t>Preemptory challenges in jury selection and whether it was "harmless error"</t>
+  </si>
+  <si>
+    <t>is a state court's determination that a federal constitutional violation is harmless error an "adjudication on the merits" for purposes of the antiterrorism and effective death penalty act of 1996? Did the court of appeals properly apply the standard articulated in brecht v abrahamson for reviewing whether a constitutional violation is harmless error?</t>
+  </si>
+  <si>
+    <t>harmless error</t>
+  </si>
+  <si>
+    <t>doctrinl, pragmatic</t>
+  </si>
+  <si>
+    <t>Alito,Roberts,Scalia,Thomas,Kennedy</t>
+  </si>
+  <si>
+    <t>Sotomayor,Ginsburg,Kagan,Breyer</t>
+  </si>
+  <si>
+    <t>Holt v. Hobbs</t>
+  </si>
+  <si>
+    <t>574 U.S. 352 (2015)</t>
+  </si>
+  <si>
+    <t>Religious Land use and Institutionalized Persons Act</t>
+  </si>
+  <si>
+    <t>Does the Arkansas department of corrections grooming policy violate the religious land use and institutionalized persons act by preventing holt from growing a one half inch beard in accordance with his religious beliefs?</t>
+  </si>
+  <si>
+    <t>Ohio v. Clark</t>
+  </si>
+  <si>
+    <t>576 US ___ (2015)</t>
+  </si>
+  <si>
+    <t>sixth amendment confrontation clause</t>
+  </si>
+  <si>
+    <t>does the individual's obligation to report suspected child abuse make that individual an agent of law enforcement for purposes of the confrontation clause? Do a child's out of court statements to a teacher in response to a teachers concerns about potential child abuse qualify as testimonial statements subject to the confrontation clause?</t>
+  </si>
+  <si>
+    <t>Birchfield v. North Dakota</t>
+  </si>
+  <si>
+    <t>579 U.S. ___ (2016)</t>
+  </si>
+  <si>
+    <t>4th amendment</t>
+  </si>
+  <si>
+    <t>in the absence of a warrant may a state statute criminalize an individuals refusal to submit to a blood alcohol test?</t>
+  </si>
+  <si>
+    <t>Alito,Roberts,Kennedy,Breyer,Ginsburg,Kagan,Sotomayor</t>
+  </si>
+  <si>
+    <t>Nichols v. US</t>
+  </si>
+  <si>
+    <t>578 US __ (2016)</t>
+  </si>
+  <si>
+    <t>sex offender registration and notification act</t>
+  </si>
+  <si>
+    <t>is a convicted sexual offender required to update his residency under the sex offender registration and notification act if he moves outside of us jurisdiction?</t>
+  </si>
+  <si>
+    <t>Alito,Roberts,Kennedy,Thomas,Breyer,Ginsburg,Sotomayor,Kagan</t>
+  </si>
+  <si>
+    <t>RJR Nabisco v. European Community</t>
+  </si>
+  <si>
+    <t>579 U.S. ____ (2016)</t>
+  </si>
+  <si>
+    <t>can the recketeer influenced corrupt organization statute apply extraterritorially?</t>
+  </si>
+  <si>
+    <t>RICO (18 U.S.C. §§1962(a)-(d) &amp;amp; §1964(c))</t>
+  </si>
+  <si>
+    <t>Yes | No</t>
+  </si>
+  <si>
+    <t>doctrinal, textualism, pragmatic</t>
+  </si>
+  <si>
+    <t>Taylor v. US</t>
+  </si>
+  <si>
+    <t>579 US __ (2016)</t>
+  </si>
+  <si>
+    <t>commerce clause analysis in context of hobbs act</t>
+  </si>
+  <si>
+    <t>can congress authorize a cause of action based on a violation of a federal statute and therefore confer article III standing on a plaintiff who has not suffered concrete harm?</t>
+  </si>
+  <si>
+    <t>Alito,Roberts,Kennedy,Ginsburg,Sotomayor,Breyer,Kagan</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1690,6 +1828,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2123,6 +2267,9 @@
   <threadedComment ref="M61" dT="2020-07-21T21:01:44.01" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{F5907484-1F67-418A-8263-E2E9C18888C5}">
     <text>Scalia's seat empty, so contentious?</text>
   </threadedComment>
+  <threadedComment ref="B62" dT="2020-07-23T19:05:48.52" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{172A06DA-0462-7942-A104-EFAF337D8F7F}">
+    <text>There is so much going on idk what to do</text>
+  </threadedComment>
   <threadedComment ref="G63" dT="2020-07-21T21:03:34.53" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{29BD8916-C473-4AD3-99BD-980DB0A6B111}">
     <text>remanded for further consideration</text>
   </threadedComment>
@@ -2157,8 +2304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060A011E-60FD-5047-91C8-6B9B09AABF05}">
   <dimension ref="A1:AS78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="AT64" sqref="AT64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8290,8 +8437,125 @@
       <c r="A50">
         <v>49</v>
       </c>
+      <c r="B50" t="s">
+        <v>449</v>
+      </c>
+      <c r="C50" t="s">
+        <v>444</v>
+      </c>
       <c r="D50">
         <v>2014</v>
+      </c>
+      <c r="E50" t="s">
+        <v>445</v>
+      </c>
+      <c r="F50" t="s">
+        <v>446</v>
+      </c>
+      <c r="G50" t="s">
+        <v>64</v>
+      </c>
+      <c r="H50" t="s">
+        <v>243</v>
+      </c>
+      <c r="K50">
+        <v>10</v>
+      </c>
+      <c r="L50" t="s">
+        <v>78</v>
+      </c>
+      <c r="M50">
+        <v>2</v>
+      </c>
+      <c r="N50" t="s">
+        <v>447</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>448</v>
+      </c>
+      <c r="R50">
+        <v>3</v>
+      </c>
+      <c r="S50">
+        <v>0</v>
+      </c>
+      <c r="T50">
+        <v>0</v>
+      </c>
+      <c r="U50">
+        <v>0</v>
+      </c>
+      <c r="V50">
+        <v>0</v>
+      </c>
+      <c r="W50">
+        <v>0</v>
+      </c>
+      <c r="X50">
+        <v>0</v>
+      </c>
+      <c r="Y50">
+        <v>3</v>
+      </c>
+      <c r="Z50">
+        <v>30</v>
+      </c>
+      <c r="AA50">
+        <v>14</v>
+      </c>
+      <c r="AB50">
+        <v>0</v>
+      </c>
+      <c r="AC50">
+        <v>0</v>
+      </c>
+      <c r="AD50">
+        <v>6</v>
+      </c>
+      <c r="AE50">
+        <v>5</v>
+      </c>
+      <c r="AF50">
+        <v>3.5</v>
+      </c>
+      <c r="AG50">
+        <v>36</v>
+      </c>
+      <c r="AH50">
+        <v>68</v>
+      </c>
+      <c r="AI50">
+        <v>2</v>
+      </c>
+      <c r="AJ50">
+        <v>0</v>
+      </c>
+      <c r="AK50">
+        <v>8</v>
+      </c>
+      <c r="AL50">
+        <v>5</v>
+      </c>
+      <c r="AM50">
+        <v>0.5</v>
+      </c>
+      <c r="AN50">
+        <v>0</v>
+      </c>
+      <c r="AO50">
+        <v>0</v>
+      </c>
+      <c r="AP50">
+        <v>0</v>
+      </c>
+      <c r="AQ50">
+        <v>0</v>
+      </c>
+      <c r="AR50">
+        <v>0</v>
+      </c>
+      <c r="AS50">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:45" x14ac:dyDescent="0.2">
@@ -8420,8 +8684,125 @@
       <c r="A52">
         <v>51</v>
       </c>
+      <c r="B52" t="s">
+        <v>450</v>
+      </c>
+      <c r="C52" t="s">
+        <v>451</v>
+      </c>
       <c r="D52">
         <v>2014</v>
+      </c>
+      <c r="E52" t="s">
+        <v>452</v>
+      </c>
+      <c r="F52" t="s">
+        <v>453</v>
+      </c>
+      <c r="G52" t="s">
+        <v>454</v>
+      </c>
+      <c r="H52" t="s">
+        <v>455</v>
+      </c>
+      <c r="K52">
+        <v>29</v>
+      </c>
+      <c r="L52" t="s">
+        <v>48</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52" t="s">
+        <v>456</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>457</v>
+      </c>
+      <c r="R52">
+        <v>8</v>
+      </c>
+      <c r="S52">
+        <v>0</v>
+      </c>
+      <c r="T52">
+        <v>0</v>
+      </c>
+      <c r="U52">
+        <v>0</v>
+      </c>
+      <c r="V52">
+        <v>0</v>
+      </c>
+      <c r="W52">
+        <v>0</v>
+      </c>
+      <c r="X52">
+        <v>0</v>
+      </c>
+      <c r="Y52">
+        <v>14</v>
+      </c>
+      <c r="Z52">
+        <v>97</v>
+      </c>
+      <c r="AA52">
+        <v>94</v>
+      </c>
+      <c r="AB52">
+        <v>0</v>
+      </c>
+      <c r="AC52">
+        <v>0</v>
+      </c>
+      <c r="AD52">
+        <v>0</v>
+      </c>
+      <c r="AE52">
+        <v>0</v>
+      </c>
+      <c r="AF52">
+        <v>6</v>
+      </c>
+      <c r="AG52">
+        <v>9.5</v>
+      </c>
+      <c r="AH52">
+        <v>68.5</v>
+      </c>
+      <c r="AI52">
+        <v>0</v>
+      </c>
+      <c r="AJ52">
+        <v>0</v>
+      </c>
+      <c r="AK52">
+        <v>0</v>
+      </c>
+      <c r="AL52">
+        <v>0</v>
+      </c>
+      <c r="AM52">
+        <v>1</v>
+      </c>
+      <c r="AN52">
+        <v>14</v>
+      </c>
+      <c r="AO52">
+        <v>14</v>
+      </c>
+      <c r="AP52">
+        <v>0</v>
+      </c>
+      <c r="AQ52">
+        <v>0</v>
+      </c>
+      <c r="AR52">
+        <v>0</v>
+      </c>
+      <c r="AS52">
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:45" x14ac:dyDescent="0.2">
@@ -8553,8 +8934,122 @@
       <c r="A54">
         <v>53</v>
       </c>
+      <c r="B54" t="s">
+        <v>458</v>
+      </c>
+      <c r="C54" t="s">
+        <v>459</v>
+      </c>
       <c r="D54">
         <v>2014</v>
+      </c>
+      <c r="E54" t="s">
+        <v>460</v>
+      </c>
+      <c r="F54" t="s">
+        <v>461</v>
+      </c>
+      <c r="G54" t="s">
+        <v>64</v>
+      </c>
+      <c r="H54" t="s">
+        <v>443</v>
+      </c>
+      <c r="K54">
+        <v>15</v>
+      </c>
+      <c r="L54" t="s">
+        <v>70</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54" t="s">
+        <v>316</v>
+      </c>
+      <c r="R54">
+        <v>5.5</v>
+      </c>
+      <c r="S54">
+        <v>0</v>
+      </c>
+      <c r="T54">
+        <v>0</v>
+      </c>
+      <c r="U54">
+        <v>0</v>
+      </c>
+      <c r="V54">
+        <v>27</v>
+      </c>
+      <c r="W54">
+        <v>0</v>
+      </c>
+      <c r="X54">
+        <v>0</v>
+      </c>
+      <c r="Y54">
+        <v>5.5</v>
+      </c>
+      <c r="Z54">
+        <v>35</v>
+      </c>
+      <c r="AA54">
+        <v>110</v>
+      </c>
+      <c r="AB54">
+        <v>0</v>
+      </c>
+      <c r="AC54">
+        <v>21</v>
+      </c>
+      <c r="AD54">
+        <v>0</v>
+      </c>
+      <c r="AE54">
+        <v>0</v>
+      </c>
+      <c r="AF54">
+        <v>3.5</v>
+      </c>
+      <c r="AG54">
+        <v>13</v>
+      </c>
+      <c r="AH54">
+        <v>63</v>
+      </c>
+      <c r="AI54">
+        <v>0</v>
+      </c>
+      <c r="AJ54">
+        <v>17</v>
+      </c>
+      <c r="AK54">
+        <v>0</v>
+      </c>
+      <c r="AL54">
+        <v>0</v>
+      </c>
+      <c r="AM54">
+        <v>0.5</v>
+      </c>
+      <c r="AN54">
+        <v>0</v>
+      </c>
+      <c r="AO54">
+        <v>0</v>
+      </c>
+      <c r="AP54">
+        <v>0</v>
+      </c>
+      <c r="AQ54">
+        <v>0</v>
+      </c>
+      <c r="AR54">
+        <v>0</v>
+      </c>
+      <c r="AS54">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:45" x14ac:dyDescent="0.2">
@@ -8686,8 +9181,122 @@
       <c r="A56">
         <v>55</v>
       </c>
+      <c r="B56" t="s">
+        <v>462</v>
+      </c>
+      <c r="C56" t="s">
+        <v>463</v>
+      </c>
       <c r="D56">
         <v>2014</v>
+      </c>
+      <c r="E56" t="s">
+        <v>464</v>
+      </c>
+      <c r="F56" t="s">
+        <v>465</v>
+      </c>
+      <c r="G56" t="s">
+        <v>44</v>
+      </c>
+      <c r="H56" t="s">
+        <v>133</v>
+      </c>
+      <c r="K56">
+        <v>12</v>
+      </c>
+      <c r="L56" t="s">
+        <v>70</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56" t="s">
+        <v>316</v>
+      </c>
+      <c r="R56">
+        <v>6.5</v>
+      </c>
+      <c r="S56">
+        <v>91</v>
+      </c>
+      <c r="T56">
+        <v>6</v>
+      </c>
+      <c r="U56">
+        <v>0</v>
+      </c>
+      <c r="V56">
+        <v>0</v>
+      </c>
+      <c r="W56">
+        <v>0</v>
+      </c>
+      <c r="X56">
+        <v>0</v>
+      </c>
+      <c r="Y56">
+        <v>3.5</v>
+      </c>
+      <c r="Z56">
+        <v>41</v>
+      </c>
+      <c r="AA56">
+        <v>78</v>
+      </c>
+      <c r="AB56">
+        <v>22</v>
+      </c>
+      <c r="AC56">
+        <v>5</v>
+      </c>
+      <c r="AD56">
+        <v>0</v>
+      </c>
+      <c r="AE56">
+        <v>0</v>
+      </c>
+      <c r="AF56">
+        <v>2</v>
+      </c>
+      <c r="AG56">
+        <v>20</v>
+      </c>
+      <c r="AH56">
+        <v>29</v>
+      </c>
+      <c r="AI56">
+        <v>0</v>
+      </c>
+      <c r="AJ56">
+        <v>0</v>
+      </c>
+      <c r="AK56">
+        <v>0</v>
+      </c>
+      <c r="AL56">
+        <v>0</v>
+      </c>
+      <c r="AM56">
+        <v>0</v>
+      </c>
+      <c r="AN56">
+        <v>0</v>
+      </c>
+      <c r="AO56">
+        <v>0</v>
+      </c>
+      <c r="AP56">
+        <v>0</v>
+      </c>
+      <c r="AQ56">
+        <v>0</v>
+      </c>
+      <c r="AR56">
+        <v>0</v>
+      </c>
+      <c r="AS56">
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:45" x14ac:dyDescent="0.2">
@@ -8819,8 +9428,125 @@
       <c r="A58">
         <v>57</v>
       </c>
+      <c r="B58" t="s">
+        <v>466</v>
+      </c>
+      <c r="C58" t="s">
+        <v>467</v>
+      </c>
       <c r="D58">
         <v>2015</v>
+      </c>
+      <c r="E58" t="s">
+        <v>468</v>
+      </c>
+      <c r="F58" t="s">
+        <v>469</v>
+      </c>
+      <c r="G58" t="s">
+        <v>44</v>
+      </c>
+      <c r="H58" t="s">
+        <v>321</v>
+      </c>
+      <c r="K58">
+        <v>37</v>
+      </c>
+      <c r="L58" t="s">
+        <v>270</v>
+      </c>
+      <c r="M58">
+        <v>2</v>
+      </c>
+      <c r="N58" t="s">
+        <v>470</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>106</v>
+      </c>
+      <c r="R58">
+        <v>11</v>
+      </c>
+      <c r="S58">
+        <v>0</v>
+      </c>
+      <c r="T58">
+        <v>0</v>
+      </c>
+      <c r="U58">
+        <v>0</v>
+      </c>
+      <c r="V58">
+        <v>0</v>
+      </c>
+      <c r="W58">
+        <v>0</v>
+      </c>
+      <c r="X58">
+        <v>0</v>
+      </c>
+      <c r="Y58">
+        <v>15</v>
+      </c>
+      <c r="Z58">
+        <v>122.5</v>
+      </c>
+      <c r="AA58">
+        <v>109.5</v>
+      </c>
+      <c r="AB58">
+        <v>29</v>
+      </c>
+      <c r="AC58">
+        <v>0</v>
+      </c>
+      <c r="AD58">
+        <v>0</v>
+      </c>
+      <c r="AE58">
+        <v>0</v>
+      </c>
+      <c r="AF58">
+        <v>10</v>
+      </c>
+      <c r="AG58">
+        <v>69</v>
+      </c>
+      <c r="AH58">
+        <v>112.5</v>
+      </c>
+      <c r="AI58">
+        <v>0</v>
+      </c>
+      <c r="AJ58">
+        <v>13</v>
+      </c>
+      <c r="AK58">
+        <v>0</v>
+      </c>
+      <c r="AL58">
+        <v>0</v>
+      </c>
+      <c r="AM58">
+        <v>0.5</v>
+      </c>
+      <c r="AN58">
+        <v>0</v>
+      </c>
+      <c r="AO58">
+        <v>0</v>
+      </c>
+      <c r="AP58">
+        <v>0</v>
+      </c>
+      <c r="AQ58">
+        <v>0</v>
+      </c>
+      <c r="AR58">
+        <v>0</v>
+      </c>
+      <c r="AS58">
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:45" x14ac:dyDescent="0.2">
@@ -8949,8 +9675,122 @@
       <c r="A60">
         <v>59</v>
       </c>
+      <c r="B60" t="s">
+        <v>471</v>
+      </c>
+      <c r="C60" t="s">
+        <v>472</v>
+      </c>
       <c r="D60">
         <v>2015</v>
+      </c>
+      <c r="E60" t="s">
+        <v>473</v>
+      </c>
+      <c r="F60" t="s">
+        <v>474</v>
+      </c>
+      <c r="G60" t="s">
+        <v>44</v>
+      </c>
+      <c r="H60" t="s">
+        <v>365</v>
+      </c>
+      <c r="K60">
+        <v>8</v>
+      </c>
+      <c r="L60" t="s">
+        <v>293</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60" t="s">
+        <v>475</v>
+      </c>
+      <c r="R60">
+        <v>3.75</v>
+      </c>
+      <c r="S60">
+        <v>0</v>
+      </c>
+      <c r="T60">
+        <v>0</v>
+      </c>
+      <c r="U60">
+        <v>0</v>
+      </c>
+      <c r="V60">
+        <v>0</v>
+      </c>
+      <c r="W60">
+        <v>0</v>
+      </c>
+      <c r="X60">
+        <v>0</v>
+      </c>
+      <c r="Y60">
+        <v>1.5</v>
+      </c>
+      <c r="Z60">
+        <v>0</v>
+      </c>
+      <c r="AA60">
+        <v>0</v>
+      </c>
+      <c r="AB60">
+        <v>0</v>
+      </c>
+      <c r="AC60">
+        <v>8</v>
+      </c>
+      <c r="AD60">
+        <v>13</v>
+      </c>
+      <c r="AE60">
+        <v>36</v>
+      </c>
+      <c r="AF60">
+        <v>2.75</v>
+      </c>
+      <c r="AG60">
+        <v>0</v>
+      </c>
+      <c r="AH60">
+        <v>30</v>
+      </c>
+      <c r="AI60">
+        <v>0</v>
+      </c>
+      <c r="AJ60">
+        <v>5</v>
+      </c>
+      <c r="AK60">
+        <v>5</v>
+      </c>
+      <c r="AL60">
+        <v>17</v>
+      </c>
+      <c r="AM60">
+        <v>0</v>
+      </c>
+      <c r="AN60">
+        <v>0</v>
+      </c>
+      <c r="AO60">
+        <v>0</v>
+      </c>
+      <c r="AP60">
+        <v>0</v>
+      </c>
+      <c r="AQ60">
+        <v>0</v>
+      </c>
+      <c r="AR60">
+        <v>0</v>
+      </c>
+      <c r="AS60">
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:45" x14ac:dyDescent="0.2">
@@ -9080,8 +9920,29 @@
       <c r="A62">
         <v>61</v>
       </c>
+      <c r="B62" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="C62" t="s">
+        <v>477</v>
+      </c>
       <c r="D62">
         <v>2015</v>
+      </c>
+      <c r="E62" t="s">
+        <v>479</v>
+      </c>
+      <c r="F62" t="s">
+        <v>478</v>
+      </c>
+      <c r="G62" t="s">
+        <v>480</v>
+      </c>
+      <c r="H62" t="s">
+        <v>481</v>
+      </c>
+      <c r="K62">
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:45" x14ac:dyDescent="0.2">
@@ -9211,8 +10072,125 @@
       <c r="A64">
         <v>63</v>
       </c>
+      <c r="B64" t="s">
+        <v>482</v>
+      </c>
+      <c r="C64" t="s">
+        <v>483</v>
+      </c>
       <c r="D64">
         <v>2015</v>
+      </c>
+      <c r="E64" t="s">
+        <v>484</v>
+      </c>
+      <c r="F64" t="s">
+        <v>485</v>
+      </c>
+      <c r="G64" t="s">
+        <v>64</v>
+      </c>
+      <c r="H64" t="s">
+        <v>243</v>
+      </c>
+      <c r="K64">
+        <v>9</v>
+      </c>
+      <c r="L64" t="s">
+        <v>270</v>
+      </c>
+      <c r="M64">
+        <v>2</v>
+      </c>
+      <c r="N64" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>106</v>
+      </c>
+      <c r="R64">
+        <v>2.5</v>
+      </c>
+      <c r="S64">
+        <v>0</v>
+      </c>
+      <c r="T64">
+        <v>0</v>
+      </c>
+      <c r="U64">
+        <v>0</v>
+      </c>
+      <c r="V64">
+        <v>0</v>
+      </c>
+      <c r="W64">
+        <v>0</v>
+      </c>
+      <c r="X64">
+        <v>0</v>
+      </c>
+      <c r="Y64">
+        <v>3.5</v>
+      </c>
+      <c r="Z64">
+        <v>62</v>
+      </c>
+      <c r="AA64">
+        <v>16</v>
+      </c>
+      <c r="AB64">
+        <v>0</v>
+      </c>
+      <c r="AC64">
+        <v>0</v>
+      </c>
+      <c r="AD64">
+        <v>0</v>
+      </c>
+      <c r="AE64">
+        <v>5</v>
+      </c>
+      <c r="AF64">
+        <v>2.5</v>
+      </c>
+      <c r="AG64">
+        <v>14</v>
+      </c>
+      <c r="AH64">
+        <v>16</v>
+      </c>
+      <c r="AI64">
+        <v>0</v>
+      </c>
+      <c r="AJ64">
+        <v>9</v>
+      </c>
+      <c r="AK64">
+        <v>0</v>
+      </c>
+      <c r="AL64">
+        <v>2</v>
+      </c>
+      <c r="AM64">
+        <v>0.5</v>
+      </c>
+      <c r="AN64">
+        <v>0</v>
+      </c>
+      <c r="AO64">
+        <v>8</v>
+      </c>
+      <c r="AP64">
+        <v>0</v>
+      </c>
+      <c r="AQ64">
+        <v>0</v>
+      </c>
+      <c r="AR64">
+        <v>0</v>
+      </c>
+      <c r="AS64">
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:45" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
All years finished; no oyez difference flags entered yet
</commit_message>
<xml_diff>
--- a/AlitoDataset.xlsx
+++ b/AlitoDataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineparnell/alito-research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jtsanz\alito-research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A87ADD-0C0C-B441-B72D-3B8B693F2223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3E6667-1E01-4362-89D6-A11B912BE922}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
+    <workbookView xWindow="4800" yWindow="1330" windowWidth="14400" windowHeight="7360" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,13 +60,16 @@
     <author>tc={F5907484-1F67-418A-8263-E2E9C18888C5}</author>
     <author>tc={172A06DA-0462-7942-A104-EFAF337D8F7F}</author>
     <author>tc={29BD8916-C473-4AD3-99BD-980DB0A6B111}</author>
+    <author>tc={E8ECB88B-20FB-427C-BA5A-E55F0CA3A4FE}</author>
     <author>tc={E76B42E8-7392-42FF-9D0D-4771AF924F11}</author>
     <author>tc={72089604-F3E5-43FD-BB29-19F63B5D3451}</author>
     <author>tc={332B7A30-BB9D-49DC-BFB2-C0D3DF1392D4}</author>
     <author>tc={007B5D8A-F2ED-4913-B91D-14040B184733}</author>
     <author>tc={72CF621A-23CD-487A-A5C4-F1F5F52BEE03}</author>
+    <author>tc={A4DF1674-26FC-4C25-8DF7-2385D5EAC7EB}</author>
     <author>tc={945D29AB-E037-4687-BFF4-24AB13377B9D}</author>
     <author>tc={A8BB29DE-2D6C-43B6-AB81-6C0E7925BF84}</author>
+    <author>tc={A6A15053-58E0-4B97-9B80-191DA346406A}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5010FC8D-4B2F-2744-9AA3-E06DCDD6F440}">
@@ -271,7 +274,15 @@
     remanded for further consideration</t>
       </text>
     </comment>
-    <comment ref="C67" authorId="25" shapeId="0" xr:uid="{E76B42E8-7392-42FF-9D0D-4771AF924F11}">
+    <comment ref="G66" authorId="25" shapeId="0" xr:uid="{E8ECB88B-20FB-427C-BA5A-E55F0CA3A4FE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    yes or no answer?</t>
+      </text>
+    </comment>
+    <comment ref="C67" authorId="26" shapeId="0" xr:uid="{E76B42E8-7392-42FF-9D0D-4771AF924F11}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -279,7 +290,7 @@
     Date is off for a case in 2016 term; case was reargued in 2017</t>
       </text>
     </comment>
-    <comment ref="P67" authorId="26" shapeId="0" xr:uid="{72089604-F3E5-43FD-BB29-19F63B5D3451}">
+    <comment ref="P67" authorId="27" shapeId="0" xr:uid="{72089604-F3E5-43FD-BB29-19F63B5D3451}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -289,7 +300,7 @@
     ???</t>
       </text>
     </comment>
-    <comment ref="C69" authorId="27" shapeId="0" xr:uid="{332B7A30-BB9D-49DC-BFB2-C0D3DF1392D4}">
+    <comment ref="C69" authorId="28" shapeId="0" xr:uid="{332B7A30-BB9D-49DC-BFB2-C0D3DF1392D4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -297,7 +308,7 @@
     Should this be 2016? Is this correct?</t>
       </text>
     </comment>
-    <comment ref="G71" authorId="28" shapeId="0" xr:uid="{007B5D8A-F2ED-4913-B91D-14040B184733}">
+    <comment ref="G71" authorId="29" shapeId="0" xr:uid="{007B5D8A-F2ED-4913-B91D-14040B184733}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -305,7 +316,7 @@
     No answer listed?</t>
       </text>
     </comment>
-    <comment ref="H71" authorId="29" shapeId="0" xr:uid="{72CF621A-23CD-487A-A5C4-F1F5F52BEE03}">
+    <comment ref="H71" authorId="30" shapeId="0" xr:uid="{72CF621A-23CD-487A-A5C4-F1F5F52BEE03}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -313,7 +324,15 @@
     no reasoning listed</t>
       </text>
     </comment>
-    <comment ref="G73" authorId="30" shapeId="0" xr:uid="{945D29AB-E037-4687-BFF4-24AB13377B9D}">
+    <comment ref="H72" authorId="31" shapeId="0" xr:uid="{A4DF1674-26FC-4C25-8DF7-2385D5EAC7EB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Legislative history at end; higlighted in orange; should i include purposiveism?</t>
+      </text>
+    </comment>
+    <comment ref="G73" authorId="32" shapeId="0" xr:uid="{945D29AB-E037-4687-BFF4-24AB13377B9D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -321,7 +340,7 @@
     "Yes to first, no to questions about merits"</t>
       </text>
     </comment>
-    <comment ref="AF73" authorId="31" shapeId="0" xr:uid="{A8BB29DE-2D6C-43B6-AB81-6C0E7925BF84}">
+    <comment ref="AF73" authorId="33" shapeId="0" xr:uid="{A8BB29DE-2D6C-43B6-AB81-6C0E7925BF84}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -329,12 +348,20 @@
     pp. 24-25 and 38; didn't code from 24-25</t>
       </text>
     </comment>
+    <comment ref="H78" authorId="34" shapeId="0" xr:uid="{A6A15053-58E0-4B97-9B80-191DA346406A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    "Congressional Intent" highlighted in orange; should i include purposeiveism?</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="525">
   <si>
     <t>Case Name</t>
   </si>
@@ -1420,9 +1447,6 @@
     <t>Briston-Myers Squibb Co. v. Superior Court of CA, San Francisco Cty.</t>
   </si>
   <si>
-    <t>582 u.S. ___(2017)</t>
-  </si>
-  <si>
     <t>Personal jurisdiction</t>
   </si>
   <si>
@@ -1507,9 +1531,6 @@
     <t>Did the district court issue an appealable interlocutory injunction when it invalidated Texas’ enacted redistricting plan and ordered the parties to appear at a remedial hearing to redraw state congressional districts unless the Governor convened a special legislative session to redraw the congressional map within three days?|Did the Texas legislature act with an unlawful purpose when it enacted a redistricting plan originally imposed by the district court to remedy any possible constitutional and statutory defects in a previous legislative plan that was repealed before it took effect?|Did the Texas legislature engage in intentional vote dilution when it adopted Congressional District (CD) 27 in 2013 after the district court’s 2012 finding that CD 27 did not support a plausible claim of racially discriminatory purpose and did not dilute Latino voting strength because it was impossible to create an additional Latino opportunity district in the region?|Did the legislature engage in racial gerrymandering in CD 35 when it simply adopted the district unchanged as part of the court-ordered remedial plan?</t>
   </si>
   <si>
-    <t>Roberts;Kennedy,Alito,Thomas,Gorsuch</t>
-  </si>
-  <si>
     <t>Thomas;Gorsuch</t>
   </si>
   <si>
@@ -1765,9 +1786,6 @@
     <t>Nichols v. US</t>
   </si>
   <si>
-    <t>578 US __ (2016)</t>
-  </si>
-  <si>
     <t>sex offender registration and notification act</t>
   </si>
   <si>
@@ -1798,9 +1816,6 @@
     <t>Taylor v. US</t>
   </si>
   <si>
-    <t>579 US __ (2016)</t>
-  </si>
-  <si>
     <t>commerce clause analysis in context of hobbs act</t>
   </si>
   <si>
@@ -1808,6 +1823,132 @@
   </si>
   <si>
     <t>Alito,Roberts,Kennedy,Ginsburg,Sotomayor,Breyer,Kagan</t>
+  </si>
+  <si>
+    <t>County of Los Angeles v. Mendez</t>
+  </si>
+  <si>
+    <t>582 U.S. ___(2017)</t>
+  </si>
+  <si>
+    <t>579 U.S. __ (2016)</t>
+  </si>
+  <si>
+    <t>578 U.S. __ (2016)</t>
+  </si>
+  <si>
+    <t>581 U.S.___(2017)</t>
+  </si>
+  <si>
+    <t>4th Amendent and "knock and announce" rule</t>
+  </si>
+  <si>
+    <t>“May an officer be found liable under the Ninth Circuit’s provocation rule where it is determined that the officer’s use of force was reasonable and not excessive|Does an incident which leads to a reasonable use of force negate a prior Fourth Amendment unlawful entry violation?</t>
+  </si>
+  <si>
+    <t>Provocation rule needs to go</t>
+  </si>
+  <si>
+    <t>Alito;Thomas,Roberts,Kennedy,Ginsburg,Sotomayor,Kagan,Breyer</t>
+  </si>
+  <si>
+    <t>Matal v. Tam</t>
+  </si>
+  <si>
+    <t>582 U.S.___(2017)</t>
+  </si>
+  <si>
+    <t>1st Amendment and disparagement clause of Lanham Act (trademark registration)</t>
+  </si>
+  <si>
+    <t>“Is the Disparagement Clause invalid under the First Amendment?”</t>
+  </si>
+  <si>
+    <t>SCA Hygiene Products Aktiebolag v. First Quality Baby Products, LLC</t>
+  </si>
+  <si>
+    <t>580 U.S.___(2017)</t>
+  </si>
+  <si>
+    <t>Statute of limitations for patent infringement</t>
+  </si>
+  <si>
+    <t>Can the defense of an unreasonable delay in litigation bar claims for patent infringement that are brought within the six-year statutory period of limitations?</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Kennedy,Thomas,Ginsburg,Sotomayor,Kagan</t>
+  </si>
+  <si>
+    <t>Breyer</t>
+  </si>
+  <si>
+    <t>Water Splash v. Menon</t>
+  </si>
+  <si>
+    <t>Hague Service Convention - service of process when party is in foreign country</t>
+  </si>
+  <si>
+    <t>“Does the Hague Service Convention authorize service of process by mail?”</t>
+  </si>
+  <si>
+    <t>structuralism and textualism</t>
+  </si>
+  <si>
+    <t>Alito;Thomas,Roberts,Kennedy,Ginsburg,Breyer,Kagan,Sotomayor</t>
+  </si>
+  <si>
+    <t>Ayestas v. Davis</t>
+  </si>
+  <si>
+    <t>584 U.S. ___(2018)</t>
+  </si>
+  <si>
+    <t>18 U.S.C. § 3599(f)</t>
+  </si>
+  <si>
+    <t>Are investigative services under 18 U.S.C. § 3599(f) only “reasonably necessary” when the habeas petitioner requesting the services can meet the burden of proof for the underlying claim for habeas relief at the time of the request for the investigative services?</t>
+  </si>
+  <si>
+    <t>textualism and pragmatism</t>
+  </si>
+  <si>
+    <t>Janus v. American Federation of State, County &amp;amp; Municipal Employees</t>
+  </si>
+  <si>
+    <t>585 U.S.___(2018)</t>
+  </si>
+  <si>
+    <t>1 st Amendment. Union agency fees – final case in the line to overturn Abood</t>
+  </si>
+  <si>
+    <t>“Should the Court’s decision in Abood v. Detroit Board of Education be overturned so that public employees who do not belong to a union cannot be required to pay a fee to cover the union’s costs to negotiate a contract that applies to all public employees, including those who are not union members?”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doctrinal and pragmatic </t>
+  </si>
+  <si>
+    <t>Alito;Kennedy,Roberts,Thomas,Gorsuch</t>
+  </si>
+  <si>
+    <t>Alito;Thomas,Roberts,Kennedy,Gorsuch</t>
+  </si>
+  <si>
+    <t>Kagan;Breyer,Sotomayor,Ginsburg</t>
+  </si>
+  <si>
+    <t>Murphy v. NCAA</t>
+  </si>
+  <si>
+    <t>The 1992 Professional &amp;amp; Amateur Sports Protection Act (PASPA) 28 U.S.C. §§ 3701-3704, which prohibits state-sanctioned sports gambling|Anti-commandeering doctrine (10th Amendment)</t>
+  </si>
+  <si>
+    <t>“Does a federal statute that prohibits modification or repeal of state-law prohibitions on private conduct impermissibly commandeer the regulatory power of states in contravention of New York v. United States?”</t>
+  </si>
+  <si>
+    <t>Alito;Kagan,Kennedy,Roberts,Gorsuch,Thomas</t>
+  </si>
+  <si>
+    <t>Ginsburg;Sotomayor,Breyer</t>
   </si>
 </sst>
 </file>
@@ -1830,10 +1971,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="9"/>
+      <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2273,6 +2414,9 @@
   <threadedComment ref="G63" dT="2020-07-21T21:03:34.53" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{29BD8916-C473-4AD3-99BD-980DB0A6B111}">
     <text>remanded for further consideration</text>
   </threadedComment>
+  <threadedComment ref="G66" dT="2020-07-23T19:16:11.27" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{E8ECB88B-20FB-427C-BA5A-E55F0CA3A4FE}">
+    <text>yes or no answer?</text>
+  </threadedComment>
   <threadedComment ref="C67" dT="2020-07-21T21:07:50.61" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{E76B42E8-7392-42FF-9D0D-4771AF924F11}">
     <text>Date is off for a case in 2016 term; case was reargued in 2017</text>
   </threadedComment>
@@ -2291,11 +2435,17 @@
   <threadedComment ref="H71" dT="2020-07-21T21:15:28.11" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{72CF621A-23CD-487A-A5C4-F1F5F52BEE03}">
     <text>no reasoning listed</text>
   </threadedComment>
+  <threadedComment ref="H72" dT="2020-07-23T19:22:15.30" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{A4DF1674-26FC-4C25-8DF7-2385D5EAC7EB}">
+    <text>Legislative history at end; higlighted in orange; should i include purposiveism?</text>
+  </threadedComment>
   <threadedComment ref="G73" dT="2020-07-21T21:18:40.67" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{945D29AB-E037-4687-BFF4-24AB13377B9D}">
     <text>"Yes to first, no to questions about merits"</text>
   </threadedComment>
   <threadedComment ref="AF73" dT="2020-07-21T21:20:58.84" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{A8BB29DE-2D6C-43B6-AB81-6C0E7925BF84}">
     <text>pp. 24-25 and 38; didn't code from 24-25</text>
+  </threadedComment>
+  <threadedComment ref="H78" dT="2020-07-23T19:29:31.29" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{A6A15053-58E0-4B97-9B80-191DA346406A}">
+    <text>"Congressional Intent" highlighted in orange; should i include purposeiveism?</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -2304,11 +2454,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060A011E-60FD-5047-91C8-6B9B09AABF05}">
   <dimension ref="A1:AS78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="AT64" sqref="AT64"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
@@ -2357,7 +2507,7 @@
     <col min="45" max="45" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -2494,7 +2644,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2622,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:45" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" ht="65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2747,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:45" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" ht="62" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2872,7 +3022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:45" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" ht="37" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2994,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:45" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" ht="62" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3119,7 +3269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:45" ht="153" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:45" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3242,7 +3392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:45" ht="85" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3364,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3486,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3609,7 +3759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3731,7 +3881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3853,7 +4003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3978,7 +4128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4100,7 +4250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4225,7 +4375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4350,7 +4500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4472,7 +4622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4591,7 +4741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:45" ht="68" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:45" ht="62" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -4714,7 +4864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4839,7 +4989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4967,7 +5117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5092,7 +5242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5217,7 +5367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5342,7 +5492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5467,7 +5617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5583,7 +5733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5708,7 +5858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5833,7 +5983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5955,7 +6105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:45" ht="85" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:45" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -6078,7 +6228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -6203,7 +6353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6326,7 +6476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -6340,16 +6490,16 @@
         <v>2011</v>
       </c>
       <c r="E33" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F33" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="G33" t="s">
         <v>44</v>
       </c>
       <c r="H33" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="K33">
         <v>23</v>
@@ -6361,10 +6511,10 @@
         <v>2</v>
       </c>
       <c r="N33" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Q33" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="R33">
         <v>6</v>
@@ -6445,7 +6595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -6567,30 +6717,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C35" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D35">
         <v>2011</v>
       </c>
       <c r="E35" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F35" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="G35" t="s">
         <v>44</v>
       </c>
       <c r="H35" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="K35">
         <v>15</v>
@@ -6602,10 +6752,10 @@
         <v>2</v>
       </c>
       <c r="N35" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="Q35" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="R35">
         <v>3</v>
@@ -6692,7 +6842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -6817,7 +6967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6942,24 +7092,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C38" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D38">
         <v>2012</v>
       </c>
       <c r="E38" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F38" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="G38" t="s">
         <v>44</v>
@@ -7067,7 +7217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -7081,7 +7231,7 @@
         <v>2012</v>
       </c>
       <c r="E39" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F39" t="s">
         <v>230</v>
@@ -7192,30 +7342,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C40" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D40">
         <v>2012</v>
       </c>
       <c r="E40" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F40" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G40" t="s">
         <v>64</v>
       </c>
       <c r="H40" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="K40">
         <v>20</v>
@@ -7227,10 +7377,10 @@
         <v>1</v>
       </c>
       <c r="N40" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="Q40" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="R40">
         <v>5</v>
@@ -7317,7 +7467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -7445,24 +7595,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C42" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D42">
         <v>2012</v>
       </c>
       <c r="E42" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F42" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G42" t="s">
         <v>44</v>
@@ -7480,13 +7630,13 @@
         <v>1</v>
       </c>
       <c r="N42" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="P42" t="s">
         <v>106</v>
       </c>
       <c r="Q42" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="R42">
         <v>4.5</v>
@@ -7573,7 +7723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -7695,30 +7845,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C44" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D44">
         <v>2013</v>
       </c>
       <c r="E44" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F44" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G44" t="s">
         <v>305</v>
       </c>
       <c r="H44" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="K44">
         <v>11</v>
@@ -7730,7 +7880,7 @@
         <v>0</v>
       </c>
       <c r="N44" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="R44">
         <v>4</v>
@@ -7817,7 +7967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -7942,27 +8092,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C46" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D46">
         <v>2013</v>
       </c>
       <c r="E46" t="s">
+        <v>433</v>
+      </c>
+      <c r="F46" t="s">
+        <v>434</v>
+      </c>
+      <c r="G46" t="s">
         <v>435</v>
-      </c>
-      <c r="F46" t="s">
-        <v>436</v>
-      </c>
-      <c r="G46" t="s">
-        <v>437</v>
       </c>
       <c r="H46" t="s">
         <v>244</v>
@@ -7977,10 +8127,10 @@
         <v>1</v>
       </c>
       <c r="N46" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="Q46" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="R46">
         <v>8</v>
@@ -8067,7 +8217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -8081,7 +8231,7 @@
         <v>2013</v>
       </c>
       <c r="E47" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F47" t="s">
         <v>254</v>
@@ -8189,30 +8339,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C48" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D48">
         <v>2013</v>
       </c>
       <c r="E48" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F48" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="G48" t="s">
         <v>64</v>
       </c>
       <c r="H48" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="K48">
         <v>14</v>
@@ -8311,7 +8461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -8433,24 +8583,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C50" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D50">
         <v>2014</v>
       </c>
       <c r="E50" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F50" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G50" t="s">
         <v>64</v>
@@ -8468,10 +8618,10 @@
         <v>2</v>
       </c>
       <c r="N50" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="Q50" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="R50">
         <v>3</v>
@@ -8558,7 +8708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -8680,30 +8830,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C52" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D52">
         <v>2014</v>
       </c>
       <c r="E52" t="s">
+        <v>450</v>
+      </c>
+      <c r="F52" t="s">
+        <v>451</v>
+      </c>
+      <c r="G52" t="s">
         <v>452</v>
       </c>
-      <c r="F52" t="s">
+      <c r="H52" t="s">
         <v>453</v>
-      </c>
-      <c r="G52" t="s">
-        <v>454</v>
-      </c>
-      <c r="H52" t="s">
-        <v>455</v>
       </c>
       <c r="K52">
         <v>29</v>
@@ -8715,10 +8865,10 @@
         <v>1</v>
       </c>
       <c r="N52" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="Q52" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="R52">
         <v>8</v>
@@ -8805,7 +8955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -8930,30 +9080,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C54" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D54">
         <v>2014</v>
       </c>
       <c r="E54" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F54" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="G54" t="s">
         <v>64</v>
       </c>
       <c r="H54" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="K54">
         <v>15</v>
@@ -9052,7 +9202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -9177,24 +9327,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C56" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D56">
         <v>2014</v>
       </c>
       <c r="E56" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="F56" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G56" t="s">
         <v>44</v>
@@ -9299,7 +9449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -9424,24 +9574,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C58" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D58">
         <v>2015</v>
       </c>
       <c r="E58" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F58" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G58" t="s">
         <v>44</v>
@@ -9459,7 +9609,7 @@
         <v>2</v>
       </c>
       <c r="N58" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="Q58" t="s">
         <v>106</v>
@@ -9549,7 +9699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -9671,30 +9821,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C60" t="s">
-        <v>472</v>
+        <v>486</v>
       </c>
       <c r="D60">
         <v>2015</v>
       </c>
       <c r="E60" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="F60" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="G60" t="s">
         <v>44</v>
       </c>
       <c r="H60" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K60">
         <v>8</v>
@@ -9706,7 +9856,7 @@
         <v>0</v>
       </c>
       <c r="N60" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="R60">
         <v>3.75</v>
@@ -9793,7 +9943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -9916,36 +10066,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C62" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D62">
         <v>2015</v>
       </c>
       <c r="E62" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="F62" t="s">
+        <v>475</v>
+      </c>
+      <c r="G62" t="s">
+        <v>477</v>
+      </c>
+      <c r="H62" t="s">
         <v>478</v>
-      </c>
-      <c r="G62" t="s">
-        <v>480</v>
-      </c>
-      <c r="H62" t="s">
-        <v>481</v>
       </c>
       <c r="K62">
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -9959,7 +10109,7 @@
         <v>2015</v>
       </c>
       <c r="E63" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F63" t="s">
         <v>352</v>
@@ -10068,24 +10218,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C64" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D64">
         <v>2015</v>
       </c>
       <c r="E64" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="F64" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="G64" t="s">
         <v>64</v>
@@ -10103,7 +10253,7 @@
         <v>2</v>
       </c>
       <c r="N64" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="Q64" t="s">
         <v>106</v>
@@ -10193,7 +10343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -10201,16 +10351,16 @@
         <v>356</v>
       </c>
       <c r="C65" t="s">
-        <v>357</v>
+        <v>484</v>
       </c>
       <c r="D65">
         <v>2016</v>
       </c>
       <c r="E65" t="s">
+        <v>357</v>
+      </c>
+      <c r="F65" t="s">
         <v>358</v>
-      </c>
-      <c r="F65" t="s">
-        <v>359</v>
       </c>
       <c r="G65" t="s">
         <v>44</v>
@@ -10228,7 +10378,7 @@
         <v>2</v>
       </c>
       <c r="N65" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="Q65" t="s">
         <v>300</v>
@@ -10318,38 +10468,152 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
+      <c r="B66" t="s">
+        <v>483</v>
+      </c>
+      <c r="C66" t="s">
+        <v>487</v>
+      </c>
       <c r="D66">
         <v>2016</v>
       </c>
+      <c r="E66" t="s">
+        <v>488</v>
+      </c>
+      <c r="F66" t="s">
+        <v>489</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="H66" t="s">
+        <v>237</v>
+      </c>
+      <c r="K66">
+        <v>11</v>
+      </c>
+      <c r="L66" t="s">
+        <v>293</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66" t="s">
+        <v>491</v>
+      </c>
+      <c r="R66">
+        <v>4.75</v>
+      </c>
+      <c r="S66">
+        <v>0</v>
+      </c>
+      <c r="T66">
+        <v>0</v>
+      </c>
+      <c r="U66">
+        <v>0</v>
+      </c>
+      <c r="V66">
+        <v>0</v>
+      </c>
+      <c r="W66">
+        <v>0</v>
+      </c>
+      <c r="X66">
+        <v>0</v>
+      </c>
+      <c r="Y66">
+        <v>5</v>
+      </c>
+      <c r="Z66">
+        <v>38.5</v>
+      </c>
+      <c r="AA66">
+        <v>48</v>
+      </c>
+      <c r="AB66">
+        <v>0</v>
+      </c>
+      <c r="AC66">
+        <v>0</v>
+      </c>
+      <c r="AD66">
+        <v>0</v>
+      </c>
+      <c r="AE66">
+        <v>0</v>
+      </c>
+      <c r="AF66">
+        <v>1</v>
+      </c>
+      <c r="AG66">
+        <v>0</v>
+      </c>
+      <c r="AH66">
+        <v>12</v>
+      </c>
+      <c r="AI66">
+        <v>0</v>
+      </c>
+      <c r="AJ66">
+        <v>0</v>
+      </c>
+      <c r="AK66">
+        <v>0</v>
+      </c>
+      <c r="AL66">
+        <v>0</v>
+      </c>
+      <c r="AM66" t="s">
+        <v>107</v>
+      </c>
+      <c r="AN66">
+        <v>0</v>
+      </c>
+      <c r="AO66">
+        <v>0</v>
+      </c>
+      <c r="AP66">
+        <v>0</v>
+      </c>
+      <c r="AQ66">
+        <v>0</v>
+      </c>
+      <c r="AR66">
+        <v>0</v>
+      </c>
+      <c r="AS66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
+        <v>360</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>361</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>362</v>
       </c>
       <c r="D67">
         <v>2016</v>
       </c>
       <c r="E67" t="s">
+        <v>362</v>
+      </c>
+      <c r="F67" t="s">
         <v>363</v>
-      </c>
-      <c r="F67" t="s">
-        <v>364</v>
       </c>
       <c r="G67" t="s">
         <v>44</v>
       </c>
       <c r="H67" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K67">
         <v>31</v>
@@ -10361,13 +10625,13 @@
         <v>1</v>
       </c>
       <c r="N67" t="s">
+        <v>365</v>
+      </c>
+      <c r="P67" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="P67" s="3" t="s">
+      <c r="Q67" t="s">
         <v>367</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>368</v>
       </c>
       <c r="R67">
         <v>12</v>
@@ -10454,32 +10718,146 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
+      <c r="B68" t="s">
+        <v>492</v>
+      </c>
+      <c r="C68" t="s">
+        <v>493</v>
+      </c>
       <c r="D68">
         <v>2016</v>
       </c>
+      <c r="E68" t="s">
+        <v>494</v>
+      </c>
+      <c r="F68" t="s">
+        <v>495</v>
+      </c>
+      <c r="G68" t="s">
+        <v>64</v>
+      </c>
+      <c r="H68" t="s">
+        <v>346</v>
+      </c>
+      <c r="K68">
+        <v>25</v>
+      </c>
+      <c r="L68" t="s">
+        <v>293</v>
+      </c>
+      <c r="M68">
+        <v>0</v>
+      </c>
+      <c r="N68" t="s">
+        <v>491</v>
+      </c>
+      <c r="R68">
+        <v>8</v>
+      </c>
+      <c r="S68">
+        <v>0</v>
+      </c>
+      <c r="T68">
+        <v>0</v>
+      </c>
+      <c r="U68">
+        <v>0</v>
+      </c>
+      <c r="V68">
+        <v>2</v>
+      </c>
+      <c r="W68">
+        <v>0</v>
+      </c>
+      <c r="X68">
+        <v>0</v>
+      </c>
+      <c r="Y68">
+        <v>4.5</v>
+      </c>
+      <c r="Z68">
+        <v>24</v>
+      </c>
+      <c r="AA68">
+        <v>12</v>
+      </c>
+      <c r="AB68">
+        <v>0</v>
+      </c>
+      <c r="AC68">
+        <v>22</v>
+      </c>
+      <c r="AD68">
+        <v>0</v>
+      </c>
+      <c r="AE68">
+        <v>0</v>
+      </c>
+      <c r="AF68">
+        <v>13</v>
+      </c>
+      <c r="AG68">
+        <v>100</v>
+      </c>
+      <c r="AH68">
+        <v>78</v>
+      </c>
+      <c r="AI68">
+        <v>0</v>
+      </c>
+      <c r="AJ68">
+        <v>0</v>
+      </c>
+      <c r="AK68">
+        <v>0</v>
+      </c>
+      <c r="AL68">
+        <v>33</v>
+      </c>
+      <c r="AM68" t="s">
+        <v>107</v>
+      </c>
+      <c r="AN68">
+        <v>0</v>
+      </c>
+      <c r="AO68">
+        <v>0</v>
+      </c>
+      <c r="AP68">
+        <v>0</v>
+      </c>
+      <c r="AQ68">
+        <v>0</v>
+      </c>
+      <c r="AR68">
+        <v>0</v>
+      </c>
+      <c r="AS68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>368</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>369</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>370</v>
       </c>
       <c r="D69">
         <v>2016</v>
       </c>
       <c r="E69" t="s">
+        <v>373</v>
+      </c>
+      <c r="F69" t="s">
         <v>374</v>
-      </c>
-      <c r="F69" t="s">
-        <v>375</v>
       </c>
       <c r="G69" t="s">
         <v>64</v>
@@ -10497,7 +10875,7 @@
         <v>0</v>
       </c>
       <c r="N69" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="R69">
         <v>7.5</v>
@@ -10584,32 +10962,149 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
+      <c r="B70" t="s">
+        <v>496</v>
+      </c>
+      <c r="C70" t="s">
+        <v>497</v>
+      </c>
       <c r="D70">
         <v>2016</v>
       </c>
+      <c r="E70" t="s">
+        <v>498</v>
+      </c>
+      <c r="F70" t="s">
+        <v>499</v>
+      </c>
+      <c r="G70" t="s">
+        <v>64</v>
+      </c>
+      <c r="H70" t="s">
+        <v>243</v>
+      </c>
+      <c r="K70">
+        <v>16</v>
+      </c>
+      <c r="L70" t="s">
+        <v>270</v>
+      </c>
+      <c r="M70">
+        <v>2</v>
+      </c>
+      <c r="N70" t="s">
+        <v>500</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>501</v>
+      </c>
+      <c r="R70">
+        <v>4.5</v>
+      </c>
+      <c r="S70">
+        <v>13</v>
+      </c>
+      <c r="T70">
+        <v>0</v>
+      </c>
+      <c r="U70">
+        <v>0</v>
+      </c>
+      <c r="V70">
+        <v>23</v>
+      </c>
+      <c r="W70">
+        <v>0</v>
+      </c>
+      <c r="X70">
+        <v>0</v>
+      </c>
+      <c r="Y70">
+        <v>1</v>
+      </c>
+      <c r="Z70">
+        <v>15</v>
+      </c>
+      <c r="AA70">
+        <v>0</v>
+      </c>
+      <c r="AB70">
+        <v>0</v>
+      </c>
+      <c r="AC70">
+        <v>12</v>
+      </c>
+      <c r="AD70">
+        <v>0</v>
+      </c>
+      <c r="AE70">
+        <v>0</v>
+      </c>
+      <c r="AF70">
+        <v>10</v>
+      </c>
+      <c r="AG70">
+        <v>74</v>
+      </c>
+      <c r="AH70">
+        <v>32</v>
+      </c>
+      <c r="AI70">
+        <v>0</v>
+      </c>
+      <c r="AJ70">
+        <v>27</v>
+      </c>
+      <c r="AK70">
+        <v>9</v>
+      </c>
+      <c r="AL70">
+        <v>3</v>
+      </c>
+      <c r="AM70">
+        <v>0</v>
+      </c>
+      <c r="AN70">
+        <v>0</v>
+      </c>
+      <c r="AO70">
+        <v>0</v>
+      </c>
+      <c r="AP70">
+        <v>0</v>
+      </c>
+      <c r="AQ70">
+        <v>0</v>
+      </c>
+      <c r="AR70">
+        <v>0</v>
+      </c>
+      <c r="AS70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
+        <v>376</v>
+      </c>
+      <c r="C71" t="s">
         <v>377</v>
-      </c>
-      <c r="C71" t="s">
-        <v>378</v>
       </c>
       <c r="D71">
         <v>2016</v>
       </c>
       <c r="E71" t="s">
+        <v>378</v>
+      </c>
+      <c r="F71" t="s">
         <v>379</v>
-      </c>
-      <c r="F71" t="s">
-        <v>380</v>
       </c>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
@@ -10623,7 +11118,7 @@
         <v>0</v>
       </c>
       <c r="N71" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="R71">
         <v>3.5</v>
@@ -10710,32 +11205,146 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
+      <c r="B72" t="s">
+        <v>502</v>
+      </c>
+      <c r="C72" t="s">
+        <v>377</v>
+      </c>
       <c r="D72">
         <v>2016</v>
       </c>
+      <c r="E72" t="s">
+        <v>503</v>
+      </c>
+      <c r="F72" t="s">
+        <v>504</v>
+      </c>
+      <c r="G72" t="s">
+        <v>64</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="K72">
+        <v>12</v>
+      </c>
+      <c r="L72" t="s">
+        <v>293</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72" t="s">
+        <v>506</v>
+      </c>
+      <c r="R72">
+        <v>3</v>
+      </c>
+      <c r="S72">
+        <v>0</v>
+      </c>
+      <c r="T72">
+        <v>0</v>
+      </c>
+      <c r="U72">
+        <v>0</v>
+      </c>
+      <c r="V72">
+        <v>0</v>
+      </c>
+      <c r="W72">
+        <v>0</v>
+      </c>
+      <c r="X72">
+        <v>0</v>
+      </c>
+      <c r="Y72">
+        <v>8</v>
+      </c>
+      <c r="Z72">
+        <v>41.5</v>
+      </c>
+      <c r="AA72">
+        <v>0</v>
+      </c>
+      <c r="AB72">
+        <v>0</v>
+      </c>
+      <c r="AC72">
+        <v>16</v>
+      </c>
+      <c r="AD72">
+        <v>29</v>
+      </c>
+      <c r="AE72">
+        <v>14.5</v>
+      </c>
+      <c r="AF72">
+        <v>3</v>
+      </c>
+      <c r="AG72">
+        <v>4</v>
+      </c>
+      <c r="AH72">
+        <v>0</v>
+      </c>
+      <c r="AI72">
+        <v>0</v>
+      </c>
+      <c r="AJ72">
+        <v>4</v>
+      </c>
+      <c r="AK72">
+        <v>12.5</v>
+      </c>
+      <c r="AL72">
+        <v>33.5</v>
+      </c>
+      <c r="AM72" t="s">
+        <v>107</v>
+      </c>
+      <c r="AN72">
+        <v>0</v>
+      </c>
+      <c r="AO72">
+        <v>0</v>
+      </c>
+      <c r="AP72">
+        <v>0</v>
+      </c>
+      <c r="AQ72">
+        <v>0</v>
+      </c>
+      <c r="AR72">
+        <v>0</v>
+      </c>
+      <c r="AS72">
+        <v>0</v>
+      </c>
     </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>381</v>
+      </c>
+      <c r="C73" t="s">
         <v>382</v>
-      </c>
-      <c r="C73" t="s">
-        <v>383</v>
       </c>
       <c r="D73">
         <v>2017</v>
       </c>
       <c r="E73" t="s">
+        <v>383</v>
+      </c>
+      <c r="F73" t="s">
         <v>384</v>
-      </c>
-      <c r="F73" t="s">
-        <v>385</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>44</v>
@@ -10753,13 +11362,13 @@
         <v>1</v>
       </c>
       <c r="N73" t="s">
+        <v>517</v>
+      </c>
+      <c r="P73" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q73" t="s">
         <v>386</v>
-      </c>
-      <c r="P73" t="s">
-        <v>387</v>
-      </c>
-      <c r="Q73" t="s">
-        <v>388</v>
       </c>
       <c r="R73">
         <v>20</v>
@@ -10844,38 +11453,152 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
+      <c r="B74" t="s">
+        <v>507</v>
+      </c>
+      <c r="C74" t="s">
+        <v>508</v>
+      </c>
       <c r="D74">
         <v>2017</v>
       </c>
+      <c r="E74" t="s">
+        <v>509</v>
+      </c>
+      <c r="F74" t="s">
+        <v>510</v>
+      </c>
+      <c r="G74" t="s">
+        <v>64</v>
+      </c>
+      <c r="H74" t="s">
+        <v>511</v>
+      </c>
+      <c r="K74">
+        <v>19</v>
+      </c>
+      <c r="L74" t="s">
+        <v>70</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74" t="s">
+        <v>380</v>
+      </c>
+      <c r="R74">
+        <v>14</v>
+      </c>
+      <c r="S74">
+        <v>16</v>
+      </c>
+      <c r="T74">
+        <v>48</v>
+      </c>
+      <c r="U74">
+        <v>0</v>
+      </c>
+      <c r="V74">
+        <v>6</v>
+      </c>
+      <c r="W74">
+        <v>0</v>
+      </c>
+      <c r="X74">
+        <v>12</v>
+      </c>
+      <c r="Y74">
+        <v>5</v>
+      </c>
+      <c r="Z74">
+        <v>11</v>
+      </c>
+      <c r="AA74">
+        <v>39</v>
+      </c>
+      <c r="AB74">
+        <v>0</v>
+      </c>
+      <c r="AC74">
+        <v>11</v>
+      </c>
+      <c r="AD74">
+        <v>0</v>
+      </c>
+      <c r="AE74">
+        <v>51</v>
+      </c>
+      <c r="AF74">
+        <v>0</v>
+      </c>
+      <c r="AG74">
+        <v>0</v>
+      </c>
+      <c r="AH74">
+        <v>0</v>
+      </c>
+      <c r="AI74">
+        <v>0</v>
+      </c>
+      <c r="AJ74">
+        <v>0</v>
+      </c>
+      <c r="AK74">
+        <v>0</v>
+      </c>
+      <c r="AL74">
+        <v>0</v>
+      </c>
+      <c r="AM74">
+        <v>0</v>
+      </c>
+      <c r="AN74">
+        <v>0</v>
+      </c>
+      <c r="AO74">
+        <v>0</v>
+      </c>
+      <c r="AP74">
+        <v>0</v>
+      </c>
+      <c r="AQ74">
+        <v>0</v>
+      </c>
+      <c r="AR74">
+        <v>0</v>
+      </c>
+      <c r="AS74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="75" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C75" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D75">
         <v>2017</v>
       </c>
       <c r="E75" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F75" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G75" t="s">
         <v>64</v>
       </c>
       <c r="H75" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K75">
         <v>21</v>
@@ -10887,7 +11610,7 @@
         <v>1</v>
       </c>
       <c r="N75" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="Q75" t="s">
         <v>153</v>
@@ -10977,38 +11700,155 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
+      <c r="B76" t="s">
+        <v>512</v>
+      </c>
+      <c r="C76" t="s">
+        <v>513</v>
+      </c>
       <c r="D76">
         <v>2017</v>
       </c>
+      <c r="E76" t="s">
+        <v>514</v>
+      </c>
+      <c r="F76" t="s">
+        <v>515</v>
+      </c>
+      <c r="G76" t="s">
+        <v>64</v>
+      </c>
+      <c r="H76" t="s">
+        <v>516</v>
+      </c>
+      <c r="K76">
+        <v>48</v>
+      </c>
+      <c r="L76" t="s">
+        <v>48</v>
+      </c>
+      <c r="M76">
+        <v>1</v>
+      </c>
+      <c r="N76" t="s">
+        <v>518</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>519</v>
+      </c>
+      <c r="R76">
+        <v>4</v>
+      </c>
+      <c r="S76">
+        <v>0</v>
+      </c>
+      <c r="T76">
+        <v>0</v>
+      </c>
+      <c r="U76">
+        <v>0</v>
+      </c>
+      <c r="V76">
+        <v>0</v>
+      </c>
+      <c r="W76">
+        <v>0</v>
+      </c>
+      <c r="X76">
+        <v>0</v>
+      </c>
+      <c r="Y76">
+        <v>16</v>
+      </c>
+      <c r="Z76">
+        <v>130</v>
+      </c>
+      <c r="AA76">
+        <v>105</v>
+      </c>
+      <c r="AB76">
+        <v>0</v>
+      </c>
+      <c r="AC76">
+        <v>29.5</v>
+      </c>
+      <c r="AD76">
+        <v>0</v>
+      </c>
+      <c r="AE76">
+        <v>0</v>
+      </c>
+      <c r="AF76">
+        <v>25</v>
+      </c>
+      <c r="AG76">
+        <v>129</v>
+      </c>
+      <c r="AH76">
+        <v>266</v>
+      </c>
+      <c r="AI76">
+        <v>41</v>
+      </c>
+      <c r="AJ76">
+        <v>3</v>
+      </c>
+      <c r="AK76">
+        <v>0</v>
+      </c>
+      <c r="AL76">
+        <v>0</v>
+      </c>
+      <c r="AM76" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN76">
+        <v>0</v>
+      </c>
+      <c r="AO76">
+        <v>0</v>
+      </c>
+      <c r="AP76">
+        <v>0</v>
+      </c>
+      <c r="AQ76">
+        <v>0</v>
+      </c>
+      <c r="AR76">
+        <v>0</v>
+      </c>
+      <c r="AS76">
+        <v>0</v>
+      </c>
     </row>
-    <row r="77" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C77" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D77">
         <v>2017</v>
       </c>
       <c r="E77" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F77" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="G77" t="s">
         <v>44</v>
       </c>
       <c r="H77" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="K77">
         <v>7</v>
@@ -11020,7 +11860,7 @@
         <v>0</v>
       </c>
       <c r="N77" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="R77">
         <v>3</v>
@@ -11107,12 +11947,129 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
+      <c r="B78" t="s">
+        <v>520</v>
+      </c>
+      <c r="C78" t="s">
+        <v>508</v>
+      </c>
       <c r="D78">
         <v>2017</v>
+      </c>
+      <c r="E78" t="s">
+        <v>521</v>
+      </c>
+      <c r="F78" t="s">
+        <v>522</v>
+      </c>
+      <c r="G78" t="s">
+        <v>64</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="K78">
+        <v>30</v>
+      </c>
+      <c r="L78" t="s">
+        <v>160</v>
+      </c>
+      <c r="M78">
+        <v>2</v>
+      </c>
+      <c r="N78" t="s">
+        <v>523</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>524</v>
+      </c>
+      <c r="R78">
+        <v>11</v>
+      </c>
+      <c r="S78">
+        <v>0</v>
+      </c>
+      <c r="T78">
+        <v>0</v>
+      </c>
+      <c r="U78">
+        <v>0</v>
+      </c>
+      <c r="V78">
+        <v>0</v>
+      </c>
+      <c r="W78">
+        <v>0</v>
+      </c>
+      <c r="X78">
+        <v>0</v>
+      </c>
+      <c r="Y78">
+        <v>11</v>
+      </c>
+      <c r="Z78">
+        <v>39</v>
+      </c>
+      <c r="AA78">
+        <v>46</v>
+      </c>
+      <c r="AB78">
+        <v>0</v>
+      </c>
+      <c r="AC78">
+        <v>129.5</v>
+      </c>
+      <c r="AD78">
+        <v>29</v>
+      </c>
+      <c r="AE78">
+        <v>17.5</v>
+      </c>
+      <c r="AF78">
+        <v>8</v>
+      </c>
+      <c r="AG78">
+        <v>122.5</v>
+      </c>
+      <c r="AH78">
+        <v>107.5</v>
+      </c>
+      <c r="AI78">
+        <v>0</v>
+      </c>
+      <c r="AJ78">
+        <v>8</v>
+      </c>
+      <c r="AK78">
+        <v>0</v>
+      </c>
+      <c r="AL78">
+        <v>7</v>
+      </c>
+      <c r="AM78">
+        <v>0.5</v>
+      </c>
+      <c r="AN78">
+        <v>0</v>
+      </c>
+      <c r="AO78">
+        <v>0</v>
+      </c>
+      <c r="AP78">
+        <v>0</v>
+      </c>
+      <c r="AQ78">
+        <v>7</v>
+      </c>
+      <c r="AR78">
+        <v>0</v>
+      </c>
+      <c r="AS78">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
woohoo we did it
</commit_message>
<xml_diff>
--- a/AlitoDataset.xlsx
+++ b/AlitoDataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jtsanz\alito-research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineparnell/alito-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3E6667-1E01-4362-89D6-A11B912BE922}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0C4FA8-D1FD-294F-97BB-F16F108BB1FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1330" windowWidth="14400" windowHeight="7360" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,8 +47,6 @@
     <author>tc={0F4748BD-5B03-439A-B8A7-8872FFB421BA}</author>
     <author>tc={2810AD96-B8B6-4798-A014-AFDE2C354919}</author>
     <author>tc={3A0F3EBF-F4B9-214C-9AA5-DBFCC7D44035}</author>
-    <author>tc={915C01E3-6C9F-0E49-9FDE-186D12E45115}</author>
-    <author>tc={85C62DE5-A215-7844-ADDB-F6A767BB5222}</author>
     <author>tc={3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}</author>
     <author>tc={A1A2FE14-15BB-E544-93B0-765E82F8CD8A}</author>
     <author>tc={93985E51-4186-401D-B292-10D9DC17CEB8}</author>
@@ -170,23 +168,7 @@
     There are three different ones?</t>
       </text>
     </comment>
-    <comment ref="AM10" authorId="12" shapeId="0" xr:uid="{915C01E3-6C9F-0E49-9FDE-186D12E45115}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    6 lines</t>
-      </text>
-    </comment>
-    <comment ref="AM14" authorId="13" shapeId="0" xr:uid="{85C62DE5-A215-7844-ADDB-F6A767BB5222}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    5 lines</t>
-      </text>
-    </comment>
-    <comment ref="A19" authorId="14" shapeId="0" xr:uid="{3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}">
+    <comment ref="A19" authorId="12" shapeId="0" xr:uid="{3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -194,7 +176,7 @@
     missing lengths on a lot of sections, but have line count highlights</t>
       </text>
     </comment>
-    <comment ref="Y19" authorId="15" shapeId="0" xr:uid="{A1A2FE14-15BB-E544-93B0-765E82F8CD8A}">
+    <comment ref="Y19" authorId="13" shapeId="0" xr:uid="{A1A2FE14-15BB-E544-93B0-765E82F8CD8A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -202,7 +184,7 @@
     no length provided</t>
       </text>
     </comment>
-    <comment ref="M23" authorId="16" shapeId="0" xr:uid="{93985E51-4186-401D-B292-10D9DC17CEB8}">
+    <comment ref="M23" authorId="14" shapeId="0" xr:uid="{93985E51-4186-401D-B292-10D9DC17CEB8}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -210,7 +192,7 @@
     it's 5-3, is this contentious or ambigious? haha</t>
       </text>
     </comment>
-    <comment ref="G30" authorId="17" shapeId="0" xr:uid="{916A852D-1D9C-43FD-9526-91B03FAC048E}">
+    <comment ref="G30" authorId="15" shapeId="0" xr:uid="{916A852D-1D9C-43FD-9526-91B03FAC048E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -218,7 +200,7 @@
     Not sure what to put as the answer here: "Pharmaceutical sales reps are outside salesmen"</t>
       </text>
     </comment>
-    <comment ref="Y32" authorId="18" shapeId="0" xr:uid="{191E2626-B001-4B9D-95BB-3DFE681133E5}">
+    <comment ref="Y32" authorId="16" shapeId="0" xr:uid="{191E2626-B001-4B9D-95BB-3DFE681133E5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -226,7 +208,7 @@
     Howes v Fields, no MA length given</t>
       </text>
     </comment>
-    <comment ref="A36" authorId="19" shapeId="0" xr:uid="{A4DC1BA9-4A23-4C06-A9DF-A3D4F083B19B}">
+    <comment ref="A36" authorId="17" shapeId="0" xr:uid="{A4DC1BA9-4A23-4C06-A9DF-A3D4F083B19B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -234,7 +216,7 @@
     accidentally got out of order, my b haha</t>
       </text>
     </comment>
-    <comment ref="C51" authorId="20" shapeId="0" xr:uid="{B21FA207-DD6C-4EC4-AA1E-647AEEC95CBA}">
+    <comment ref="C51" authorId="18" shapeId="0" xr:uid="{B21FA207-DD6C-4EC4-AA1E-647AEEC95CBA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -242,7 +224,7 @@
     No citation, just underlines :(</t>
       </text>
     </comment>
-    <comment ref="G61" authorId="21" shapeId="0" xr:uid="{EDBFDAAD-D50D-473D-8856-A184FE763FEC}">
+    <comment ref="G61" authorId="19" shapeId="0" xr:uid="{EDBFDAAD-D50D-473D-8856-A184FE763FEC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -250,7 +232,7 @@
     not a direct answer to the QP; victims of a conspiracy can also be perpetrators of one.</t>
       </text>
     </comment>
-    <comment ref="M61" authorId="22" shapeId="0" xr:uid="{F5907484-1F67-418A-8263-E2E9C18888C5}">
+    <comment ref="M61" authorId="20" shapeId="0" xr:uid="{F5907484-1F67-418A-8263-E2E9C18888C5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -258,7 +240,7 @@
     Scalia's seat empty, so contentious?</t>
       </text>
     </comment>
-    <comment ref="B62" authorId="23" shapeId="0" xr:uid="{172A06DA-0462-7942-A104-EFAF337D8F7F}">
+    <comment ref="B62" authorId="21" shapeId="0" xr:uid="{172A06DA-0462-7942-A104-EFAF337D8F7F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -266,7 +248,7 @@
     There is so much going on idk what to do</t>
       </text>
     </comment>
-    <comment ref="G63" authorId="24" shapeId="0" xr:uid="{29BD8916-C473-4AD3-99BD-980DB0A6B111}">
+    <comment ref="G63" authorId="22" shapeId="0" xr:uid="{29BD8916-C473-4AD3-99BD-980DB0A6B111}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -274,7 +256,7 @@
     remanded for further consideration</t>
       </text>
     </comment>
-    <comment ref="G66" authorId="25" shapeId="0" xr:uid="{E8ECB88B-20FB-427C-BA5A-E55F0CA3A4FE}">
+    <comment ref="G66" authorId="23" shapeId="0" xr:uid="{E8ECB88B-20FB-427C-BA5A-E55F0CA3A4FE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -282,7 +264,7 @@
     yes or no answer?</t>
       </text>
     </comment>
-    <comment ref="C67" authorId="26" shapeId="0" xr:uid="{E76B42E8-7392-42FF-9D0D-4771AF924F11}">
+    <comment ref="C67" authorId="24" shapeId="0" xr:uid="{E76B42E8-7392-42FF-9D0D-4771AF924F11}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -290,7 +272,7 @@
     Date is off for a case in 2016 term; case was reargued in 2017</t>
       </text>
     </comment>
-    <comment ref="P67" authorId="27" shapeId="0" xr:uid="{72089604-F3E5-43FD-BB29-19F63B5D3451}">
+    <comment ref="P67" authorId="25" shapeId="0" xr:uid="{72089604-F3E5-43FD-BB29-19F63B5D3451}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -300,7 +282,7 @@
     ???</t>
       </text>
     </comment>
-    <comment ref="C69" authorId="28" shapeId="0" xr:uid="{332B7A30-BB9D-49DC-BFB2-C0D3DF1392D4}">
+    <comment ref="C69" authorId="26" shapeId="0" xr:uid="{332B7A30-BB9D-49DC-BFB2-C0D3DF1392D4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -308,7 +290,7 @@
     Should this be 2016? Is this correct?</t>
       </text>
     </comment>
-    <comment ref="G71" authorId="29" shapeId="0" xr:uid="{007B5D8A-F2ED-4913-B91D-14040B184733}">
+    <comment ref="G71" authorId="27" shapeId="0" xr:uid="{007B5D8A-F2ED-4913-B91D-14040B184733}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -316,7 +298,7 @@
     No answer listed?</t>
       </text>
     </comment>
-    <comment ref="H71" authorId="30" shapeId="0" xr:uid="{72CF621A-23CD-487A-A5C4-F1F5F52BEE03}">
+    <comment ref="H71" authorId="28" shapeId="0" xr:uid="{72CF621A-23CD-487A-A5C4-F1F5F52BEE03}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -324,7 +306,7 @@
     no reasoning listed</t>
       </text>
     </comment>
-    <comment ref="H72" authorId="31" shapeId="0" xr:uid="{A4DF1674-26FC-4C25-8DF7-2385D5EAC7EB}">
+    <comment ref="H72" authorId="29" shapeId="0" xr:uid="{A4DF1674-26FC-4C25-8DF7-2385D5EAC7EB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -332,7 +314,7 @@
     Legislative history at end; higlighted in orange; should i include purposiveism?</t>
       </text>
     </comment>
-    <comment ref="G73" authorId="32" shapeId="0" xr:uid="{945D29AB-E037-4687-BFF4-24AB13377B9D}">
+    <comment ref="G73" authorId="30" shapeId="0" xr:uid="{945D29AB-E037-4687-BFF4-24AB13377B9D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -340,7 +322,7 @@
     "Yes to first, no to questions about merits"</t>
       </text>
     </comment>
-    <comment ref="AF73" authorId="33" shapeId="0" xr:uid="{A8BB29DE-2D6C-43B6-AB81-6C0E7925BF84}">
+    <comment ref="AF73" authorId="31" shapeId="0" xr:uid="{A8BB29DE-2D6C-43B6-AB81-6C0E7925BF84}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -348,7 +330,7 @@
     pp. 24-25 and 38; didn't code from 24-25</t>
       </text>
     </comment>
-    <comment ref="H78" authorId="34" shapeId="0" xr:uid="{A6A15053-58E0-4B97-9B80-191DA346406A}">
+    <comment ref="H78" authorId="32" shapeId="0" xr:uid="{A6A15053-58E0-4B97-9B80-191DA346406A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -361,7 +343,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="522">
   <si>
     <t>Case Name</t>
   </si>
@@ -1216,15 +1198,6 @@
     <t>Roberts;Thomas,Ginsburg,Sotomayor</t>
   </si>
   <si>
-    <t>4 lines</t>
-  </si>
-  <si>
-    <t>5 lines</t>
-  </si>
-  <si>
-    <t>6 lines</t>
-  </si>
-  <si>
     <t>Davis v. United States</t>
   </si>
   <si>
@@ -1955,7 +1928,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1969,12 +1942,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2375,12 +2342,6 @@
   <threadedComment ref="F10" dT="2020-07-17T13:39:40.63" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{3A0F3EBF-F4B9-214C-9AA5-DBFCC7D44035}">
     <text>There are three different ones?</text>
   </threadedComment>
-  <threadedComment ref="AM10" dT="2020-07-17T13:45:40.48" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{915C01E3-6C9F-0E49-9FDE-186D12E45115}">
-    <text>6 lines</text>
-  </threadedComment>
-  <threadedComment ref="AM14" dT="2020-07-17T14:06:17.88" personId="{536D3E69-A7F7-6641-BE07-967F7E1D3B0A}" id="{85C62DE5-A215-7844-ADDB-F6A767BB5222}">
-    <text>5 lines</text>
-  </threadedComment>
   <threadedComment ref="A19" dT="2020-07-05T08:06:57.89" personId="{16B5576D-7CA9-4572-8E89-80998E37D5E9}" id="{3F4679BA-84FF-4A7E-AC1E-793CB3E61C6C}">
     <text>missing lengths on a lot of sections, but have line count highlights</text>
   </threadedComment>
@@ -2454,29 +2415,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060A011E-60FD-5047-91C8-6B9B09AABF05}">
   <dimension ref="A1:AS78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AN24" sqref="AN24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="79" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="164" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="72.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="66.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.5" bestFit="1" customWidth="1"/>
@@ -2507,7 +2468,7 @@
     <col min="45" max="45" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -2644,7 +2605,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:45" ht="51" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2772,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:45" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:45" ht="65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2897,7 +2858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:45" ht="62" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:45" ht="68" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3022,7 +2983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:45" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:45" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3144,7 +3105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:45" ht="62" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:45" ht="68" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3269,7 +3230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:45" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:45" ht="153" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3392,7 +3353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:45" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:45" ht="85" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3514,7 +3475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3636,7 +3597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3737,8 +3698,8 @@
       <c r="AL10">
         <v>14.5</v>
       </c>
-      <c r="AM10" s="3" t="s">
-        <v>282</v>
+      <c r="AM10" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="AN10">
         <v>0</v>
@@ -3759,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3881,7 +3842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4003,7 +3964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4128,7 +4089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4228,8 +4189,8 @@
       <c r="AL14">
         <v>0</v>
       </c>
-      <c r="AM14" s="3" t="s">
-        <v>281</v>
+      <c r="AM14" s="8" t="s">
+        <v>232</v>
       </c>
       <c r="AN14">
         <v>0</v>
@@ -4250,7 +4211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4375,7 +4336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4500,7 +4461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4622,7 +4583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4741,7 +4702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:45" ht="62" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:45" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -4864,7 +4825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4989,7 +4950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5117,7 +5078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5221,7 +5182,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>280</v>
+        <v>85</v>
       </c>
       <c r="AN22">
         <v>0</v>
@@ -5242,7 +5203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5367,15 +5328,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C24" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D24">
         <v>2010</v>
@@ -5384,7 +5345,7 @@
         <v>138</v>
       </c>
       <c r="F24" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G24" t="s">
         <v>64</v>
@@ -5402,10 +5363,10 @@
         <v>2</v>
       </c>
       <c r="N24" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="Q24" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="R24">
         <v>8.5</v>
@@ -5492,7 +5453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5617,42 +5578,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C26" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D26">
         <v>2010</v>
       </c>
       <c r="E26" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F26" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G26" t="s">
         <v>64</v>
       </c>
       <c r="H26" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="K26">
         <v>13</v>
       </c>
       <c r="L26" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="M26">
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="R26">
         <v>4</v>
@@ -5733,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5858,24 +5819,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C28" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D28">
         <v>2010</v>
       </c>
       <c r="E28" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F28" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G28" t="s">
         <v>64</v>
@@ -5893,10 +5854,10 @@
         <v>2</v>
       </c>
       <c r="N28" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="Q28" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="R28">
         <v>5</v>
@@ -5983,7 +5944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -6105,7 +6066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:45" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:45" ht="85" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -6228,30 +6189,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C31" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D31">
         <v>2011</v>
       </c>
       <c r="E31" t="s">
+        <v>300</v>
+      </c>
+      <c r="F31" t="s">
+        <v>301</v>
+      </c>
+      <c r="G31" t="s">
+        <v>302</v>
+      </c>
+      <c r="H31" t="s">
         <v>303</v>
-      </c>
-      <c r="F31" t="s">
-        <v>304</v>
-      </c>
-      <c r="G31" t="s">
-        <v>305</v>
-      </c>
-      <c r="H31" t="s">
-        <v>306</v>
       </c>
       <c r="K31">
         <v>25</v>
@@ -6263,7 +6224,7 @@
         <v>2</v>
       </c>
       <c r="N31" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="Q31" t="s">
         <v>162</v>
@@ -6353,7 +6314,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6476,30 +6437,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C33" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D33">
         <v>2011</v>
       </c>
       <c r="E33" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F33" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="G33" t="s">
         <v>44</v>
       </c>
       <c r="H33" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="K33">
         <v>23</v>
@@ -6511,10 +6472,10 @@
         <v>2</v>
       </c>
       <c r="N33" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="Q33" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="R33">
         <v>6</v>
@@ -6595,7 +6556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -6717,30 +6678,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C35" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D35">
         <v>2011</v>
       </c>
       <c r="E35" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F35" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="G35" t="s">
         <v>44</v>
       </c>
       <c r="H35" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="K35">
         <v>15</v>
@@ -6752,10 +6713,10 @@
         <v>2</v>
       </c>
       <c r="N35" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="Q35" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="R35">
         <v>3</v>
@@ -6842,7 +6803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -6967,7 +6928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -7092,30 +7053,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C38" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D38">
         <v>2012</v>
       </c>
       <c r="E38" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F38" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="G38" t="s">
         <v>44</v>
       </c>
       <c r="H38" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="K38">
         <v>24</v>
@@ -7217,7 +7178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -7231,7 +7192,7 @@
         <v>2012</v>
       </c>
       <c r="E39" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F39" t="s">
         <v>230</v>
@@ -7342,30 +7303,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C40" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D40">
         <v>2012</v>
       </c>
       <c r="E40" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="F40" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G40" t="s">
         <v>64</v>
       </c>
       <c r="H40" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="K40">
         <v>20</v>
@@ -7377,10 +7338,10 @@
         <v>1</v>
       </c>
       <c r="N40" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="Q40" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="R40">
         <v>5</v>
@@ -7467,7 +7428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -7595,24 +7556,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C42" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D42">
         <v>2012</v>
       </c>
       <c r="E42" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="F42" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="G42" t="s">
         <v>44</v>
@@ -7630,13 +7591,13 @@
         <v>1</v>
       </c>
       <c r="N42" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="P42" t="s">
         <v>106</v>
       </c>
       <c r="Q42" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="R42">
         <v>4.5</v>
@@ -7723,7 +7684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -7845,30 +7806,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C44" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D44">
         <v>2013</v>
       </c>
       <c r="E44" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F44" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G44" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H44" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="K44">
         <v>11</v>
@@ -7880,7 +7841,7 @@
         <v>0</v>
       </c>
       <c r="N44" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="R44">
         <v>4</v>
@@ -7967,7 +7928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -8092,27 +8053,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C46" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D46">
         <v>2013</v>
       </c>
       <c r="E46" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="F46" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="G46" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H46" t="s">
         <v>244</v>
@@ -8127,10 +8088,10 @@
         <v>1</v>
       </c>
       <c r="N46" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="Q46" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="R46">
         <v>8</v>
@@ -8217,7 +8178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -8231,7 +8192,7 @@
         <v>2013</v>
       </c>
       <c r="E47" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F47" t="s">
         <v>254</v>
@@ -8339,30 +8300,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C48" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D48">
         <v>2013</v>
       </c>
       <c r="E48" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F48" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="G48" t="s">
         <v>64</v>
       </c>
       <c r="H48" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="K48">
         <v>14</v>
@@ -8461,7 +8422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -8583,24 +8544,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C50" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D50">
         <v>2014</v>
       </c>
       <c r="E50" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="F50" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G50" t="s">
         <v>64</v>
@@ -8618,10 +8579,10 @@
         <v>2</v>
       </c>
       <c r="N50" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="Q50" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="R50">
         <v>3</v>
@@ -8708,30 +8669,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D51">
         <v>2014</v>
       </c>
       <c r="E51" t="s">
+        <v>309</v>
+      </c>
+      <c r="F51" t="s">
+        <v>310</v>
+      </c>
+      <c r="G51" t="s">
+        <v>311</v>
+      </c>
+      <c r="H51" t="s">
         <v>312</v>
-      </c>
-      <c r="F51" t="s">
-        <v>313</v>
-      </c>
-      <c r="G51" t="s">
-        <v>314</v>
-      </c>
-      <c r="H51" t="s">
-        <v>315</v>
       </c>
       <c r="K51">
         <v>13</v>
@@ -8743,7 +8704,7 @@
         <v>0</v>
       </c>
       <c r="N51" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R51">
         <v>5</v>
@@ -8830,30 +8791,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C52" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D52">
         <v>2014</v>
       </c>
       <c r="E52" t="s">
+        <v>447</v>
+      </c>
+      <c r="F52" t="s">
+        <v>448</v>
+      </c>
+      <c r="G52" t="s">
+        <v>449</v>
+      </c>
+      <c r="H52" t="s">
         <v>450</v>
-      </c>
-      <c r="F52" t="s">
-        <v>451</v>
-      </c>
-      <c r="G52" t="s">
-        <v>452</v>
-      </c>
-      <c r="H52" t="s">
-        <v>453</v>
       </c>
       <c r="K52">
         <v>29</v>
@@ -8865,10 +8826,10 @@
         <v>1</v>
       </c>
       <c r="N52" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="Q52" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="R52">
         <v>8</v>
@@ -8955,30 +8916,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C53" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D53">
         <v>2014</v>
       </c>
       <c r="E53" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F53" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G53" t="s">
         <v>44</v>
       </c>
       <c r="H53" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="K53">
         <v>29</v>
@@ -8993,7 +8954,7 @@
         <v>59</v>
       </c>
       <c r="Q53" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R53">
         <v>8.5</v>
@@ -9059,7 +9020,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="AN53">
         <v>0</v>
@@ -9080,30 +9041,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C54" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D54">
         <v>2014</v>
       </c>
       <c r="E54" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="F54" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="G54" t="s">
         <v>64</v>
       </c>
       <c r="H54" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="K54">
         <v>15</v>
@@ -9115,7 +9076,7 @@
         <v>0</v>
       </c>
       <c r="N54" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R54">
         <v>5.5</v>
@@ -9202,24 +9163,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C55" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D55">
         <v>2014</v>
       </c>
       <c r="E55" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F55" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G55" t="s">
         <v>64</v>
@@ -9237,10 +9198,10 @@
         <v>1</v>
       </c>
       <c r="N55" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Q55" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="R55">
         <v>4</v>
@@ -9327,24 +9288,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C56" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D56">
         <v>2014</v>
       </c>
       <c r="E56" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="F56" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="G56" t="s">
         <v>44</v>
@@ -9362,7 +9323,7 @@
         <v>0</v>
       </c>
       <c r="N56" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R56">
         <v>6.5</v>
@@ -9449,27 +9410,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C57" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D57">
         <v>2014</v>
       </c>
       <c r="E57" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F57" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G57" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="H57" t="s">
         <v>243</v>
@@ -9478,16 +9439,16 @@
         <v>17</v>
       </c>
       <c r="L57" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="M57">
         <v>2</v>
       </c>
       <c r="N57" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="Q57" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="R57">
         <v>6</v>
@@ -9574,30 +9535,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C58" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D58">
         <v>2015</v>
       </c>
       <c r="E58" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="F58" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="G58" t="s">
         <v>44</v>
       </c>
       <c r="H58" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="K58">
         <v>37</v>
@@ -9609,7 +9570,7 @@
         <v>2</v>
       </c>
       <c r="N58" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="Q58" t="s">
         <v>106</v>
@@ -9699,24 +9660,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C59" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D59">
         <v>2015</v>
       </c>
       <c r="E59" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F59" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G59" t="s">
         <v>64</v>
@@ -9734,7 +9695,7 @@
         <v>0</v>
       </c>
       <c r="N59" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="R59">
         <v>4</v>
@@ -9821,42 +9782,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C60" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D60">
         <v>2015</v>
       </c>
       <c r="E60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F60" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G60" t="s">
         <v>44</v>
       </c>
       <c r="H60" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="K60">
         <v>8</v>
       </c>
       <c r="L60" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="M60">
         <v>0</v>
       </c>
       <c r="N60" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="R60">
         <v>3.75</v>
@@ -9943,28 +9904,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C61" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D61">
         <v>2015</v>
       </c>
       <c r="E61" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="F61" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="K61">
         <v>17</v>
@@ -9976,10 +9937,10 @@
         <v>1</v>
       </c>
       <c r="N61" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="Q61" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="R61">
         <v>4</v>
@@ -10045,7 +10006,7 @@
         <v>13.5</v>
       </c>
       <c r="AM61" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="AN61">
         <v>0</v>
@@ -10066,72 +10027,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C62" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D62">
         <v>2015</v>
       </c>
       <c r="E62" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="F62" t="s">
+        <v>472</v>
+      </c>
+      <c r="G62" t="s">
+        <v>474</v>
+      </c>
+      <c r="H62" t="s">
         <v>475</v>
-      </c>
-      <c r="G62" t="s">
-        <v>477</v>
-      </c>
-      <c r="H62" t="s">
-        <v>478</v>
       </c>
       <c r="K62">
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C63" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D63">
         <v>2015</v>
       </c>
       <c r="E63" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F63" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="K63">
         <v>11</v>
       </c>
       <c r="L63" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="M63">
         <v>2</v>
       </c>
       <c r="N63" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="Q63" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="R63">
         <v>6</v>
@@ -10218,24 +10179,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C64" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D64">
         <v>2015</v>
       </c>
       <c r="E64" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F64" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="G64" t="s">
         <v>64</v>
@@ -10253,7 +10214,7 @@
         <v>2</v>
       </c>
       <c r="N64" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="Q64" t="s">
         <v>106</v>
@@ -10343,30 +10304,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C65" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D65">
         <v>2016</v>
       </c>
       <c r="E65" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F65" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G65" t="s">
         <v>44</v>
       </c>
       <c r="H65" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="K65">
         <v>12</v>
@@ -10378,10 +10339,10 @@
         <v>2</v>
       </c>
       <c r="N65" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="Q65" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="R65">
         <v>3.75</v>
@@ -10468,27 +10429,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C66" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D66">
         <v>2016</v>
       </c>
       <c r="E66" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="F66" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="H66" t="s">
         <v>237</v>
@@ -10497,13 +10458,13 @@
         <v>11</v>
       </c>
       <c r="L66" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="M66">
         <v>0</v>
       </c>
       <c r="N66" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="R66">
         <v>4.75</v>
@@ -10590,30 +10551,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D67">
         <v>2016</v>
       </c>
       <c r="E67" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F67" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="G67" t="s">
         <v>44</v>
       </c>
       <c r="H67" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="K67">
         <v>31</v>
@@ -10625,13 +10586,13 @@
         <v>1</v>
       </c>
       <c r="N67" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="P67" s="3" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="Q67" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="R67">
         <v>12</v>
@@ -10718,42 +10679,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C68" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D68">
         <v>2016</v>
       </c>
       <c r="E68" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="F68" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="G68" t="s">
         <v>64</v>
       </c>
       <c r="H68" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="K68">
         <v>25</v>
       </c>
       <c r="L68" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="M68">
         <v>0</v>
       </c>
       <c r="N68" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="R68">
         <v>8</v>
@@ -10840,24 +10801,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D69">
         <v>2016</v>
       </c>
       <c r="E69" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F69" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G69" t="s">
         <v>64</v>
@@ -10869,13 +10830,13 @@
         <v>12</v>
       </c>
       <c r="L69" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="M69">
         <v>0</v>
       </c>
       <c r="N69" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="R69">
         <v>7.5</v>
@@ -10962,24 +10923,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C70" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D70">
         <v>2016</v>
       </c>
       <c r="E70" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="F70" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="G70" t="s">
         <v>64</v>
@@ -10997,10 +10958,10 @@
         <v>2</v>
       </c>
       <c r="N70" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="Q70" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="R70">
         <v>4.5</v>
@@ -11087,24 +11048,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C71" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D71">
         <v>2016</v>
       </c>
       <c r="E71" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F71" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
@@ -11118,7 +11079,7 @@
         <v>0</v>
       </c>
       <c r="N71" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="R71">
         <v>3.5</v>
@@ -11205,42 +11166,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C72" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D72">
         <v>2016</v>
       </c>
       <c r="E72" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="F72" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="G72" t="s">
         <v>64</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="K72">
         <v>12</v>
       </c>
       <c r="L72" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="M72">
         <v>0</v>
       </c>
       <c r="N72" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="R72">
         <v>3</v>
@@ -11327,24 +11288,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C73" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D73">
         <v>2017</v>
       </c>
       <c r="E73" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F73" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>44</v>
@@ -11362,13 +11323,13 @@
         <v>1</v>
       </c>
       <c r="N73" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="P73" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="Q73" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="R73">
         <v>20</v>
@@ -11453,30 +11414,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C74" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D74">
         <v>2017</v>
       </c>
       <c r="E74" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="F74" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="G74" t="s">
         <v>64</v>
       </c>
       <c r="H74" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="K74">
         <v>19</v>
@@ -11488,7 +11449,7 @@
         <v>0</v>
       </c>
       <c r="N74" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="R74">
         <v>14</v>
@@ -11575,30 +11536,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C75" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D75">
         <v>2017</v>
       </c>
       <c r="E75" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F75" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G75" t="s">
         <v>64</v>
       </c>
       <c r="H75" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="K75">
         <v>21</v>
@@ -11610,7 +11571,7 @@
         <v>1</v>
       </c>
       <c r="N75" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="Q75" t="s">
         <v>153</v>
@@ -11700,30 +11661,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C76" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D76">
         <v>2017</v>
       </c>
       <c r="E76" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="F76" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="G76" t="s">
         <v>64</v>
       </c>
       <c r="H76" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="K76">
         <v>48</v>
@@ -11735,10 +11696,10 @@
         <v>1</v>
       </c>
       <c r="N76" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="Q76" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="R76">
         <v>4</v>
@@ -11825,30 +11786,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C77" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D77">
         <v>2017</v>
       </c>
       <c r="E77" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F77" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="G77" t="s">
         <v>44</v>
       </c>
       <c r="H77" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="K77">
         <v>7</v>
@@ -11860,7 +11821,7 @@
         <v>0</v>
       </c>
       <c r="N77" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="R77">
         <v>3</v>
@@ -11947,24 +11908,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C78" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D78">
         <v>2017</v>
       </c>
       <c r="E78" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F78" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="G78" t="s">
         <v>64</v>
@@ -11982,10 +11943,10 @@
         <v>2</v>
       </c>
       <c r="N78" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="Q78" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="R78">
         <v>11</v>

</xml_diff>

<commit_message>
Cleaned data in R and made basic visualizations
</commit_message>
<xml_diff>
--- a/AlitoDataset.xlsx
+++ b/AlitoDataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineparnell/alito-research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jtsanz\alito-research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97108553-A416-1F4D-A6C9-DE1F2F54A514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535A7CAD-AED0-46BC-9A36-85076EEF3787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C9421483-4F05-4E4D-8616-FB0DB15F9718}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -353,7 +353,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="521">
   <si>
     <t>Case Name</t>
   </si>
@@ -579,9 +579,6 @@
     <t>9,0</t>
   </si>
   <si>
-    <t>Alito;Roberts,Stevens,Scalia,Kennedy,Souter,Thomas,Ginsberg,Breyer</t>
-  </si>
-  <si>
     <t>Thomas;</t>
   </si>
   <si>
@@ -1049,9 +1046,6 @@
     <t>Kagan;Sotomayor,Ginsburg,Scalia</t>
   </si>
   <si>
-    <t>Alito;Roberts,Stevens,Scalia,Kennedy,Souter,Thomas,Ginsberg,Breyer,Thomas</t>
-  </si>
-  <si>
     <t>Johnson v. Wlliams</t>
   </si>
   <si>
@@ -1932,6 +1926,9 @@
   </si>
   <si>
     <t>Ginsburg;Sotomayor,Breyer</t>
+  </si>
+  <si>
+    <t>Alito;Roberts,Stevens,Scalia,Kennedy,Souter,Thomas,Ginsburg,Breyer,Thomas</t>
   </si>
 </sst>
 </file>
@@ -2428,11 +2425,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060A011E-60FD-5047-91C8-6B9B09AABF05}">
   <dimension ref="A1:AS78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="82" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="82.1640625" customWidth="1"/>
@@ -2481,7 +2478,7 @@
     <col min="45" max="45" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -2618,7 +2615,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2626,7 +2623,7 @@
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D2">
         <v>2006</v>
@@ -2656,13 +2653,13 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
+        <v>173</v>
+      </c>
+      <c r="P2" t="s">
         <v>174</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>175</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>176</v>
       </c>
       <c r="R2">
         <v>6</v>
@@ -2749,7 +2746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:45" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" ht="65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2757,7 +2754,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D3">
         <v>2006</v>
@@ -2877,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:45" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" ht="62" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2885,7 +2882,7 @@
         <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D4">
         <v>2006</v>
@@ -2915,10 +2912,10 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q4" t="s">
         <v>177</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>178</v>
       </c>
       <c r="R4">
         <v>9</v>
@@ -3005,7 +3002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:45" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" ht="37" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3013,7 +3010,7 @@
         <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D5">
         <v>2007</v>
@@ -3043,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="R5">
         <v>1.25</v>
@@ -3130,30 +3127,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:45" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" t="s">
         <v>179</v>
-      </c>
-      <c r="C6" t="s">
-        <v>180</v>
       </c>
       <c r="D6">
         <v>2007</v>
       </c>
       <c r="E6" t="s">
+        <v>184</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="G6" t="s">
         <v>64</v>
       </c>
       <c r="H6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J6">
         <v>2</v>
@@ -3168,10 +3165,10 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Q6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R6">
         <v>5</v>
@@ -3258,7 +3255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:45" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:45" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3266,7 +3263,7 @@
         <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D7">
         <v>2007</v>
@@ -3294,10 +3291,10 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
+        <v>198</v>
+      </c>
+      <c r="P7" t="s">
         <v>71</v>
-      </c>
-      <c r="P7" t="s">
-        <v>72</v>
       </c>
       <c r="R7">
         <v>5.5</v>
@@ -3384,30 +3381,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:45" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" t="s">
         <v>189</v>
-      </c>
-      <c r="C8" t="s">
-        <v>190</v>
       </c>
       <c r="D8">
         <v>2007</v>
       </c>
       <c r="E8" t="s">
+        <v>191</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="G8" t="s">
         <v>64</v>
       </c>
       <c r="H8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J8">
         <v>2</v>
@@ -3422,7 +3419,7 @@
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>227</v>
+        <v>520</v>
       </c>
       <c r="R8">
         <v>0.25</v>
@@ -3509,30 +3506,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
         <v>73</v>
-      </c>
-      <c r="C9" t="s">
-        <v>74</v>
       </c>
       <c r="D9">
         <v>2007</v>
       </c>
       <c r="E9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" t="s">
         <v>75</v>
-      </c>
-      <c r="F9" t="s">
-        <v>76</v>
       </c>
       <c r="G9" t="s">
         <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J9">
         <v>2</v>
@@ -3541,16 +3538,16 @@
         <v>13</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M9">
         <v>2</v>
       </c>
       <c r="N9" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q9" t="s">
         <v>79</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>80</v>
       </c>
       <c r="R9">
         <v>3</v>
@@ -3634,28 +3631,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" t="s">
         <v>195</v>
-      </c>
-      <c r="C10" t="s">
-        <v>196</v>
       </c>
       <c r="D10">
         <v>2007</v>
       </c>
       <c r="E10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" t="s">
         <v>64</v>
       </c>
       <c r="H10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -3664,16 +3661,16 @@
         <v>14</v>
       </c>
       <c r="L10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M10">
         <v>2</v>
       </c>
       <c r="N10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R10">
         <v>3</v>
@@ -3739,7 +3736,7 @@
         <v>14.5</v>
       </c>
       <c r="AM10" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AN10">
         <v>0</v>
@@ -3760,30 +3757,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" t="s">
         <v>81</v>
-      </c>
-      <c r="C11" t="s">
-        <v>82</v>
       </c>
       <c r="D11">
         <v>2008</v>
       </c>
       <c r="E11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" t="s">
         <v>83</v>
-      </c>
-      <c r="F11" t="s">
-        <v>84</v>
       </c>
       <c r="G11" t="s">
         <v>44</v>
       </c>
       <c r="H11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J11">
         <v>2</v>
@@ -3798,7 +3795,7 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R11">
         <v>4</v>
@@ -3864,7 +3861,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AN11">
         <v>0</v>
@@ -3885,30 +3882,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" t="s">
         <v>201</v>
-      </c>
-      <c r="C12" t="s">
-        <v>202</v>
       </c>
       <c r="D12">
         <v>2008</v>
       </c>
       <c r="E12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F12" t="s">
         <v>203</v>
-      </c>
-      <c r="F12" t="s">
-        <v>204</v>
       </c>
       <c r="G12" t="s">
         <v>44</v>
       </c>
       <c r="H12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -3923,7 +3920,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R12">
         <v>5.5</v>
@@ -4010,30 +4007,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" t="s">
         <v>86</v>
-      </c>
-      <c r="C13" t="s">
-        <v>87</v>
       </c>
       <c r="D13">
         <v>2008</v>
       </c>
       <c r="E13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" t="s">
         <v>88</v>
-      </c>
-      <c r="F13" t="s">
-        <v>89</v>
       </c>
       <c r="G13" t="s">
         <v>64</v>
       </c>
       <c r="H13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J13">
         <v>2</v>
@@ -4051,7 +4048,7 @@
         <v>59</v>
       </c>
       <c r="Q13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R13">
         <v>7.5</v>
@@ -4117,7 +4114,7 @@
         <v>14</v>
       </c>
       <c r="AM13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AN13">
         <v>0</v>
@@ -4138,30 +4135,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C14" t="s">
         <v>207</v>
-      </c>
-      <c r="C14" t="s">
-        <v>208</v>
       </c>
       <c r="D14">
         <v>2008</v>
       </c>
       <c r="E14" t="s">
+        <v>208</v>
+      </c>
+      <c r="F14" t="s">
         <v>209</v>
-      </c>
-      <c r="F14" t="s">
-        <v>210</v>
       </c>
       <c r="G14" t="s">
         <v>64</v>
       </c>
       <c r="H14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -4173,10 +4170,10 @@
         <v>70</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="R14">
         <v>4</v>
@@ -4242,7 +4239,7 @@
         <v>0</v>
       </c>
       <c r="AM14" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="AN14">
         <v>0</v>
@@ -4263,30 +4260,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" t="s">
         <v>93</v>
-      </c>
-      <c r="C15" t="s">
-        <v>94</v>
       </c>
       <c r="D15">
         <v>2008</v>
       </c>
       <c r="E15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" t="s">
         <v>95</v>
-      </c>
-      <c r="F15" t="s">
-        <v>96</v>
       </c>
       <c r="G15" t="s">
         <v>44</v>
       </c>
       <c r="H15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -4301,10 +4298,10 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
+        <v>97</v>
+      </c>
+      <c r="P15" t="s">
         <v>98</v>
-      </c>
-      <c r="P15" t="s">
-        <v>99</v>
       </c>
       <c r="R15">
         <v>3</v>
@@ -4370,7 +4367,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AN15">
         <v>0</v>
@@ -4391,30 +4388,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C16" t="s">
         <v>213</v>
-      </c>
-      <c r="C16" t="s">
-        <v>214</v>
       </c>
       <c r="D16">
         <v>2009</v>
       </c>
       <c r="E16" t="s">
+        <v>214</v>
+      </c>
+      <c r="F16" t="s">
         <v>215</v>
-      </c>
-      <c r="F16" t="s">
-        <v>216</v>
       </c>
       <c r="G16" t="s">
         <v>64</v>
       </c>
       <c r="H16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J16">
         <v>2</v>
@@ -4423,16 +4420,16 @@
         <v>18</v>
       </c>
       <c r="L16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M16">
         <v>2</v>
       </c>
       <c r="N16" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q16" t="s">
         <v>218</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>219</v>
       </c>
       <c r="R16">
         <v>6</v>
@@ -4519,24 +4516,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" t="s">
         <v>101</v>
-      </c>
-      <c r="C17" t="s">
-        <v>102</v>
       </c>
       <c r="D17">
         <v>2009</v>
       </c>
       <c r="E17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" t="s">
         <v>103</v>
-      </c>
-      <c r="F17" t="s">
-        <v>104</v>
       </c>
       <c r="G17" t="s">
         <v>64</v>
@@ -4554,10 +4551,10 @@
         <v>0</v>
       </c>
       <c r="N17" t="s">
+        <v>104</v>
+      </c>
+      <c r="P17" t="s">
         <v>105</v>
-      </c>
-      <c r="P17" t="s">
-        <v>106</v>
       </c>
       <c r="R17">
         <v>6</v>
@@ -4623,7 +4620,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AN17">
         <v>0</v>
@@ -4644,30 +4641,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D18">
         <v>2009</v>
       </c>
       <c r="E18" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G18" t="s">
         <v>44</v>
       </c>
       <c r="H18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -4682,7 +4679,7 @@
         <v>0</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="R18">
         <v>5</v>
@@ -4766,30 +4763,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:45" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" t="s">
         <v>108</v>
-      </c>
-      <c r="C19" t="s">
-        <v>109</v>
       </c>
       <c r="D19">
         <v>2009</v>
       </c>
       <c r="E19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="G19" t="s">
         <v>64</v>
       </c>
       <c r="H19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -4804,10 +4801,10 @@
         <v>1</v>
       </c>
       <c r="N19" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q19" t="s">
         <v>113</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>114</v>
       </c>
       <c r="R19">
         <v>10</v>
@@ -4892,30 +4889,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C20" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D20">
         <v>2009</v>
       </c>
       <c r="E20" t="s">
+        <v>265</v>
+      </c>
+      <c r="F20" t="s">
+        <v>266</v>
+      </c>
+      <c r="G20" t="s">
         <v>267</v>
       </c>
-      <c r="F20" t="s">
-        <v>268</v>
-      </c>
-      <c r="G20" t="s">
-        <v>269</v>
-      </c>
       <c r="H20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -4924,16 +4921,16 @@
         <v>24</v>
       </c>
       <c r="L20" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="M20">
         <v>2</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="Q20" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="R20">
         <v>6</v>
@@ -5020,30 +5017,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" t="s">
         <v>115</v>
-      </c>
-      <c r="C21" t="s">
-        <v>116</v>
       </c>
       <c r="D21">
         <v>2009</v>
       </c>
       <c r="E21" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" t="s">
         <v>117</v>
-      </c>
-      <c r="F21" t="s">
-        <v>118</v>
       </c>
       <c r="G21" t="s">
         <v>64</v>
       </c>
       <c r="H21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -5058,13 +5055,13 @@
         <v>1</v>
       </c>
       <c r="N21" t="s">
+        <v>119</v>
+      </c>
+      <c r="P21" t="s">
         <v>120</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>121</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>122</v>
       </c>
       <c r="R21">
         <v>5</v>
@@ -5130,7 +5127,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AN21">
         <v>0</v>
@@ -5151,30 +5148,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C22" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D22">
         <v>2009</v>
       </c>
       <c r="E22" t="s">
+        <v>273</v>
+      </c>
+      <c r="F22" t="s">
+        <v>274</v>
+      </c>
+      <c r="G22" t="s">
         <v>275</v>
       </c>
-      <c r="F22" t="s">
-        <v>276</v>
-      </c>
-      <c r="G22" t="s">
-        <v>277</v>
-      </c>
       <c r="H22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -5189,10 +5186,10 @@
         <v>1</v>
       </c>
       <c r="N22" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="Q22" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="R22">
         <v>6</v>
@@ -5258,7 +5255,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AN22">
         <v>0</v>
@@ -5279,30 +5276,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" t="s">
         <v>123</v>
-      </c>
-      <c r="C23" t="s">
-        <v>124</v>
       </c>
       <c r="D23">
         <v>2009</v>
       </c>
       <c r="E23" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23" t="s">
         <v>125</v>
-      </c>
-      <c r="F23" t="s">
-        <v>126</v>
       </c>
       <c r="G23" t="s">
         <v>44</v>
       </c>
       <c r="H23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -5311,7 +5308,7 @@
         <v>24</v>
       </c>
       <c r="L23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M23" s="3">
         <v>2</v>
@@ -5320,7 +5317,7 @@
         <v>59</v>
       </c>
       <c r="Q23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="R23">
         <v>6</v>
@@ -5386,7 +5383,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AN23">
         <v>0</v>
@@ -5407,30 +5404,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C24" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D24">
         <v>2010</v>
       </c>
       <c r="E24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F24" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G24" t="s">
         <v>64</v>
       </c>
       <c r="H24" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J24">
         <v>3</v>
@@ -5439,16 +5436,16 @@
         <v>20</v>
       </c>
       <c r="L24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M24">
         <v>2</v>
       </c>
       <c r="N24" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="Q24" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R24">
         <v>8.5</v>
@@ -5535,30 +5532,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" t="s">
         <v>129</v>
-      </c>
-      <c r="C25" t="s">
-        <v>130</v>
       </c>
       <c r="D25">
         <v>2010</v>
       </c>
       <c r="E25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" t="s">
         <v>131</v>
-      </c>
-      <c r="F25" t="s">
-        <v>132</v>
       </c>
       <c r="G25" t="s">
         <v>64</v>
       </c>
       <c r="H25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J25">
         <v>3</v>
@@ -5567,16 +5564,16 @@
         <v>16</v>
       </c>
       <c r="L25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M25">
         <v>2</v>
       </c>
       <c r="N25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R25">
         <v>3</v>
@@ -5663,30 +5660,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C26" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D26">
         <v>2010</v>
       </c>
       <c r="E26" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F26" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G26" t="s">
         <v>64</v>
       </c>
       <c r="H26" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J26">
         <v>3</v>
@@ -5695,13 +5692,13 @@
         <v>13</v>
       </c>
       <c r="L26" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M26">
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="R26">
         <v>4</v>
@@ -5782,30 +5779,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" t="s">
         <v>136</v>
-      </c>
-      <c r="C27" t="s">
-        <v>137</v>
       </c>
       <c r="D27">
         <v>2010</v>
       </c>
       <c r="E27" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27" t="s">
         <v>138</v>
-      </c>
-      <c r="F27" t="s">
-        <v>139</v>
       </c>
       <c r="G27" t="s">
         <v>64</v>
       </c>
       <c r="H27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J27">
         <v>3</v>
@@ -5814,16 +5811,16 @@
         <v>19</v>
       </c>
       <c r="L27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M27">
         <v>2</v>
       </c>
       <c r="N27" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q27" t="s">
         <v>142</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>143</v>
       </c>
       <c r="R27">
         <v>4</v>
@@ -5910,30 +5907,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C28" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D28">
         <v>2010</v>
       </c>
       <c r="E28" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F28" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G28" t="s">
         <v>64</v>
       </c>
       <c r="H28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J28">
         <v>3</v>
@@ -5942,16 +5939,16 @@
         <v>24</v>
       </c>
       <c r="L28" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="M28">
         <v>2</v>
       </c>
       <c r="N28" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="Q28" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="R28">
         <v>5</v>
@@ -6038,30 +6035,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" t="s">
         <v>144</v>
-      </c>
-      <c r="C29" t="s">
-        <v>145</v>
       </c>
       <c r="D29">
         <v>2010</v>
       </c>
       <c r="E29" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" t="s">
         <v>146</v>
-      </c>
-      <c r="F29" t="s">
-        <v>147</v>
       </c>
       <c r="G29" t="s">
         <v>64</v>
       </c>
       <c r="H29" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J29">
         <v>3</v>
@@ -6076,7 +6073,7 @@
         <v>0</v>
       </c>
       <c r="N29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R29">
         <v>4.5</v>
@@ -6163,28 +6160,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:45" ht="51" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:45" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>148</v>
+      </c>
+      <c r="C30" t="s">
         <v>149</v>
-      </c>
-      <c r="C30" t="s">
-        <v>150</v>
       </c>
       <c r="D30">
         <v>2011</v>
       </c>
       <c r="E30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J30">
         <v>2</v>
@@ -6199,10 +6196,10 @@
         <v>1</v>
       </c>
       <c r="N30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R30">
         <v>8</v>
@@ -6289,30 +6286,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C31" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D31">
         <v>2011</v>
       </c>
       <c r="E31" t="s">
+        <v>298</v>
+      </c>
+      <c r="F31" t="s">
+        <v>299</v>
+      </c>
+      <c r="G31" t="s">
         <v>300</v>
       </c>
-      <c r="F31" t="s">
+      <c r="H31" t="s">
         <v>301</v>
-      </c>
-      <c r="G31" t="s">
-        <v>302</v>
-      </c>
-      <c r="H31" t="s">
-        <v>303</v>
       </c>
       <c r="J31">
         <v>2</v>
@@ -6321,16 +6318,16 @@
         <v>25</v>
       </c>
       <c r="L31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M31">
         <v>2</v>
       </c>
       <c r="N31" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="Q31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R31">
         <v>5</v>
@@ -6417,30 +6414,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" t="s">
         <v>154</v>
-      </c>
-      <c r="C32" t="s">
-        <v>155</v>
       </c>
       <c r="D32">
         <v>2011</v>
       </c>
       <c r="E32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G32" t="s">
         <v>44</v>
       </c>
       <c r="H32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J32">
         <v>0</v>
@@ -6449,16 +6446,16 @@
         <v>16</v>
       </c>
       <c r="L32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M32">
         <v>2</v>
       </c>
       <c r="N32" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q32" t="s">
         <v>161</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>162</v>
       </c>
       <c r="R32">
         <v>4</v>
@@ -6543,30 +6540,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C33" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D33">
         <v>2011</v>
       </c>
       <c r="E33" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F33" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G33" t="s">
         <v>44</v>
       </c>
       <c r="H33" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J33">
         <v>0</v>
@@ -6575,16 +6572,16 @@
         <v>23</v>
       </c>
       <c r="L33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M33">
         <v>2</v>
       </c>
       <c r="N33" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="Q33" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="R33">
         <v>6</v>
@@ -6665,30 +6662,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" t="s">
         <v>163</v>
-      </c>
-      <c r="C34" t="s">
-        <v>164</v>
       </c>
       <c r="D34">
         <v>2011</v>
       </c>
       <c r="E34" t="s">
+        <v>164</v>
+      </c>
+      <c r="F34" t="s">
         <v>165</v>
-      </c>
-      <c r="F34" t="s">
-        <v>166</v>
       </c>
       <c r="G34" t="s">
         <v>64</v>
       </c>
       <c r="H34" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -6703,7 +6700,7 @@
         <v>0</v>
       </c>
       <c r="N34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R34">
         <v>2.5</v>
@@ -6790,30 +6787,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C35" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D35">
         <v>2011</v>
       </c>
       <c r="E35" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F35" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G35" t="s">
         <v>44</v>
       </c>
       <c r="H35" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J35">
         <v>2</v>
@@ -6822,16 +6819,16 @@
         <v>15</v>
       </c>
       <c r="L35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M35">
         <v>2</v>
       </c>
       <c r="N35" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q35" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="R35">
         <v>3</v>
@@ -6918,30 +6915,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>167</v>
+      </c>
+      <c r="C36" t="s">
         <v>168</v>
-      </c>
-      <c r="C36" t="s">
-        <v>169</v>
       </c>
       <c r="D36">
         <v>2011</v>
       </c>
       <c r="E36" t="s">
+        <v>169</v>
+      </c>
+      <c r="F36" t="s">
         <v>170</v>
-      </c>
-      <c r="F36" t="s">
-        <v>171</v>
       </c>
       <c r="G36" t="s">
         <v>64</v>
       </c>
       <c r="H36" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J36">
         <v>1</v>
@@ -6956,10 +6953,10 @@
         <v>1</v>
       </c>
       <c r="N36" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q36" t="s">
         <v>172</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>173</v>
       </c>
       <c r="R36">
         <v>11</v>
@@ -7046,30 +7043,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>219</v>
+      </c>
+      <c r="C37" t="s">
         <v>220</v>
-      </c>
-      <c r="C37" t="s">
-        <v>221</v>
       </c>
       <c r="D37">
         <v>2012</v>
       </c>
       <c r="E37" t="s">
+        <v>221</v>
+      </c>
+      <c r="F37" t="s">
         <v>222</v>
-      </c>
-      <c r="F37" t="s">
-        <v>223</v>
       </c>
       <c r="G37" t="s">
         <v>44</v>
       </c>
       <c r="H37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J37">
         <v>1</v>
@@ -7084,10 +7081,10 @@
         <v>1</v>
       </c>
       <c r="N37" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q37" t="s">
         <v>225</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>226</v>
       </c>
       <c r="R37">
         <v>2</v>
@@ -7174,30 +7171,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C38" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D38">
         <v>2012</v>
       </c>
       <c r="E38" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F38" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G38" t="s">
         <v>44</v>
       </c>
       <c r="H38" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J38">
         <v>2</v>
@@ -7215,7 +7212,7 @@
         <v>59</v>
       </c>
       <c r="Q38" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="R38">
         <v>8</v>
@@ -7302,30 +7299,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C39" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D39">
         <v>2012</v>
       </c>
       <c r="E39" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F39" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G39" t="s">
         <v>64</v>
       </c>
       <c r="H39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -7340,10 +7337,10 @@
         <v>0</v>
       </c>
       <c r="N39" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="P39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R39">
         <v>6.5</v>
@@ -7409,7 +7406,7 @@
         <v>27</v>
       </c>
       <c r="AM39" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="AN39">
         <v>0</v>
@@ -7430,30 +7427,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C40" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D40">
         <v>2012</v>
       </c>
       <c r="E40" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F40" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G40" t="s">
         <v>64</v>
       </c>
       <c r="H40" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -7468,10 +7465,10 @@
         <v>1</v>
       </c>
       <c r="N40" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="Q40" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="R40">
         <v>5</v>
@@ -7558,30 +7555,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C41" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D41">
         <v>2012</v>
       </c>
       <c r="E41" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F41" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G41" t="s">
         <v>44</v>
       </c>
       <c r="H41" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -7596,13 +7593,13 @@
         <v>1</v>
       </c>
       <c r="N41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q41" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="R41">
         <v>3</v>
@@ -7668,7 +7665,7 @@
         <v>4</v>
       </c>
       <c r="AM41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AN41">
         <v>0</v>
@@ -7689,30 +7686,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C42" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D42">
         <v>2012</v>
       </c>
       <c r="E42" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F42" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G42" t="s">
         <v>44</v>
       </c>
       <c r="H42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J42">
         <v>2</v>
@@ -7727,13 +7724,13 @@
         <v>1</v>
       </c>
       <c r="N42" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="P42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q42" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="R42">
         <v>4.5</v>
@@ -7820,30 +7817,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C43" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D43">
         <v>2013</v>
       </c>
       <c r="E43" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F43" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G43" t="s">
         <v>64</v>
       </c>
       <c r="H43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -7858,7 +7855,7 @@
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R43">
         <v>3</v>
@@ -7945,30 +7942,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C44" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D44">
         <v>2013</v>
       </c>
       <c r="E44" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F44" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G44" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H44" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="J44">
         <v>0</v>
@@ -7983,7 +7980,7 @@
         <v>0</v>
       </c>
       <c r="N44" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="R44">
         <v>4</v>
@@ -8070,30 +8067,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C45" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D45">
         <v>2013</v>
       </c>
       <c r="E45" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F45" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G45" t="s">
         <v>64</v>
       </c>
       <c r="H45" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J45">
         <v>0</v>
@@ -8108,10 +8105,10 @@
         <v>1</v>
       </c>
       <c r="N45" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="Q45" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="R45">
         <v>15.5</v>
@@ -8198,30 +8195,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C46" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D46">
         <v>2013</v>
       </c>
       <c r="E46" t="s">
+        <v>428</v>
+      </c>
+      <c r="F46" t="s">
+        <v>429</v>
+      </c>
+      <c r="G46" t="s">
         <v>430</v>
       </c>
-      <c r="F46" t="s">
-        <v>431</v>
-      </c>
-      <c r="G46" t="s">
-        <v>432</v>
-      </c>
       <c r="H46" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -8236,10 +8233,10 @@
         <v>1</v>
       </c>
       <c r="N46" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="Q46" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="R46">
         <v>8</v>
@@ -8326,30 +8323,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C47" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D47">
         <v>2013</v>
       </c>
       <c r="E47" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F47" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G47" t="s">
         <v>64</v>
       </c>
       <c r="H47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -8364,7 +8361,7 @@
         <v>0</v>
       </c>
       <c r="N47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R47">
         <v>4</v>
@@ -8451,30 +8448,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C48" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D48">
         <v>2013</v>
       </c>
       <c r="E48" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F48" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="G48" t="s">
         <v>64</v>
       </c>
       <c r="H48" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="J48">
         <v>1</v>
@@ -8489,7 +8486,7 @@
         <v>0</v>
       </c>
       <c r="N48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R48">
         <v>5.5</v>
@@ -8576,30 +8573,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C49" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D49">
         <v>2013</v>
       </c>
       <c r="E49" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F49" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G49" t="s">
         <v>64</v>
       </c>
       <c r="H49" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J49">
         <v>1</v>
@@ -8614,7 +8611,7 @@
         <v>0</v>
       </c>
       <c r="N49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R49">
         <v>4</v>
@@ -8701,30 +8698,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C50" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D50">
         <v>2014</v>
       </c>
       <c r="E50" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F50" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G50" t="s">
         <v>64</v>
       </c>
       <c r="H50" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J50">
         <v>2</v>
@@ -8733,16 +8730,16 @@
         <v>10</v>
       </c>
       <c r="L50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M50">
         <v>2</v>
       </c>
       <c r="N50" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="Q50" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="R50">
         <v>3</v>
@@ -8829,30 +8826,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D51">
         <v>2014</v>
       </c>
       <c r="E51" t="s">
+        <v>307</v>
+      </c>
+      <c r="F51" t="s">
+        <v>308</v>
+      </c>
+      <c r="G51" t="s">
         <v>309</v>
       </c>
-      <c r="F51" t="s">
+      <c r="H51" t="s">
         <v>310</v>
-      </c>
-      <c r="G51" t="s">
-        <v>311</v>
-      </c>
-      <c r="H51" t="s">
-        <v>312</v>
       </c>
       <c r="J51">
         <v>2</v>
@@ -8867,7 +8864,7 @@
         <v>0</v>
       </c>
       <c r="N51" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="R51">
         <v>5</v>
@@ -8954,30 +8951,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C52" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D52">
         <v>2014</v>
       </c>
       <c r="E52" t="s">
+        <v>445</v>
+      </c>
+      <c r="F52" t="s">
+        <v>446</v>
+      </c>
+      <c r="G52" t="s">
         <v>447</v>
       </c>
-      <c r="F52" t="s">
+      <c r="H52" t="s">
         <v>448</v>
-      </c>
-      <c r="G52" t="s">
-        <v>449</v>
-      </c>
-      <c r="H52" t="s">
-        <v>450</v>
       </c>
       <c r="J52">
         <v>0</v>
@@ -8992,10 +8989,10 @@
         <v>1</v>
       </c>
       <c r="N52" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="Q52" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="R52">
         <v>8</v>
@@ -9082,30 +9079,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C53" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D53">
         <v>2014</v>
       </c>
       <c r="E53" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F53" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G53" t="s">
         <v>44</v>
       </c>
       <c r="H53" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J53">
         <v>0</v>
@@ -9123,7 +9120,7 @@
         <v>59</v>
       </c>
       <c r="Q53" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="R53">
         <v>8.5</v>
@@ -9189,7 +9186,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AN53">
         <v>0</v>
@@ -9210,30 +9207,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C54" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D54">
         <v>2014</v>
       </c>
       <c r="E54" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F54" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="G54" t="s">
         <v>64</v>
       </c>
       <c r="H54" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="J54">
         <v>2</v>
@@ -9248,7 +9245,7 @@
         <v>0</v>
       </c>
       <c r="N54" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="R54">
         <v>5.5</v>
@@ -9335,30 +9332,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C55" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D55">
         <v>2014</v>
       </c>
       <c r="E55" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F55" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G55" t="s">
         <v>64</v>
       </c>
       <c r="H55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J55">
         <v>2</v>
@@ -9373,10 +9370,10 @@
         <v>1</v>
       </c>
       <c r="N55" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="Q55" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="R55">
         <v>4</v>
@@ -9463,30 +9460,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C56" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D56">
         <v>2014</v>
       </c>
       <c r="E56" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="F56" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G56" t="s">
         <v>44</v>
       </c>
       <c r="H56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J56">
         <v>0</v>
@@ -9501,7 +9498,7 @@
         <v>0</v>
       </c>
       <c r="N56" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="R56">
         <v>6.5</v>
@@ -9588,30 +9585,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C57" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D57">
         <v>2014</v>
       </c>
       <c r="E57" t="s">
+        <v>326</v>
+      </c>
+      <c r="F57" t="s">
+        <v>327</v>
+      </c>
+      <c r="G57" t="s">
         <v>328</v>
       </c>
-      <c r="F57" t="s">
-        <v>329</v>
-      </c>
-      <c r="G57" t="s">
-        <v>330</v>
-      </c>
       <c r="H57" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J57">
         <v>2</v>
@@ -9620,16 +9617,16 @@
         <v>17</v>
       </c>
       <c r="L57" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M57">
         <v>2</v>
       </c>
       <c r="N57" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="Q57" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="R57">
         <v>6</v>
@@ -9716,30 +9713,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C58" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D58">
         <v>2015</v>
       </c>
       <c r="E58" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F58" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="G58" t="s">
         <v>44</v>
       </c>
       <c r="H58" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J58">
         <v>0</v>
@@ -9748,16 +9745,16 @@
         <v>37</v>
       </c>
       <c r="L58" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="M58">
         <v>2</v>
       </c>
       <c r="N58" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="Q58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R58">
         <v>11</v>
@@ -9844,30 +9841,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C59" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D59">
         <v>2015</v>
       </c>
       <c r="E59" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F59" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G59" t="s">
         <v>64</v>
       </c>
       <c r="H59" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J59">
         <v>2</v>
@@ -9882,7 +9879,7 @@
         <v>0</v>
       </c>
       <c r="N59" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="R59">
         <v>4</v>
@@ -9969,30 +9966,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C60" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D60">
         <v>2015</v>
       </c>
       <c r="E60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F60" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G60" t="s">
         <v>44</v>
       </c>
       <c r="H60" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J60">
         <v>0</v>
@@ -10001,13 +9998,13 @@
         <v>8</v>
       </c>
       <c r="L60" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M60">
         <v>0</v>
       </c>
       <c r="N60" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="R60">
         <v>3.75</v>
@@ -10094,28 +10091,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C61" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D61">
         <v>2015</v>
       </c>
       <c r="E61" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F61" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="J61">
         <v>2</v>
@@ -10124,16 +10121,16 @@
         <v>17</v>
       </c>
       <c r="L61" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M61" s="3">
         <v>1</v>
       </c>
       <c r="N61" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="Q61" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="R61">
         <v>4</v>
@@ -10199,7 +10196,7 @@
         <v>13.5</v>
       </c>
       <c r="AM61" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="AN61">
         <v>0</v>
@@ -10220,30 +10217,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C62" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D62">
         <v>2015</v>
       </c>
       <c r="E62" t="s">
+        <v>471</v>
+      </c>
+      <c r="F62" t="s">
+        <v>470</v>
+      </c>
+      <c r="G62" t="s">
+        <v>472</v>
+      </c>
+      <c r="H62" t="s">
         <v>473</v>
-      </c>
-      <c r="F62" t="s">
-        <v>472</v>
-      </c>
-      <c r="G62" t="s">
-        <v>474</v>
-      </c>
-      <c r="H62" t="s">
-        <v>475</v>
       </c>
       <c r="J62">
         <v>2</v>
@@ -10252,28 +10249,28 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C63" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D63">
         <v>2015</v>
       </c>
       <c r="E63" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F63" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J63">
         <v>1</v>
@@ -10282,16 +10279,16 @@
         <v>11</v>
       </c>
       <c r="L63" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M63">
         <v>2</v>
       </c>
       <c r="N63" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="Q63" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="R63">
         <v>6</v>
@@ -10378,30 +10375,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C64" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D64">
         <v>2015</v>
       </c>
       <c r="E64" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F64" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G64" t="s">
         <v>64</v>
       </c>
       <c r="H64" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J64">
         <v>0</v>
@@ -10410,16 +10407,16 @@
         <v>9</v>
       </c>
       <c r="L64" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="M64">
         <v>2</v>
       </c>
       <c r="N64" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="Q64" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R64">
         <v>2.5</v>
@@ -10506,30 +10503,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C65" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D65">
         <v>2016</v>
       </c>
       <c r="E65" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F65" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G65" t="s">
         <v>44</v>
       </c>
       <c r="H65" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="J65">
         <v>2</v>
@@ -10538,16 +10535,16 @@
         <v>12</v>
       </c>
       <c r="L65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M65">
         <v>2</v>
       </c>
       <c r="N65" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="Q65" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="R65">
         <v>3.75</v>
@@ -10613,7 +10610,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AN65">
         <v>0</v>
@@ -10634,30 +10631,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C66" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D66">
         <v>2016</v>
       </c>
       <c r="E66" t="s">
+        <v>483</v>
+      </c>
+      <c r="F66" t="s">
+        <v>484</v>
+      </c>
+      <c r="G66" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="F66" t="s">
-        <v>486</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>487</v>
-      </c>
       <c r="H66" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J66">
         <v>0</v>
@@ -10666,13 +10663,13 @@
         <v>11</v>
       </c>
       <c r="L66" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M66">
         <v>0</v>
       </c>
       <c r="N66" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="R66">
         <v>4.75</v>
@@ -10738,7 +10735,7 @@
         <v>0</v>
       </c>
       <c r="AM66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AN66">
         <v>0</v>
@@ -10759,30 +10756,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D67">
         <v>2016</v>
       </c>
       <c r="E67" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F67" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G67" t="s">
         <v>44</v>
       </c>
       <c r="H67" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J67">
         <v>2</v>
@@ -10797,13 +10794,13 @@
         <v>1</v>
       </c>
       <c r="N67" t="s">
+        <v>360</v>
+      </c>
+      <c r="P67" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="Q67" t="s">
         <v>362</v>
-      </c>
-      <c r="P67" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>364</v>
       </c>
       <c r="R67">
         <v>12</v>
@@ -10890,30 +10887,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C68" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D68">
         <v>2016</v>
       </c>
       <c r="E68" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="F68" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="G68" t="s">
         <v>64</v>
       </c>
       <c r="H68" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="J68">
         <v>1</v>
@@ -10922,13 +10919,13 @@
         <v>25</v>
       </c>
       <c r="L68" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M68">
         <v>0</v>
       </c>
       <c r="N68" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="R68">
         <v>8</v>
@@ -10994,7 +10991,7 @@
         <v>33</v>
       </c>
       <c r="AM68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AN68">
         <v>0</v>
@@ -11015,30 +11012,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D69">
         <v>2016</v>
       </c>
       <c r="E69" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F69" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G69" t="s">
         <v>64</v>
       </c>
       <c r="H69" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J69">
         <v>2</v>
@@ -11047,13 +11044,13 @@
         <v>12</v>
       </c>
       <c r="L69" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M69">
         <v>0</v>
       </c>
       <c r="N69" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="R69">
         <v>7.5</v>
@@ -11140,30 +11137,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C70" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D70">
         <v>2016</v>
       </c>
       <c r="E70" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F70" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G70" t="s">
         <v>64</v>
       </c>
       <c r="H70" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J70">
         <v>2</v>
@@ -11172,16 +11169,16 @@
         <v>16</v>
       </c>
       <c r="L70" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="M70">
         <v>2</v>
       </c>
       <c r="N70" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="Q70" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="R70">
         <v>4.5</v>
@@ -11268,24 +11265,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C71" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D71">
         <v>2016</v>
       </c>
       <c r="E71" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F71" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
@@ -11300,7 +11297,7 @@
         <v>0</v>
       </c>
       <c r="N71" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="R71">
         <v>3.5</v>
@@ -11366,7 +11363,7 @@
         <v>0</v>
       </c>
       <c r="AM71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AN71">
         <v>0</v>
@@ -11387,30 +11384,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C72" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D72">
         <v>2016</v>
       </c>
       <c r="E72" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="F72" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="G72" t="s">
         <v>64</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="J72">
         <v>0</v>
@@ -11419,13 +11416,13 @@
         <v>12</v>
       </c>
       <c r="L72" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M72">
         <v>0</v>
       </c>
       <c r="N72" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="R72">
         <v>3</v>
@@ -11491,7 +11488,7 @@
         <v>33.5</v>
       </c>
       <c r="AM72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AN72">
         <v>0</v>
@@ -11512,30 +11509,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C73" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D73">
         <v>2017</v>
       </c>
       <c r="E73" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F73" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>44</v>
       </c>
       <c r="H73" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J73">
         <v>0</v>
@@ -11550,13 +11547,13 @@
         <v>1</v>
       </c>
       <c r="N73" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="P73" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="Q73" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="R73">
         <v>20</v>
@@ -11641,30 +11638,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C74" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D74">
         <v>2017</v>
       </c>
       <c r="E74" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F74" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="G74" t="s">
         <v>64</v>
       </c>
       <c r="H74" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="J74">
         <v>2</v>
@@ -11679,7 +11676,7 @@
         <v>0</v>
       </c>
       <c r="N74" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="R74">
         <v>14</v>
@@ -11766,30 +11763,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C75" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D75">
         <v>2017</v>
       </c>
       <c r="E75" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F75" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G75" t="s">
         <v>64</v>
       </c>
       <c r="H75" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="J75">
         <v>2</v>
@@ -11804,10 +11801,10 @@
         <v>1</v>
       </c>
       <c r="N75" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="Q75" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R75">
         <v>8</v>
@@ -11894,30 +11891,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C76" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D76">
         <v>2017</v>
       </c>
       <c r="E76" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F76" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G76" t="s">
         <v>64</v>
       </c>
       <c r="H76" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J76">
         <v>2</v>
@@ -11932,10 +11929,10 @@
         <v>1</v>
       </c>
       <c r="N76" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="Q76" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="R76">
         <v>4</v>
@@ -12001,7 +11998,7 @@
         <v>0</v>
       </c>
       <c r="AM76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AN76">
         <v>0</v>
@@ -12022,30 +12019,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C77" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D77">
         <v>2017</v>
       </c>
       <c r="E77" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F77" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G77" t="s">
         <v>44</v>
       </c>
       <c r="H77" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J77">
         <v>0</v>
@@ -12060,7 +12057,7 @@
         <v>0</v>
       </c>
       <c r="N77" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="R77">
         <v>3</v>
@@ -12147,30 +12144,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C78" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D78">
         <v>2017</v>
       </c>
       <c r="E78" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F78" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="G78" t="s">
         <v>64</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J78">
         <v>2</v>
@@ -12179,16 +12176,16 @@
         <v>30</v>
       </c>
       <c r="L78" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M78">
         <v>2</v>
       </c>
       <c r="N78" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="Q78" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="R78">
         <v>11</v>

</xml_diff>